<commit_message>
Aug 26 data entry and prelim figures
</commit_message>
<xml_diff>
--- a/Oyster/cultchmass/cultchmass_packet.xlsx
+++ b/Oyster/cultchmass/cultchmass_packet.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="datasheet" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="44">
   <si>
     <t>REEF MASS FIELD DATASHEET</t>
   </si>
@@ -644,7 +644,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
@@ -1012,10 +1012,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K1"/>
+  <dimension ref="A1:K17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O20" sqref="O20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1056,6 +1056,566 @@
       </c>
       <c r="K1" t="s">
         <v>37</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>2019</v>
+      </c>
+      <c r="B2">
+        <v>8</v>
+      </c>
+      <c r="C2">
+        <v>26</v>
+      </c>
+      <c r="D2" t="s">
+        <v>39</v>
+      </c>
+      <c r="E2" t="s">
+        <v>42</v>
+      </c>
+      <c r="F2">
+        <v>19</v>
+      </c>
+      <c r="G2">
+        <v>1</v>
+      </c>
+      <c r="H2">
+        <v>0.86</v>
+      </c>
+      <c r="I2">
+        <v>16.920000000000002</v>
+      </c>
+      <c r="J2">
+        <v>0.86</v>
+      </c>
+      <c r="K2">
+        <v>1.06</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2019</v>
+      </c>
+      <c r="B3">
+        <v>8</v>
+      </c>
+      <c r="C3">
+        <v>26</v>
+      </c>
+      <c r="D3" t="s">
+        <v>39</v>
+      </c>
+      <c r="E3" t="s">
+        <v>42</v>
+      </c>
+      <c r="F3">
+        <v>19</v>
+      </c>
+      <c r="G3">
+        <v>2</v>
+      </c>
+      <c r="H3">
+        <v>0.86</v>
+      </c>
+      <c r="I3">
+        <v>13.7</v>
+      </c>
+      <c r="J3">
+        <v>0.86</v>
+      </c>
+      <c r="K3">
+        <v>1.08</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>2019</v>
+      </c>
+      <c r="B4">
+        <v>8</v>
+      </c>
+      <c r="C4">
+        <v>26</v>
+      </c>
+      <c r="D4" t="s">
+        <v>39</v>
+      </c>
+      <c r="E4" t="s">
+        <v>42</v>
+      </c>
+      <c r="F4">
+        <v>19</v>
+      </c>
+      <c r="G4">
+        <v>3</v>
+      </c>
+      <c r="H4">
+        <v>0.86</v>
+      </c>
+      <c r="I4">
+        <v>10.94</v>
+      </c>
+      <c r="J4">
+        <v>0.86</v>
+      </c>
+      <c r="K4">
+        <v>1.06</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>2019</v>
+      </c>
+      <c r="B5">
+        <v>8</v>
+      </c>
+      <c r="C5">
+        <v>26</v>
+      </c>
+      <c r="D5" t="s">
+        <v>39</v>
+      </c>
+      <c r="E5" t="s">
+        <v>42</v>
+      </c>
+      <c r="F5">
+        <v>19</v>
+      </c>
+      <c r="G5">
+        <v>4</v>
+      </c>
+      <c r="H5">
+        <v>0.86</v>
+      </c>
+      <c r="I5">
+        <v>15.02</v>
+      </c>
+      <c r="J5">
+        <v>0.86</v>
+      </c>
+      <c r="K5">
+        <v>1.86</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>2019</v>
+      </c>
+      <c r="B6">
+        <v>8</v>
+      </c>
+      <c r="C6">
+        <v>26</v>
+      </c>
+      <c r="D6" t="s">
+        <v>39</v>
+      </c>
+      <c r="E6" t="s">
+        <v>42</v>
+      </c>
+      <c r="F6">
+        <v>2</v>
+      </c>
+      <c r="G6">
+        <v>2</v>
+      </c>
+      <c r="H6">
+        <v>0.86</v>
+      </c>
+      <c r="I6">
+        <v>20.04</v>
+      </c>
+      <c r="J6">
+        <v>1.84</v>
+      </c>
+      <c r="K6">
+        <v>1.22</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>2019</v>
+      </c>
+      <c r="B7">
+        <v>8</v>
+      </c>
+      <c r="C7">
+        <v>26</v>
+      </c>
+      <c r="D7" t="s">
+        <v>39</v>
+      </c>
+      <c r="E7" t="s">
+        <v>42</v>
+      </c>
+      <c r="F7">
+        <v>2</v>
+      </c>
+      <c r="G7">
+        <v>4</v>
+      </c>
+      <c r="H7">
+        <v>0.86</v>
+      </c>
+      <c r="I7">
+        <v>17.739999999999998</v>
+      </c>
+      <c r="J7">
+        <v>2.86</v>
+      </c>
+      <c r="K7">
+        <v>1.6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>2019</v>
+      </c>
+      <c r="B8">
+        <v>8</v>
+      </c>
+      <c r="C8">
+        <v>26</v>
+      </c>
+      <c r="D8" t="s">
+        <v>39</v>
+      </c>
+      <c r="E8" t="s">
+        <v>42</v>
+      </c>
+      <c r="F8">
+        <v>2</v>
+      </c>
+      <c r="G8">
+        <v>3</v>
+      </c>
+      <c r="H8">
+        <v>0.86</v>
+      </c>
+      <c r="I8">
+        <v>16.46</v>
+      </c>
+      <c r="J8">
+        <v>2.2599999999999998</v>
+      </c>
+      <c r="K8">
+        <v>0.96</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>2019</v>
+      </c>
+      <c r="B9">
+        <v>8</v>
+      </c>
+      <c r="C9">
+        <v>26</v>
+      </c>
+      <c r="D9" t="s">
+        <v>39</v>
+      </c>
+      <c r="E9" t="s">
+        <v>42</v>
+      </c>
+      <c r="F9">
+        <v>2</v>
+      </c>
+      <c r="G9">
+        <v>1</v>
+      </c>
+      <c r="H9">
+        <v>0.86</v>
+      </c>
+      <c r="I9">
+        <v>12.02</v>
+      </c>
+      <c r="J9">
+        <v>1.36</v>
+      </c>
+      <c r="K9">
+        <v>0.86</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>2019</v>
+      </c>
+      <c r="B10">
+        <v>8</v>
+      </c>
+      <c r="C10">
+        <v>26</v>
+      </c>
+      <c r="D10" t="s">
+        <v>39</v>
+      </c>
+      <c r="E10" t="s">
+        <v>42</v>
+      </c>
+      <c r="F10">
+        <v>1</v>
+      </c>
+      <c r="G10">
+        <v>4</v>
+      </c>
+      <c r="H10">
+        <v>0.86</v>
+      </c>
+      <c r="I10">
+        <v>21.28</v>
+      </c>
+      <c r="J10">
+        <v>4.53</v>
+      </c>
+      <c r="K10">
+        <v>2.15</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>2019</v>
+      </c>
+      <c r="B11">
+        <v>8</v>
+      </c>
+      <c r="C11">
+        <v>26</v>
+      </c>
+      <c r="D11" t="s">
+        <v>39</v>
+      </c>
+      <c r="E11" t="s">
+        <v>42</v>
+      </c>
+      <c r="F11">
+        <v>1</v>
+      </c>
+      <c r="G11">
+        <v>2</v>
+      </c>
+      <c r="H11">
+        <v>0.86</v>
+      </c>
+      <c r="I11">
+        <v>17.690000000000001</v>
+      </c>
+      <c r="J11">
+        <v>4.99</v>
+      </c>
+      <c r="K11">
+        <v>2.4900000000000002</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>2019</v>
+      </c>
+      <c r="B12">
+        <v>8</v>
+      </c>
+      <c r="C12">
+        <v>26</v>
+      </c>
+      <c r="D12" t="s">
+        <v>39</v>
+      </c>
+      <c r="E12" t="s">
+        <v>42</v>
+      </c>
+      <c r="F12">
+        <v>1</v>
+      </c>
+      <c r="G12">
+        <v>1</v>
+      </c>
+      <c r="H12">
+        <v>0.86</v>
+      </c>
+      <c r="I12">
+        <v>23.13</v>
+      </c>
+      <c r="J12">
+        <v>2.38</v>
+      </c>
+      <c r="K12">
+        <v>7.03</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>2019</v>
+      </c>
+      <c r="B13">
+        <v>8</v>
+      </c>
+      <c r="C13">
+        <v>26</v>
+      </c>
+      <c r="D13" t="s">
+        <v>39</v>
+      </c>
+      <c r="E13" t="s">
+        <v>42</v>
+      </c>
+      <c r="F13">
+        <v>1</v>
+      </c>
+      <c r="G13">
+        <v>3</v>
+      </c>
+      <c r="H13">
+        <v>0.86</v>
+      </c>
+      <c r="I13">
+        <v>-999</v>
+      </c>
+      <c r="J13">
+        <v>0.86</v>
+      </c>
+      <c r="K13">
+        <v>1.25</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>2019</v>
+      </c>
+      <c r="B14">
+        <v>8</v>
+      </c>
+      <c r="C14">
+        <v>26</v>
+      </c>
+      <c r="D14" t="s">
+        <v>39</v>
+      </c>
+      <c r="E14" t="s">
+        <v>42</v>
+      </c>
+      <c r="F14">
+        <v>12</v>
+      </c>
+      <c r="G14">
+        <v>1</v>
+      </c>
+      <c r="H14">
+        <v>0.86</v>
+      </c>
+      <c r="I14">
+        <v>-999</v>
+      </c>
+      <c r="J14">
+        <v>2.4900000000000002</v>
+      </c>
+      <c r="K14">
+        <v>2.15</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>2019</v>
+      </c>
+      <c r="B15">
+        <v>8</v>
+      </c>
+      <c r="C15">
+        <v>26</v>
+      </c>
+      <c r="D15" t="s">
+        <v>39</v>
+      </c>
+      <c r="E15" t="s">
+        <v>42</v>
+      </c>
+      <c r="F15">
+        <v>12</v>
+      </c>
+      <c r="G15">
+        <v>4</v>
+      </c>
+      <c r="H15">
+        <v>0.86</v>
+      </c>
+      <c r="I15">
+        <v>-999</v>
+      </c>
+      <c r="J15">
+        <v>1.59</v>
+      </c>
+      <c r="K15">
+        <v>0.86</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>2019</v>
+      </c>
+      <c r="B16">
+        <v>8</v>
+      </c>
+      <c r="C16">
+        <v>26</v>
+      </c>
+      <c r="D16" t="s">
+        <v>39</v>
+      </c>
+      <c r="E16" t="s">
+        <v>42</v>
+      </c>
+      <c r="F16">
+        <v>12</v>
+      </c>
+      <c r="G16">
+        <v>3</v>
+      </c>
+      <c r="H16">
+        <v>0.86</v>
+      </c>
+      <c r="I16">
+        <v>-999</v>
+      </c>
+      <c r="J16">
+        <v>0.86</v>
+      </c>
+      <c r="K16">
+        <v>0.86</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>2019</v>
+      </c>
+      <c r="B17">
+        <v>8</v>
+      </c>
+      <c r="C17">
+        <v>26</v>
+      </c>
+      <c r="D17" t="s">
+        <v>39</v>
+      </c>
+      <c r="E17" t="s">
+        <v>42</v>
+      </c>
+      <c r="F17">
+        <v>12</v>
+      </c>
+      <c r="G17">
+        <v>2</v>
+      </c>
+      <c r="H17">
+        <v>0.86</v>
+      </c>
+      <c r="I17">
+        <v>-999</v>
+      </c>
+      <c r="J17">
+        <v>4.08</v>
+      </c>
+      <c r="K17">
+        <v>0.86</v>
       </c>
     </row>
   </sheetData>
@@ -1260,737 +1820,737 @@
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="str">
         <f>IF(raw_data_1!A2=raw_data_2!A2,"","check")</f>
-        <v/>
+        <v>check</v>
       </c>
       <c r="B2" t="str">
         <f>IF(raw_data_1!B2=raw_data_2!B2,"","check")</f>
-        <v/>
+        <v>check</v>
       </c>
       <c r="C2" t="str">
         <f>IF(raw_data_1!C2=raw_data_2!C2,"","check")</f>
-        <v/>
+        <v>check</v>
       </c>
       <c r="D2" t="str">
         <f>IF(raw_data_1!D2=raw_data_2!D2,"","check")</f>
-        <v/>
+        <v>check</v>
       </c>
       <c r="E2" t="str">
         <f>IF(raw_data_1!E2=raw_data_2!E2,"","check")</f>
-        <v/>
+        <v>check</v>
       </c>
       <c r="F2" t="str">
         <f>IF(raw_data_1!F2=raw_data_2!F2,"","check")</f>
-        <v/>
+        <v>check</v>
       </c>
       <c r="G2" t="str">
         <f>IF(raw_data_1!G2=raw_data_2!G2,"","check")</f>
-        <v/>
+        <v>check</v>
       </c>
       <c r="H2" t="str">
         <f>IF(raw_data_1!H2=raw_data_2!H2,"","check")</f>
-        <v/>
+        <v>check</v>
       </c>
       <c r="I2" t="str">
         <f>IF(raw_data_1!I2=raw_data_2!I2,"","check")</f>
-        <v/>
+        <v>check</v>
       </c>
       <c r="J2" t="str">
         <f>IF(raw_data_1!J2=raw_data_2!J2,"","check")</f>
-        <v/>
+        <v>check</v>
       </c>
       <c r="K2" t="str">
         <f>IF(raw_data_1!K2=raw_data_2!K2,"","check")</f>
-        <v/>
+        <v>check</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" t="str">
         <f>IF(raw_data_1!A3=raw_data_2!A3,"","check")</f>
-        <v/>
+        <v>check</v>
       </c>
       <c r="B3" t="str">
         <f>IF(raw_data_1!B3=raw_data_2!B3,"","check")</f>
-        <v/>
+        <v>check</v>
       </c>
       <c r="C3" t="str">
         <f>IF(raw_data_1!C3=raw_data_2!C3,"","check")</f>
-        <v/>
+        <v>check</v>
       </c>
       <c r="D3" t="str">
         <f>IF(raw_data_1!D3=raw_data_2!D3,"","check")</f>
-        <v/>
+        <v>check</v>
       </c>
       <c r="E3" t="str">
         <f>IF(raw_data_1!E3=raw_data_2!E3,"","check")</f>
-        <v/>
+        <v>check</v>
       </c>
       <c r="F3" t="str">
         <f>IF(raw_data_1!F3=raw_data_2!F3,"","check")</f>
-        <v/>
+        <v>check</v>
       </c>
       <c r="G3" t="str">
         <f>IF(raw_data_1!G3=raw_data_2!G3,"","check")</f>
-        <v/>
+        <v>check</v>
       </c>
       <c r="H3" t="str">
         <f>IF(raw_data_1!H3=raw_data_2!H3,"","check")</f>
-        <v/>
+        <v>check</v>
       </c>
       <c r="I3" t="str">
         <f>IF(raw_data_1!I3=raw_data_2!I3,"","check")</f>
-        <v/>
+        <v>check</v>
       </c>
       <c r="J3" t="str">
         <f>IF(raw_data_1!J3=raw_data_2!J3,"","check")</f>
-        <v/>
+        <v>check</v>
       </c>
       <c r="K3" t="str">
         <f>IF(raw_data_1!K3=raw_data_2!K3,"","check")</f>
-        <v/>
+        <v>check</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" t="str">
         <f>IF(raw_data_1!A4=raw_data_2!A4,"","check")</f>
-        <v/>
+        <v>check</v>
       </c>
       <c r="B4" t="str">
         <f>IF(raw_data_1!B4=raw_data_2!B4,"","check")</f>
-        <v/>
+        <v>check</v>
       </c>
       <c r="C4" t="str">
         <f>IF(raw_data_1!C4=raw_data_2!C4,"","check")</f>
-        <v/>
+        <v>check</v>
       </c>
       <c r="D4" t="str">
         <f>IF(raw_data_1!D4=raw_data_2!D4,"","check")</f>
-        <v/>
+        <v>check</v>
       </c>
       <c r="E4" t="str">
         <f>IF(raw_data_1!E4=raw_data_2!E4,"","check")</f>
-        <v/>
+        <v>check</v>
       </c>
       <c r="F4" t="str">
         <f>IF(raw_data_1!F4=raw_data_2!F4,"","check")</f>
-        <v/>
+        <v>check</v>
       </c>
       <c r="G4" t="str">
         <f>IF(raw_data_1!G4=raw_data_2!G4,"","check")</f>
-        <v/>
+        <v>check</v>
       </c>
       <c r="H4" t="str">
         <f>IF(raw_data_1!H4=raw_data_2!H4,"","check")</f>
-        <v/>
+        <v>check</v>
       </c>
       <c r="I4" t="str">
         <f>IF(raw_data_1!I4=raw_data_2!I4,"","check")</f>
-        <v/>
+        <v>check</v>
       </c>
       <c r="J4" t="str">
         <f>IF(raw_data_1!J4=raw_data_2!J4,"","check")</f>
-        <v/>
+        <v>check</v>
       </c>
       <c r="K4" t="str">
         <f>IF(raw_data_1!K4=raw_data_2!K4,"","check")</f>
-        <v/>
+        <v>check</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" t="str">
         <f>IF(raw_data_1!A5=raw_data_2!A5,"","check")</f>
-        <v/>
+        <v>check</v>
       </c>
       <c r="B5" t="str">
         <f>IF(raw_data_1!B5=raw_data_2!B5,"","check")</f>
-        <v/>
+        <v>check</v>
       </c>
       <c r="C5" t="str">
         <f>IF(raw_data_1!C5=raw_data_2!C5,"","check")</f>
-        <v/>
+        <v>check</v>
       </c>
       <c r="D5" t="str">
         <f>IF(raw_data_1!D5=raw_data_2!D5,"","check")</f>
-        <v/>
+        <v>check</v>
       </c>
       <c r="E5" t="str">
         <f>IF(raw_data_1!E5=raw_data_2!E5,"","check")</f>
-        <v/>
+        <v>check</v>
       </c>
       <c r="F5" t="str">
         <f>IF(raw_data_1!F5=raw_data_2!F5,"","check")</f>
-        <v/>
+        <v>check</v>
       </c>
       <c r="G5" t="str">
         <f>IF(raw_data_1!G5=raw_data_2!G5,"","check")</f>
-        <v/>
+        <v>check</v>
       </c>
       <c r="H5" t="str">
         <f>IF(raw_data_1!H5=raw_data_2!H5,"","check")</f>
-        <v/>
+        <v>check</v>
       </c>
       <c r="I5" t="str">
         <f>IF(raw_data_1!I5=raw_data_2!I5,"","check")</f>
-        <v/>
+        <v>check</v>
       </c>
       <c r="J5" t="str">
         <f>IF(raw_data_1!J5=raw_data_2!J5,"","check")</f>
-        <v/>
+        <v>check</v>
       </c>
       <c r="K5" t="str">
         <f>IF(raw_data_1!K5=raw_data_2!K5,"","check")</f>
-        <v/>
+        <v>check</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" t="str">
         <f>IF(raw_data_1!A6=raw_data_2!A6,"","check")</f>
-        <v/>
+        <v>check</v>
       </c>
       <c r="B6" t="str">
         <f>IF(raw_data_1!B6=raw_data_2!B6,"","check")</f>
-        <v/>
+        <v>check</v>
       </c>
       <c r="C6" t="str">
         <f>IF(raw_data_1!C6=raw_data_2!C6,"","check")</f>
-        <v/>
+        <v>check</v>
       </c>
       <c r="D6" t="str">
         <f>IF(raw_data_1!D6=raw_data_2!D6,"","check")</f>
-        <v/>
+        <v>check</v>
       </c>
       <c r="E6" t="str">
         <f>IF(raw_data_1!E6=raw_data_2!E6,"","check")</f>
-        <v/>
+        <v>check</v>
       </c>
       <c r="F6" t="str">
         <f>IF(raw_data_1!F6=raw_data_2!F6,"","check")</f>
-        <v/>
+        <v>check</v>
       </c>
       <c r="G6" t="str">
         <f>IF(raw_data_1!G6=raw_data_2!G6,"","check")</f>
-        <v/>
+        <v>check</v>
       </c>
       <c r="H6" t="str">
         <f>IF(raw_data_1!H6=raw_data_2!H6,"","check")</f>
-        <v/>
+        <v>check</v>
       </c>
       <c r="I6" t="str">
         <f>IF(raw_data_1!I6=raw_data_2!I6,"","check")</f>
-        <v/>
+        <v>check</v>
       </c>
       <c r="J6" t="str">
         <f>IF(raw_data_1!J6=raw_data_2!J6,"","check")</f>
-        <v/>
+        <v>check</v>
       </c>
       <c r="K6" t="str">
         <f>IF(raw_data_1!K6=raw_data_2!K6,"","check")</f>
-        <v/>
+        <v>check</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" t="str">
         <f>IF(raw_data_1!A7=raw_data_2!A7,"","check")</f>
-        <v/>
+        <v>check</v>
       </c>
       <c r="B7" t="str">
         <f>IF(raw_data_1!B7=raw_data_2!B7,"","check")</f>
-        <v/>
+        <v>check</v>
       </c>
       <c r="C7" t="str">
         <f>IF(raw_data_1!C7=raw_data_2!C7,"","check")</f>
-        <v/>
+        <v>check</v>
       </c>
       <c r="D7" t="str">
         <f>IF(raw_data_1!D7=raw_data_2!D7,"","check")</f>
-        <v/>
+        <v>check</v>
       </c>
       <c r="E7" t="str">
         <f>IF(raw_data_1!E7=raw_data_2!E7,"","check")</f>
-        <v/>
+        <v>check</v>
       </c>
       <c r="F7" t="str">
         <f>IF(raw_data_1!F7=raw_data_2!F7,"","check")</f>
-        <v/>
+        <v>check</v>
       </c>
       <c r="G7" t="str">
         <f>IF(raw_data_1!G7=raw_data_2!G7,"","check")</f>
-        <v/>
+        <v>check</v>
       </c>
       <c r="H7" t="str">
         <f>IF(raw_data_1!H7=raw_data_2!H7,"","check")</f>
-        <v/>
+        <v>check</v>
       </c>
       <c r="I7" t="str">
         <f>IF(raw_data_1!I7=raw_data_2!I7,"","check")</f>
-        <v/>
+        <v>check</v>
       </c>
       <c r="J7" t="str">
         <f>IF(raw_data_1!J7=raw_data_2!J7,"","check")</f>
-        <v/>
+        <v>check</v>
       </c>
       <c r="K7" t="str">
         <f>IF(raw_data_1!K7=raw_data_2!K7,"","check")</f>
-        <v/>
+        <v>check</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" t="str">
         <f>IF(raw_data_1!A8=raw_data_2!A8,"","check")</f>
-        <v/>
+        <v>check</v>
       </c>
       <c r="B8" t="str">
         <f>IF(raw_data_1!B8=raw_data_2!B8,"","check")</f>
-        <v/>
+        <v>check</v>
       </c>
       <c r="C8" t="str">
         <f>IF(raw_data_1!C8=raw_data_2!C8,"","check")</f>
-        <v/>
+        <v>check</v>
       </c>
       <c r="D8" t="str">
         <f>IF(raw_data_1!D8=raw_data_2!D8,"","check")</f>
-        <v/>
+        <v>check</v>
       </c>
       <c r="E8" t="str">
         <f>IF(raw_data_1!E8=raw_data_2!E8,"","check")</f>
-        <v/>
+        <v>check</v>
       </c>
       <c r="F8" t="str">
         <f>IF(raw_data_1!F8=raw_data_2!F8,"","check")</f>
-        <v/>
+        <v>check</v>
       </c>
       <c r="G8" t="str">
         <f>IF(raw_data_1!G8=raw_data_2!G8,"","check")</f>
-        <v/>
+        <v>check</v>
       </c>
       <c r="H8" t="str">
         <f>IF(raw_data_1!H8=raw_data_2!H8,"","check")</f>
-        <v/>
+        <v>check</v>
       </c>
       <c r="I8" t="str">
         <f>IF(raw_data_1!I8=raw_data_2!I8,"","check")</f>
-        <v/>
+        <v>check</v>
       </c>
       <c r="J8" t="str">
         <f>IF(raw_data_1!J8=raw_data_2!J8,"","check")</f>
-        <v/>
+        <v>check</v>
       </c>
       <c r="K8" t="str">
         <f>IF(raw_data_1!K8=raw_data_2!K8,"","check")</f>
-        <v/>
+        <v>check</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" t="str">
         <f>IF(raw_data_1!A9=raw_data_2!A9,"","check")</f>
-        <v/>
+        <v>check</v>
       </c>
       <c r="B9" t="str">
         <f>IF(raw_data_1!B9=raw_data_2!B9,"","check")</f>
-        <v/>
+        <v>check</v>
       </c>
       <c r="C9" t="str">
         <f>IF(raw_data_1!C9=raw_data_2!C9,"","check")</f>
-        <v/>
+        <v>check</v>
       </c>
       <c r="D9" t="str">
         <f>IF(raw_data_1!D9=raw_data_2!D9,"","check")</f>
-        <v/>
+        <v>check</v>
       </c>
       <c r="E9" t="str">
         <f>IF(raw_data_1!E9=raw_data_2!E9,"","check")</f>
-        <v/>
+        <v>check</v>
       </c>
       <c r="F9" t="str">
         <f>IF(raw_data_1!F9=raw_data_2!F9,"","check")</f>
-        <v/>
+        <v>check</v>
       </c>
       <c r="G9" t="str">
         <f>IF(raw_data_1!G9=raw_data_2!G9,"","check")</f>
-        <v/>
+        <v>check</v>
       </c>
       <c r="H9" t="str">
         <f>IF(raw_data_1!H9=raw_data_2!H9,"","check")</f>
-        <v/>
+        <v>check</v>
       </c>
       <c r="I9" t="str">
         <f>IF(raw_data_1!I9=raw_data_2!I9,"","check")</f>
-        <v/>
+        <v>check</v>
       </c>
       <c r="J9" t="str">
         <f>IF(raw_data_1!J9=raw_data_2!J9,"","check")</f>
-        <v/>
+        <v>check</v>
       </c>
       <c r="K9" t="str">
         <f>IF(raw_data_1!K9=raw_data_2!K9,"","check")</f>
-        <v/>
+        <v>check</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" t="str">
         <f>IF(raw_data_1!A10=raw_data_2!A10,"","check")</f>
-        <v/>
+        <v>check</v>
       </c>
       <c r="B10" t="str">
         <f>IF(raw_data_1!B10=raw_data_2!B10,"","check")</f>
-        <v/>
+        <v>check</v>
       </c>
       <c r="C10" t="str">
         <f>IF(raw_data_1!C10=raw_data_2!C10,"","check")</f>
-        <v/>
+        <v>check</v>
       </c>
       <c r="D10" t="str">
         <f>IF(raw_data_1!D10=raw_data_2!D10,"","check")</f>
-        <v/>
+        <v>check</v>
       </c>
       <c r="E10" t="str">
         <f>IF(raw_data_1!E10=raw_data_2!E10,"","check")</f>
-        <v/>
+        <v>check</v>
       </c>
       <c r="F10" t="str">
         <f>IF(raw_data_1!F10=raw_data_2!F10,"","check")</f>
-        <v/>
+        <v>check</v>
       </c>
       <c r="G10" t="str">
         <f>IF(raw_data_1!G10=raw_data_2!G10,"","check")</f>
-        <v/>
+        <v>check</v>
       </c>
       <c r="H10" t="str">
         <f>IF(raw_data_1!H10=raw_data_2!H10,"","check")</f>
-        <v/>
+        <v>check</v>
       </c>
       <c r="I10" t="str">
         <f>IF(raw_data_1!I10=raw_data_2!I10,"","check")</f>
-        <v/>
+        <v>check</v>
       </c>
       <c r="J10" t="str">
         <f>IF(raw_data_1!J10=raw_data_2!J10,"","check")</f>
-        <v/>
+        <v>check</v>
       </c>
       <c r="K10" t="str">
         <f>IF(raw_data_1!K10=raw_data_2!K10,"","check")</f>
-        <v/>
+        <v>check</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" t="str">
         <f>IF(raw_data_1!A11=raw_data_2!A11,"","check")</f>
-        <v/>
+        <v>check</v>
       </c>
       <c r="B11" t="str">
         <f>IF(raw_data_1!B11=raw_data_2!B11,"","check")</f>
-        <v/>
+        <v>check</v>
       </c>
       <c r="C11" t="str">
         <f>IF(raw_data_1!C11=raw_data_2!C11,"","check")</f>
-        <v/>
+        <v>check</v>
       </c>
       <c r="D11" t="str">
         <f>IF(raw_data_1!D11=raw_data_2!D11,"","check")</f>
-        <v/>
+        <v>check</v>
       </c>
       <c r="E11" t="str">
         <f>IF(raw_data_1!E11=raw_data_2!E11,"","check")</f>
-        <v/>
+        <v>check</v>
       </c>
       <c r="F11" t="str">
         <f>IF(raw_data_1!F11=raw_data_2!F11,"","check")</f>
-        <v/>
+        <v>check</v>
       </c>
       <c r="G11" t="str">
         <f>IF(raw_data_1!G11=raw_data_2!G11,"","check")</f>
-        <v/>
+        <v>check</v>
       </c>
       <c r="H11" t="str">
         <f>IF(raw_data_1!H11=raw_data_2!H11,"","check")</f>
-        <v/>
+        <v>check</v>
       </c>
       <c r="I11" t="str">
         <f>IF(raw_data_1!I11=raw_data_2!I11,"","check")</f>
-        <v/>
+        <v>check</v>
       </c>
       <c r="J11" t="str">
         <f>IF(raw_data_1!J11=raw_data_2!J11,"","check")</f>
-        <v/>
+        <v>check</v>
       </c>
       <c r="K11" t="str">
         <f>IF(raw_data_1!K11=raw_data_2!K11,"","check")</f>
-        <v/>
+        <v>check</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" t="str">
         <f>IF(raw_data_1!A12=raw_data_2!A12,"","check")</f>
-        <v/>
+        <v>check</v>
       </c>
       <c r="B12" t="str">
         <f>IF(raw_data_1!B12=raw_data_2!B12,"","check")</f>
-        <v/>
+        <v>check</v>
       </c>
       <c r="C12" t="str">
         <f>IF(raw_data_1!C12=raw_data_2!C12,"","check")</f>
-        <v/>
+        <v>check</v>
       </c>
       <c r="D12" t="str">
         <f>IF(raw_data_1!D12=raw_data_2!D12,"","check")</f>
-        <v/>
+        <v>check</v>
       </c>
       <c r="E12" t="str">
         <f>IF(raw_data_1!E12=raw_data_2!E12,"","check")</f>
-        <v/>
+        <v>check</v>
       </c>
       <c r="F12" t="str">
         <f>IF(raw_data_1!F12=raw_data_2!F12,"","check")</f>
-        <v/>
+        <v>check</v>
       </c>
       <c r="G12" t="str">
         <f>IF(raw_data_1!G12=raw_data_2!G12,"","check")</f>
-        <v/>
+        <v>check</v>
       </c>
       <c r="H12" t="str">
         <f>IF(raw_data_1!H12=raw_data_2!H12,"","check")</f>
-        <v/>
+        <v>check</v>
       </c>
       <c r="I12" t="str">
         <f>IF(raw_data_1!I12=raw_data_2!I12,"","check")</f>
-        <v/>
+        <v>check</v>
       </c>
       <c r="J12" t="str">
         <f>IF(raw_data_1!J12=raw_data_2!J12,"","check")</f>
-        <v/>
+        <v>check</v>
       </c>
       <c r="K12" t="str">
         <f>IF(raw_data_1!K12=raw_data_2!K12,"","check")</f>
-        <v/>
+        <v>check</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" t="str">
         <f>IF(raw_data_1!A13=raw_data_2!A13,"","check")</f>
-        <v/>
+        <v>check</v>
       </c>
       <c r="B13" t="str">
         <f>IF(raw_data_1!B13=raw_data_2!B13,"","check")</f>
-        <v/>
+        <v>check</v>
       </c>
       <c r="C13" t="str">
         <f>IF(raw_data_1!C13=raw_data_2!C13,"","check")</f>
-        <v/>
+        <v>check</v>
       </c>
       <c r="D13" t="str">
         <f>IF(raw_data_1!D13=raw_data_2!D13,"","check")</f>
-        <v/>
+        <v>check</v>
       </c>
       <c r="E13" t="str">
         <f>IF(raw_data_1!E13=raw_data_2!E13,"","check")</f>
-        <v/>
+        <v>check</v>
       </c>
       <c r="F13" t="str">
         <f>IF(raw_data_1!F13=raw_data_2!F13,"","check")</f>
-        <v/>
+        <v>check</v>
       </c>
       <c r="G13" t="str">
         <f>IF(raw_data_1!G13=raw_data_2!G13,"","check")</f>
-        <v/>
+        <v>check</v>
       </c>
       <c r="H13" t="str">
         <f>IF(raw_data_1!H13=raw_data_2!H13,"","check")</f>
-        <v/>
+        <v>check</v>
       </c>
       <c r="I13" t="str">
         <f>IF(raw_data_1!I13=raw_data_2!I13,"","check")</f>
-        <v/>
+        <v>check</v>
       </c>
       <c r="J13" t="str">
         <f>IF(raw_data_1!J13=raw_data_2!J13,"","check")</f>
-        <v/>
+        <v>check</v>
       </c>
       <c r="K13" t="str">
         <f>IF(raw_data_1!K13=raw_data_2!K13,"","check")</f>
-        <v/>
+        <v>check</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" t="str">
         <f>IF(raw_data_1!A14=raw_data_2!A14,"","check")</f>
-        <v/>
+        <v>check</v>
       </c>
       <c r="B14" t="str">
         <f>IF(raw_data_1!B14=raw_data_2!B14,"","check")</f>
-        <v/>
+        <v>check</v>
       </c>
       <c r="C14" t="str">
         <f>IF(raw_data_1!C14=raw_data_2!C14,"","check")</f>
-        <v/>
+        <v>check</v>
       </c>
       <c r="D14" t="str">
         <f>IF(raw_data_1!D14=raw_data_2!D14,"","check")</f>
-        <v/>
+        <v>check</v>
       </c>
       <c r="E14" t="str">
         <f>IF(raw_data_1!E14=raw_data_2!E14,"","check")</f>
-        <v/>
+        <v>check</v>
       </c>
       <c r="F14" t="str">
         <f>IF(raw_data_1!F14=raw_data_2!F14,"","check")</f>
-        <v/>
+        <v>check</v>
       </c>
       <c r="G14" t="str">
         <f>IF(raw_data_1!G14=raw_data_2!G14,"","check")</f>
-        <v/>
+        <v>check</v>
       </c>
       <c r="H14" t="str">
         <f>IF(raw_data_1!H14=raw_data_2!H14,"","check")</f>
-        <v/>
+        <v>check</v>
       </c>
       <c r="I14" t="str">
         <f>IF(raw_data_1!I14=raw_data_2!I14,"","check")</f>
-        <v/>
+        <v>check</v>
       </c>
       <c r="J14" t="str">
         <f>IF(raw_data_1!J14=raw_data_2!J14,"","check")</f>
-        <v/>
+        <v>check</v>
       </c>
       <c r="K14" t="str">
         <f>IF(raw_data_1!K14=raw_data_2!K14,"","check")</f>
-        <v/>
+        <v>check</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" t="str">
         <f>IF(raw_data_1!A15=raw_data_2!A15,"","check")</f>
-        <v/>
+        <v>check</v>
       </c>
       <c r="B15" t="str">
         <f>IF(raw_data_1!B15=raw_data_2!B15,"","check")</f>
-        <v/>
+        <v>check</v>
       </c>
       <c r="C15" t="str">
         <f>IF(raw_data_1!C15=raw_data_2!C15,"","check")</f>
-        <v/>
+        <v>check</v>
       </c>
       <c r="D15" t="str">
         <f>IF(raw_data_1!D15=raw_data_2!D15,"","check")</f>
-        <v/>
+        <v>check</v>
       </c>
       <c r="E15" t="str">
         <f>IF(raw_data_1!E15=raw_data_2!E15,"","check")</f>
-        <v/>
+        <v>check</v>
       </c>
       <c r="F15" t="str">
         <f>IF(raw_data_1!F15=raw_data_2!F15,"","check")</f>
-        <v/>
+        <v>check</v>
       </c>
       <c r="G15" t="str">
         <f>IF(raw_data_1!G15=raw_data_2!G15,"","check")</f>
-        <v/>
+        <v>check</v>
       </c>
       <c r="H15" t="str">
         <f>IF(raw_data_1!H15=raw_data_2!H15,"","check")</f>
-        <v/>
+        <v>check</v>
       </c>
       <c r="I15" t="str">
         <f>IF(raw_data_1!I15=raw_data_2!I15,"","check")</f>
-        <v/>
+        <v>check</v>
       </c>
       <c r="J15" t="str">
         <f>IF(raw_data_1!J15=raw_data_2!J15,"","check")</f>
-        <v/>
+        <v>check</v>
       </c>
       <c r="K15" t="str">
         <f>IF(raw_data_1!K15=raw_data_2!K15,"","check")</f>
-        <v/>
+        <v>check</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" t="str">
         <f>IF(raw_data_1!A16=raw_data_2!A16,"","check")</f>
-        <v/>
+        <v>check</v>
       </c>
       <c r="B16" t="str">
         <f>IF(raw_data_1!B16=raw_data_2!B16,"","check")</f>
-        <v/>
+        <v>check</v>
       </c>
       <c r="C16" t="str">
         <f>IF(raw_data_1!C16=raw_data_2!C16,"","check")</f>
-        <v/>
+        <v>check</v>
       </c>
       <c r="D16" t="str">
         <f>IF(raw_data_1!D16=raw_data_2!D16,"","check")</f>
-        <v/>
+        <v>check</v>
       </c>
       <c r="E16" t="str">
         <f>IF(raw_data_1!E16=raw_data_2!E16,"","check")</f>
-        <v/>
+        <v>check</v>
       </c>
       <c r="F16" t="str">
         <f>IF(raw_data_1!F16=raw_data_2!F16,"","check")</f>
-        <v/>
+        <v>check</v>
       </c>
       <c r="G16" t="str">
         <f>IF(raw_data_1!G16=raw_data_2!G16,"","check")</f>
-        <v/>
+        <v>check</v>
       </c>
       <c r="H16" t="str">
         <f>IF(raw_data_1!H16=raw_data_2!H16,"","check")</f>
-        <v/>
+        <v>check</v>
       </c>
       <c r="I16" t="str">
         <f>IF(raw_data_1!I16=raw_data_2!I16,"","check")</f>
-        <v/>
+        <v>check</v>
       </c>
       <c r="J16" t="str">
         <f>IF(raw_data_1!J16=raw_data_2!J16,"","check")</f>
-        <v/>
+        <v>check</v>
       </c>
       <c r="K16" t="str">
         <f>IF(raw_data_1!K16=raw_data_2!K16,"","check")</f>
-        <v/>
+        <v>check</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" t="str">
         <f>IF(raw_data_1!A17=raw_data_2!A17,"","check")</f>
-        <v/>
+        <v>check</v>
       </c>
       <c r="B17" t="str">
         <f>IF(raw_data_1!B17=raw_data_2!B17,"","check")</f>
-        <v/>
+        <v>check</v>
       </c>
       <c r="C17" t="str">
         <f>IF(raw_data_1!C17=raw_data_2!C17,"","check")</f>
-        <v/>
+        <v>check</v>
       </c>
       <c r="D17" t="str">
         <f>IF(raw_data_1!D17=raw_data_2!D17,"","check")</f>
-        <v/>
+        <v>check</v>
       </c>
       <c r="E17" t="str">
         <f>IF(raw_data_1!E17=raw_data_2!E17,"","check")</f>
-        <v/>
+        <v>check</v>
       </c>
       <c r="F17" t="str">
         <f>IF(raw_data_1!F17=raw_data_2!F17,"","check")</f>
-        <v/>
+        <v>check</v>
       </c>
       <c r="G17" t="str">
         <f>IF(raw_data_1!G17=raw_data_2!G17,"","check")</f>
-        <v/>
+        <v>check</v>
       </c>
       <c r="H17" t="str">
         <f>IF(raw_data_1!H17=raw_data_2!H17,"","check")</f>
-        <v/>
+        <v>check</v>
       </c>
       <c r="I17" t="str">
         <f>IF(raw_data_1!I17=raw_data_2!I17,"","check")</f>
-        <v/>
+        <v>check</v>
       </c>
       <c r="J17" t="str">
         <f>IF(raw_data_1!J17=raw_data_2!J17,"","check")</f>
-        <v/>
+        <v>check</v>
       </c>
       <c r="K17" t="str">
         <f>IF(raw_data_1!K17=raw_data_2!K17,"","check")</f>
-        <v/>
+        <v>check</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Aug 26 data processing/prelim figures complete
</commit_message>
<xml_diff>
--- a/Oyster/cultchmass/cultchmass_packet.xlsx
+++ b/Oyster/cultchmass/cultchmass_packet.xlsx
@@ -4,12 +4,12 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="datasheet" sheetId="1" r:id="rId1"/>
     <sheet name="raw_data_1" sheetId="2" r:id="rId2"/>
-    <sheet name="raw_data_2" sheetId="7" r:id="rId3"/>
+    <sheet name="raw_data_2" sheetId="8" r:id="rId3"/>
     <sheet name="raw_check" sheetId="4" r:id="rId4"/>
     <sheet name="pick" sheetId="5" r:id="rId5"/>
     <sheet name="description" sheetId="6" r:id="rId6"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="53">
   <si>
     <t>REEF MASS FIELD DATASHEET</t>
   </si>
@@ -156,6 +156,33 @@
   </si>
   <si>
     <t>mass of the weighing bucket plus all reef material retained in the 5 x 5cm seive in kg.  This excludes the material retained in the 10 x 10cm seive.</t>
+  </si>
+  <si>
+    <t>collector</t>
+  </si>
+  <si>
+    <t>recorder</t>
+  </si>
+  <si>
+    <t>sb</t>
+  </si>
+  <si>
+    <t>person collecting data</t>
+  </si>
+  <si>
+    <t>person recording data</t>
+  </si>
+  <si>
+    <t>pf</t>
+  </si>
+  <si>
+    <t>sbpf</t>
+  </si>
+  <si>
+    <t>at</t>
+  </si>
+  <si>
+    <t>jh</t>
   </si>
 </sst>
 </file>
@@ -1012,10 +1039,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K17"/>
+  <dimension ref="A1:M17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O20" sqref="O20"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="N18" sqref="N18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1023,7 +1050,7 @@
     <col min="8" max="8" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>16</v>
       </c>
@@ -1057,8 +1084,14 @@
       <c r="K1" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L1" t="s">
+        <v>44</v>
+      </c>
+      <c r="M1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>2019</v>
       </c>
@@ -1092,8 +1125,14 @@
       <c r="K2">
         <v>1.06</v>
       </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L2" t="s">
+        <v>50</v>
+      </c>
+      <c r="M2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2019</v>
       </c>
@@ -1127,8 +1166,14 @@
       <c r="K3">
         <v>1.08</v>
       </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L3" t="s">
+        <v>50</v>
+      </c>
+      <c r="M3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2019</v>
       </c>
@@ -1162,8 +1207,14 @@
       <c r="K4">
         <v>1.06</v>
       </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L4" t="s">
+        <v>50</v>
+      </c>
+      <c r="M4" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>2019</v>
       </c>
@@ -1197,8 +1248,14 @@
       <c r="K5">
         <v>1.86</v>
       </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L5" t="s">
+        <v>50</v>
+      </c>
+      <c r="M5" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>2019</v>
       </c>
@@ -1232,8 +1289,14 @@
       <c r="K6">
         <v>1.22</v>
       </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L6" t="s">
+        <v>50</v>
+      </c>
+      <c r="M6" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>2019</v>
       </c>
@@ -1267,8 +1330,14 @@
       <c r="K7">
         <v>1.6</v>
       </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L7" t="s">
+        <v>50</v>
+      </c>
+      <c r="M7" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>2019</v>
       </c>
@@ -1302,8 +1371,14 @@
       <c r="K8">
         <v>0.96</v>
       </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L8" t="s">
+        <v>50</v>
+      </c>
+      <c r="M8" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>2019</v>
       </c>
@@ -1337,8 +1412,14 @@
       <c r="K9">
         <v>0.86</v>
       </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L9" t="s">
+        <v>50</v>
+      </c>
+      <c r="M9" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>2019</v>
       </c>
@@ -1372,8 +1453,14 @@
       <c r="K10">
         <v>2.15</v>
       </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L10" t="s">
+        <v>50</v>
+      </c>
+      <c r="M10" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>2019</v>
       </c>
@@ -1407,8 +1494,14 @@
       <c r="K11">
         <v>2.4900000000000002</v>
       </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L11" t="s">
+        <v>50</v>
+      </c>
+      <c r="M11" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>2019</v>
       </c>
@@ -1442,8 +1535,14 @@
       <c r="K12">
         <v>7.03</v>
       </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L12" t="s">
+        <v>50</v>
+      </c>
+      <c r="M12" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>2019</v>
       </c>
@@ -1477,8 +1576,14 @@
       <c r="K13">
         <v>1.25</v>
       </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L13" t="s">
+        <v>50</v>
+      </c>
+      <c r="M13" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>2019</v>
       </c>
@@ -1512,8 +1617,14 @@
       <c r="K14">
         <v>2.15</v>
       </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L14" t="s">
+        <v>50</v>
+      </c>
+      <c r="M14" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>2019</v>
       </c>
@@ -1547,8 +1658,14 @@
       <c r="K15">
         <v>0.86</v>
       </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L15" t="s">
+        <v>50</v>
+      </c>
+      <c r="M15" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>2019</v>
       </c>
@@ -1582,8 +1699,14 @@
       <c r="K16">
         <v>0.86</v>
       </c>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L16" t="s">
+        <v>50</v>
+      </c>
+      <c r="M16" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>2019</v>
       </c>
@@ -1616,13 +1739,19 @@
       </c>
       <c r="K17">
         <v>0.86</v>
+      </c>
+      <c r="L17" t="s">
+        <v>50</v>
+      </c>
+      <c r="M17" t="s">
+        <v>50</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="7">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="9">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>pick!$A$2</xm:f>
@@ -1665,6 +1794,18 @@
           </x14:formula1>
           <xm:sqref>G1:G1048576</xm:sqref>
         </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>pick!$L$2:$L$12</xm:f>
+          </x14:formula1>
+          <xm:sqref>L1:L1048576</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>pick!$M$2:$M$16</xm:f>
+          </x14:formula1>
+          <xm:sqref>M1:M1048576</xm:sqref>
+        </x14:dataValidation>
       </x14:dataValidations>
     </ext>
   </extLst>
@@ -1673,10 +1814,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K1"/>
+  <dimension ref="A1:M17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O19" sqref="O19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1684,7 +1825,7 @@
     <col min="8" max="8" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>16</v>
       </c>
@@ -1717,13 +1858,675 @@
       </c>
       <c r="K1" t="s">
         <v>37</v>
+      </c>
+      <c r="L1" t="s">
+        <v>44</v>
+      </c>
+      <c r="M1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>2019</v>
+      </c>
+      <c r="B2">
+        <v>8</v>
+      </c>
+      <c r="C2">
+        <v>26</v>
+      </c>
+      <c r="D2" t="s">
+        <v>39</v>
+      </c>
+      <c r="E2" t="s">
+        <v>42</v>
+      </c>
+      <c r="F2">
+        <v>19</v>
+      </c>
+      <c r="G2">
+        <v>1</v>
+      </c>
+      <c r="H2">
+        <v>0.86</v>
+      </c>
+      <c r="I2">
+        <v>16.920000000000002</v>
+      </c>
+      <c r="J2">
+        <v>0.86</v>
+      </c>
+      <c r="K2">
+        <v>1.06</v>
+      </c>
+      <c r="L2" t="s">
+        <v>50</v>
+      </c>
+      <c r="M2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2019</v>
+      </c>
+      <c r="B3">
+        <v>8</v>
+      </c>
+      <c r="C3">
+        <v>26</v>
+      </c>
+      <c r="D3" t="s">
+        <v>39</v>
+      </c>
+      <c r="E3" t="s">
+        <v>42</v>
+      </c>
+      <c r="F3">
+        <v>19</v>
+      </c>
+      <c r="G3">
+        <v>2</v>
+      </c>
+      <c r="H3">
+        <v>0.86</v>
+      </c>
+      <c r="I3">
+        <v>13.7</v>
+      </c>
+      <c r="J3">
+        <v>0.86</v>
+      </c>
+      <c r="K3">
+        <v>1.08</v>
+      </c>
+      <c r="L3" t="s">
+        <v>50</v>
+      </c>
+      <c r="M3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>2019</v>
+      </c>
+      <c r="B4">
+        <v>8</v>
+      </c>
+      <c r="C4">
+        <v>26</v>
+      </c>
+      <c r="D4" t="s">
+        <v>39</v>
+      </c>
+      <c r="E4" t="s">
+        <v>42</v>
+      </c>
+      <c r="F4">
+        <v>19</v>
+      </c>
+      <c r="G4">
+        <v>3</v>
+      </c>
+      <c r="H4">
+        <v>0.86</v>
+      </c>
+      <c r="I4">
+        <v>10.94</v>
+      </c>
+      <c r="J4">
+        <v>0.86</v>
+      </c>
+      <c r="K4">
+        <v>1.06</v>
+      </c>
+      <c r="L4" t="s">
+        <v>50</v>
+      </c>
+      <c r="M4" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>2019</v>
+      </c>
+      <c r="B5">
+        <v>8</v>
+      </c>
+      <c r="C5">
+        <v>26</v>
+      </c>
+      <c r="D5" t="s">
+        <v>39</v>
+      </c>
+      <c r="E5" t="s">
+        <v>42</v>
+      </c>
+      <c r="F5">
+        <v>19</v>
+      </c>
+      <c r="G5">
+        <v>4</v>
+      </c>
+      <c r="H5">
+        <v>0.86</v>
+      </c>
+      <c r="I5">
+        <v>15.02</v>
+      </c>
+      <c r="J5">
+        <v>0.86</v>
+      </c>
+      <c r="K5">
+        <v>1.86</v>
+      </c>
+      <c r="L5" t="s">
+        <v>50</v>
+      </c>
+      <c r="M5" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>2019</v>
+      </c>
+      <c r="B6">
+        <v>8</v>
+      </c>
+      <c r="C6">
+        <v>26</v>
+      </c>
+      <c r="D6" t="s">
+        <v>39</v>
+      </c>
+      <c r="E6" t="s">
+        <v>42</v>
+      </c>
+      <c r="F6">
+        <v>2</v>
+      </c>
+      <c r="G6">
+        <v>2</v>
+      </c>
+      <c r="H6">
+        <v>0.86</v>
+      </c>
+      <c r="I6">
+        <v>20.04</v>
+      </c>
+      <c r="J6">
+        <v>1.84</v>
+      </c>
+      <c r="K6">
+        <v>1.22</v>
+      </c>
+      <c r="L6" t="s">
+        <v>50</v>
+      </c>
+      <c r="M6" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>2019</v>
+      </c>
+      <c r="B7">
+        <v>8</v>
+      </c>
+      <c r="C7">
+        <v>26</v>
+      </c>
+      <c r="D7" t="s">
+        <v>39</v>
+      </c>
+      <c r="E7" t="s">
+        <v>42</v>
+      </c>
+      <c r="F7">
+        <v>2</v>
+      </c>
+      <c r="G7">
+        <v>4</v>
+      </c>
+      <c r="H7">
+        <v>0.86</v>
+      </c>
+      <c r="I7">
+        <v>17.739999999999998</v>
+      </c>
+      <c r="J7">
+        <v>2.86</v>
+      </c>
+      <c r="K7">
+        <v>1.6</v>
+      </c>
+      <c r="L7" t="s">
+        <v>50</v>
+      </c>
+      <c r="M7" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>2019</v>
+      </c>
+      <c r="B8">
+        <v>8</v>
+      </c>
+      <c r="C8">
+        <v>26</v>
+      </c>
+      <c r="D8" t="s">
+        <v>39</v>
+      </c>
+      <c r="E8" t="s">
+        <v>42</v>
+      </c>
+      <c r="F8">
+        <v>2</v>
+      </c>
+      <c r="G8">
+        <v>3</v>
+      </c>
+      <c r="H8">
+        <v>0.86</v>
+      </c>
+      <c r="I8">
+        <v>16.46</v>
+      </c>
+      <c r="J8">
+        <v>2.2599999999999998</v>
+      </c>
+      <c r="K8">
+        <v>0.96</v>
+      </c>
+      <c r="L8" t="s">
+        <v>50</v>
+      </c>
+      <c r="M8" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>2019</v>
+      </c>
+      <c r="B9">
+        <v>8</v>
+      </c>
+      <c r="C9">
+        <v>26</v>
+      </c>
+      <c r="D9" t="s">
+        <v>39</v>
+      </c>
+      <c r="E9" t="s">
+        <v>42</v>
+      </c>
+      <c r="F9">
+        <v>2</v>
+      </c>
+      <c r="G9">
+        <v>1</v>
+      </c>
+      <c r="H9">
+        <v>0.86</v>
+      </c>
+      <c r="I9">
+        <v>12.02</v>
+      </c>
+      <c r="J9">
+        <v>1.36</v>
+      </c>
+      <c r="K9">
+        <v>0.86</v>
+      </c>
+      <c r="L9" t="s">
+        <v>50</v>
+      </c>
+      <c r="M9" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>2019</v>
+      </c>
+      <c r="B10">
+        <v>8</v>
+      </c>
+      <c r="C10">
+        <v>26</v>
+      </c>
+      <c r="D10" t="s">
+        <v>39</v>
+      </c>
+      <c r="E10" t="s">
+        <v>42</v>
+      </c>
+      <c r="F10">
+        <v>1</v>
+      </c>
+      <c r="G10">
+        <v>4</v>
+      </c>
+      <c r="H10">
+        <v>0.86</v>
+      </c>
+      <c r="I10">
+        <v>21.28</v>
+      </c>
+      <c r="J10">
+        <v>4.53</v>
+      </c>
+      <c r="K10">
+        <v>2.15</v>
+      </c>
+      <c r="L10" t="s">
+        <v>50</v>
+      </c>
+      <c r="M10" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>2019</v>
+      </c>
+      <c r="B11">
+        <v>8</v>
+      </c>
+      <c r="C11">
+        <v>26</v>
+      </c>
+      <c r="D11" t="s">
+        <v>39</v>
+      </c>
+      <c r="E11" t="s">
+        <v>42</v>
+      </c>
+      <c r="F11">
+        <v>1</v>
+      </c>
+      <c r="G11">
+        <v>2</v>
+      </c>
+      <c r="H11">
+        <v>0.86</v>
+      </c>
+      <c r="I11">
+        <v>17.690000000000001</v>
+      </c>
+      <c r="J11">
+        <v>4.99</v>
+      </c>
+      <c r="K11">
+        <v>2.4900000000000002</v>
+      </c>
+      <c r="L11" t="s">
+        <v>50</v>
+      </c>
+      <c r="M11" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>2019</v>
+      </c>
+      <c r="B12">
+        <v>8</v>
+      </c>
+      <c r="C12">
+        <v>26</v>
+      </c>
+      <c r="D12" t="s">
+        <v>39</v>
+      </c>
+      <c r="E12" t="s">
+        <v>42</v>
+      </c>
+      <c r="F12">
+        <v>1</v>
+      </c>
+      <c r="G12">
+        <v>1</v>
+      </c>
+      <c r="H12">
+        <v>0.86</v>
+      </c>
+      <c r="I12">
+        <v>23.13</v>
+      </c>
+      <c r="J12">
+        <v>2.38</v>
+      </c>
+      <c r="K12">
+        <v>7.03</v>
+      </c>
+      <c r="L12" t="s">
+        <v>50</v>
+      </c>
+      <c r="M12" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>2019</v>
+      </c>
+      <c r="B13">
+        <v>8</v>
+      </c>
+      <c r="C13">
+        <v>26</v>
+      </c>
+      <c r="D13" t="s">
+        <v>39</v>
+      </c>
+      <c r="E13" t="s">
+        <v>42</v>
+      </c>
+      <c r="F13">
+        <v>1</v>
+      </c>
+      <c r="G13">
+        <v>3</v>
+      </c>
+      <c r="H13">
+        <v>0.86</v>
+      </c>
+      <c r="I13">
+        <v>-999</v>
+      </c>
+      <c r="J13">
+        <v>0.86</v>
+      </c>
+      <c r="K13">
+        <v>1.25</v>
+      </c>
+      <c r="L13" t="s">
+        <v>50</v>
+      </c>
+      <c r="M13" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>2019</v>
+      </c>
+      <c r="B14">
+        <v>8</v>
+      </c>
+      <c r="C14">
+        <v>26</v>
+      </c>
+      <c r="D14" t="s">
+        <v>39</v>
+      </c>
+      <c r="E14" t="s">
+        <v>42</v>
+      </c>
+      <c r="F14">
+        <v>12</v>
+      </c>
+      <c r="G14">
+        <v>1</v>
+      </c>
+      <c r="H14">
+        <v>0.86</v>
+      </c>
+      <c r="I14">
+        <v>-999</v>
+      </c>
+      <c r="J14">
+        <v>2.4900000000000002</v>
+      </c>
+      <c r="K14">
+        <v>2.15</v>
+      </c>
+      <c r="L14" t="s">
+        <v>50</v>
+      </c>
+      <c r="M14" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>2019</v>
+      </c>
+      <c r="B15">
+        <v>8</v>
+      </c>
+      <c r="C15">
+        <v>26</v>
+      </c>
+      <c r="D15" t="s">
+        <v>39</v>
+      </c>
+      <c r="E15" t="s">
+        <v>42</v>
+      </c>
+      <c r="F15">
+        <v>12</v>
+      </c>
+      <c r="G15">
+        <v>4</v>
+      </c>
+      <c r="H15">
+        <v>0.86</v>
+      </c>
+      <c r="I15">
+        <v>-999</v>
+      </c>
+      <c r="J15">
+        <v>1.59</v>
+      </c>
+      <c r="K15">
+        <v>0.86</v>
+      </c>
+      <c r="L15" t="s">
+        <v>50</v>
+      </c>
+      <c r="M15" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>2019</v>
+      </c>
+      <c r="B16">
+        <v>8</v>
+      </c>
+      <c r="C16">
+        <v>26</v>
+      </c>
+      <c r="D16" t="s">
+        <v>39</v>
+      </c>
+      <c r="E16" t="s">
+        <v>42</v>
+      </c>
+      <c r="F16">
+        <v>12</v>
+      </c>
+      <c r="G16">
+        <v>3</v>
+      </c>
+      <c r="H16">
+        <v>0.86</v>
+      </c>
+      <c r="I16">
+        <v>-999</v>
+      </c>
+      <c r="J16">
+        <v>0.86</v>
+      </c>
+      <c r="K16">
+        <v>0.86</v>
+      </c>
+      <c r="L16" t="s">
+        <v>50</v>
+      </c>
+      <c r="M16" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>2019</v>
+      </c>
+      <c r="B17">
+        <v>8</v>
+      </c>
+      <c r="C17">
+        <v>26</v>
+      </c>
+      <c r="D17" t="s">
+        <v>39</v>
+      </c>
+      <c r="E17" t="s">
+        <v>42</v>
+      </c>
+      <c r="F17">
+        <v>12</v>
+      </c>
+      <c r="G17">
+        <v>2</v>
+      </c>
+      <c r="H17">
+        <v>0.86</v>
+      </c>
+      <c r="I17">
+        <v>-999</v>
+      </c>
+      <c r="J17">
+        <v>4.08</v>
+      </c>
+      <c r="K17">
+        <v>0.86</v>
+      </c>
+      <c r="L17" t="s">
+        <v>50</v>
+      </c>
+      <c r="M17" t="s">
+        <v>50</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="7">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="9">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>pick!$G$2:$G$5</xm:f>
@@ -1766,6 +2569,18 @@
           </x14:formula1>
           <xm:sqref>A1:A1048576</xm:sqref>
         </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>pick!$L$2:$L$16</xm:f>
+          </x14:formula1>
+          <xm:sqref>L1:L1048576</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>pick!$M$2:$M$16</xm:f>
+          </x14:formula1>
+          <xm:sqref>M1:M1048576</xm:sqref>
+        </x14:dataValidation>
       </x14:dataValidations>
     </ext>
   </extLst>
@@ -1774,15 +2589,15 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K100"/>
+  <dimension ref="A1:M100"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>16</v>
       </c>
@@ -1816,744 +2631,878 @@
       <c r="K1" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L1" t="s">
+        <v>44</v>
+      </c>
+      <c r="M1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" t="str">
         <f>IF(raw_data_1!A2=raw_data_2!A2,"","check")</f>
-        <v>check</v>
+        <v/>
       </c>
       <c r="B2" t="str">
         <f>IF(raw_data_1!B2=raw_data_2!B2,"","check")</f>
-        <v>check</v>
+        <v/>
       </c>
       <c r="C2" t="str">
         <f>IF(raw_data_1!C2=raw_data_2!C2,"","check")</f>
-        <v>check</v>
+        <v/>
       </c>
       <c r="D2" t="str">
         <f>IF(raw_data_1!D2=raw_data_2!D2,"","check")</f>
-        <v>check</v>
+        <v/>
       </c>
       <c r="E2" t="str">
         <f>IF(raw_data_1!E2=raw_data_2!E2,"","check")</f>
-        <v>check</v>
+        <v/>
       </c>
       <c r="F2" t="str">
         <f>IF(raw_data_1!F2=raw_data_2!F2,"","check")</f>
-        <v>check</v>
+        <v/>
       </c>
       <c r="G2" t="str">
         <f>IF(raw_data_1!G2=raw_data_2!G2,"","check")</f>
-        <v>check</v>
+        <v/>
       </c>
       <c r="H2" t="str">
         <f>IF(raw_data_1!H2=raw_data_2!H2,"","check")</f>
-        <v>check</v>
+        <v/>
       </c>
       <c r="I2" t="str">
         <f>IF(raw_data_1!I2=raw_data_2!I2,"","check")</f>
-        <v>check</v>
+        <v/>
       </c>
       <c r="J2" t="str">
         <f>IF(raw_data_1!J2=raw_data_2!J2,"","check")</f>
-        <v>check</v>
+        <v/>
       </c>
       <c r="K2" t="str">
         <f>IF(raw_data_1!K2=raw_data_2!K2,"","check")</f>
-        <v>check</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+        <v/>
+      </c>
+      <c r="L2" t="str">
+        <f>IF(raw_data_1!L2=raw_data_2!L2,"","check")</f>
+        <v/>
+      </c>
+      <c r="M2" t="str">
+        <f>IF(raw_data_1!M2=raw_data_2!M2,"","check")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" t="str">
         <f>IF(raw_data_1!A3=raw_data_2!A3,"","check")</f>
-        <v>check</v>
+        <v/>
       </c>
       <c r="B3" t="str">
         <f>IF(raw_data_1!B3=raw_data_2!B3,"","check")</f>
-        <v>check</v>
+        <v/>
       </c>
       <c r="C3" t="str">
         <f>IF(raw_data_1!C3=raw_data_2!C3,"","check")</f>
-        <v>check</v>
+        <v/>
       </c>
       <c r="D3" t="str">
         <f>IF(raw_data_1!D3=raw_data_2!D3,"","check")</f>
-        <v>check</v>
+        <v/>
       </c>
       <c r="E3" t="str">
         <f>IF(raw_data_1!E3=raw_data_2!E3,"","check")</f>
-        <v>check</v>
+        <v/>
       </c>
       <c r="F3" t="str">
         <f>IF(raw_data_1!F3=raw_data_2!F3,"","check")</f>
-        <v>check</v>
+        <v/>
       </c>
       <c r="G3" t="str">
         <f>IF(raw_data_1!G3=raw_data_2!G3,"","check")</f>
-        <v>check</v>
+        <v/>
       </c>
       <c r="H3" t="str">
         <f>IF(raw_data_1!H3=raw_data_2!H3,"","check")</f>
-        <v>check</v>
+        <v/>
       </c>
       <c r="I3" t="str">
         <f>IF(raw_data_1!I3=raw_data_2!I3,"","check")</f>
-        <v>check</v>
+        <v/>
       </c>
       <c r="J3" t="str">
         <f>IF(raw_data_1!J3=raw_data_2!J3,"","check")</f>
-        <v>check</v>
+        <v/>
       </c>
       <c r="K3" t="str">
         <f>IF(raw_data_1!K3=raw_data_2!K3,"","check")</f>
-        <v>check</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+        <v/>
+      </c>
+      <c r="L3" t="str">
+        <f>IF(raw_data_1!L3=raw_data_2!L3,"","check")</f>
+        <v/>
+      </c>
+      <c r="M3" t="str">
+        <f>IF(raw_data_1!M3=raw_data_2!M3,"","check")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" t="str">
         <f>IF(raw_data_1!A4=raw_data_2!A4,"","check")</f>
-        <v>check</v>
+        <v/>
       </c>
       <c r="B4" t="str">
         <f>IF(raw_data_1!B4=raw_data_2!B4,"","check")</f>
-        <v>check</v>
+        <v/>
       </c>
       <c r="C4" t="str">
         <f>IF(raw_data_1!C4=raw_data_2!C4,"","check")</f>
-        <v>check</v>
+        <v/>
       </c>
       <c r="D4" t="str">
         <f>IF(raw_data_1!D4=raw_data_2!D4,"","check")</f>
-        <v>check</v>
+        <v/>
       </c>
       <c r="E4" t="str">
         <f>IF(raw_data_1!E4=raw_data_2!E4,"","check")</f>
-        <v>check</v>
+        <v/>
       </c>
       <c r="F4" t="str">
         <f>IF(raw_data_1!F4=raw_data_2!F4,"","check")</f>
-        <v>check</v>
+        <v/>
       </c>
       <c r="G4" t="str">
         <f>IF(raw_data_1!G4=raw_data_2!G4,"","check")</f>
-        <v>check</v>
+        <v/>
       </c>
       <c r="H4" t="str">
         <f>IF(raw_data_1!H4=raw_data_2!H4,"","check")</f>
-        <v>check</v>
+        <v/>
       </c>
       <c r="I4" t="str">
         <f>IF(raw_data_1!I4=raw_data_2!I4,"","check")</f>
-        <v>check</v>
+        <v/>
       </c>
       <c r="J4" t="str">
         <f>IF(raw_data_1!J4=raw_data_2!J4,"","check")</f>
-        <v>check</v>
+        <v/>
       </c>
       <c r="K4" t="str">
         <f>IF(raw_data_1!K4=raw_data_2!K4,"","check")</f>
-        <v>check</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+        <v/>
+      </c>
+      <c r="L4" t="str">
+        <f>IF(raw_data_1!L4=raw_data_2!L4,"","check")</f>
+        <v/>
+      </c>
+      <c r="M4" t="str">
+        <f>IF(raw_data_1!M4=raw_data_2!M4,"","check")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" t="str">
         <f>IF(raw_data_1!A5=raw_data_2!A5,"","check")</f>
-        <v>check</v>
+        <v/>
       </c>
       <c r="B5" t="str">
         <f>IF(raw_data_1!B5=raw_data_2!B5,"","check")</f>
-        <v>check</v>
+        <v/>
       </c>
       <c r="C5" t="str">
         <f>IF(raw_data_1!C5=raw_data_2!C5,"","check")</f>
-        <v>check</v>
+        <v/>
       </c>
       <c r="D5" t="str">
         <f>IF(raw_data_1!D5=raw_data_2!D5,"","check")</f>
-        <v>check</v>
+        <v/>
       </c>
       <c r="E5" t="str">
         <f>IF(raw_data_1!E5=raw_data_2!E5,"","check")</f>
-        <v>check</v>
+        <v/>
       </c>
       <c r="F5" t="str">
         <f>IF(raw_data_1!F5=raw_data_2!F5,"","check")</f>
-        <v>check</v>
+        <v/>
       </c>
       <c r="G5" t="str">
         <f>IF(raw_data_1!G5=raw_data_2!G5,"","check")</f>
-        <v>check</v>
+        <v/>
       </c>
       <c r="H5" t="str">
         <f>IF(raw_data_1!H5=raw_data_2!H5,"","check")</f>
-        <v>check</v>
+        <v/>
       </c>
       <c r="I5" t="str">
         <f>IF(raw_data_1!I5=raw_data_2!I5,"","check")</f>
-        <v>check</v>
+        <v/>
       </c>
       <c r="J5" t="str">
         <f>IF(raw_data_1!J5=raw_data_2!J5,"","check")</f>
-        <v>check</v>
+        <v/>
       </c>
       <c r="K5" t="str">
         <f>IF(raw_data_1!K5=raw_data_2!K5,"","check")</f>
-        <v>check</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+        <v/>
+      </c>
+      <c r="L5" t="str">
+        <f>IF(raw_data_1!L5=raw_data_2!L5,"","check")</f>
+        <v/>
+      </c>
+      <c r="M5" t="str">
+        <f>IF(raw_data_1!M5=raw_data_2!M5,"","check")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" t="str">
         <f>IF(raw_data_1!A6=raw_data_2!A6,"","check")</f>
-        <v>check</v>
+        <v/>
       </c>
       <c r="B6" t="str">
         <f>IF(raw_data_1!B6=raw_data_2!B6,"","check")</f>
-        <v>check</v>
+        <v/>
       </c>
       <c r="C6" t="str">
         <f>IF(raw_data_1!C6=raw_data_2!C6,"","check")</f>
-        <v>check</v>
+        <v/>
       </c>
       <c r="D6" t="str">
         <f>IF(raw_data_1!D6=raw_data_2!D6,"","check")</f>
-        <v>check</v>
+        <v/>
       </c>
       <c r="E6" t="str">
         <f>IF(raw_data_1!E6=raw_data_2!E6,"","check")</f>
-        <v>check</v>
+        <v/>
       </c>
       <c r="F6" t="str">
         <f>IF(raw_data_1!F6=raw_data_2!F6,"","check")</f>
-        <v>check</v>
+        <v/>
       </c>
       <c r="G6" t="str">
         <f>IF(raw_data_1!G6=raw_data_2!G6,"","check")</f>
-        <v>check</v>
+        <v/>
       </c>
       <c r="H6" t="str">
         <f>IF(raw_data_1!H6=raw_data_2!H6,"","check")</f>
-        <v>check</v>
+        <v/>
       </c>
       <c r="I6" t="str">
         <f>IF(raw_data_1!I6=raw_data_2!I6,"","check")</f>
-        <v>check</v>
+        <v/>
       </c>
       <c r="J6" t="str">
         <f>IF(raw_data_1!J6=raw_data_2!J6,"","check")</f>
-        <v>check</v>
+        <v/>
       </c>
       <c r="K6" t="str">
         <f>IF(raw_data_1!K6=raw_data_2!K6,"","check")</f>
-        <v>check</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+        <v/>
+      </c>
+      <c r="L6" t="str">
+        <f>IF(raw_data_1!L6=raw_data_2!L6,"","check")</f>
+        <v/>
+      </c>
+      <c r="M6" t="str">
+        <f>IF(raw_data_1!M6=raw_data_2!M6,"","check")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" t="str">
         <f>IF(raw_data_1!A7=raw_data_2!A7,"","check")</f>
-        <v>check</v>
+        <v/>
       </c>
       <c r="B7" t="str">
         <f>IF(raw_data_1!B7=raw_data_2!B7,"","check")</f>
-        <v>check</v>
+        <v/>
       </c>
       <c r="C7" t="str">
         <f>IF(raw_data_1!C7=raw_data_2!C7,"","check")</f>
-        <v>check</v>
+        <v/>
       </c>
       <c r="D7" t="str">
         <f>IF(raw_data_1!D7=raw_data_2!D7,"","check")</f>
-        <v>check</v>
+        <v/>
       </c>
       <c r="E7" t="str">
         <f>IF(raw_data_1!E7=raw_data_2!E7,"","check")</f>
-        <v>check</v>
+        <v/>
       </c>
       <c r="F7" t="str">
         <f>IF(raw_data_1!F7=raw_data_2!F7,"","check")</f>
-        <v>check</v>
+        <v/>
       </c>
       <c r="G7" t="str">
         <f>IF(raw_data_1!G7=raw_data_2!G7,"","check")</f>
-        <v>check</v>
+        <v/>
       </c>
       <c r="H7" t="str">
         <f>IF(raw_data_1!H7=raw_data_2!H7,"","check")</f>
-        <v>check</v>
+        <v/>
       </c>
       <c r="I7" t="str">
         <f>IF(raw_data_1!I7=raw_data_2!I7,"","check")</f>
-        <v>check</v>
+        <v/>
       </c>
       <c r="J7" t="str">
         <f>IF(raw_data_1!J7=raw_data_2!J7,"","check")</f>
-        <v>check</v>
+        <v/>
       </c>
       <c r="K7" t="str">
         <f>IF(raw_data_1!K7=raw_data_2!K7,"","check")</f>
-        <v>check</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+        <v/>
+      </c>
+      <c r="L7" t="str">
+        <f>IF(raw_data_1!L7=raw_data_2!L7,"","check")</f>
+        <v/>
+      </c>
+      <c r="M7" t="str">
+        <f>IF(raw_data_1!M7=raw_data_2!M7,"","check")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" t="str">
         <f>IF(raw_data_1!A8=raw_data_2!A8,"","check")</f>
-        <v>check</v>
+        <v/>
       </c>
       <c r="B8" t="str">
         <f>IF(raw_data_1!B8=raw_data_2!B8,"","check")</f>
-        <v>check</v>
+        <v/>
       </c>
       <c r="C8" t="str">
         <f>IF(raw_data_1!C8=raw_data_2!C8,"","check")</f>
-        <v>check</v>
+        <v/>
       </c>
       <c r="D8" t="str">
         <f>IF(raw_data_1!D8=raw_data_2!D8,"","check")</f>
-        <v>check</v>
+        <v/>
       </c>
       <c r="E8" t="str">
         <f>IF(raw_data_1!E8=raw_data_2!E8,"","check")</f>
-        <v>check</v>
+        <v/>
       </c>
       <c r="F8" t="str">
         <f>IF(raw_data_1!F8=raw_data_2!F8,"","check")</f>
-        <v>check</v>
+        <v/>
       </c>
       <c r="G8" t="str">
         <f>IF(raw_data_1!G8=raw_data_2!G8,"","check")</f>
-        <v>check</v>
+        <v/>
       </c>
       <c r="H8" t="str">
         <f>IF(raw_data_1!H8=raw_data_2!H8,"","check")</f>
-        <v>check</v>
+        <v/>
       </c>
       <c r="I8" t="str">
         <f>IF(raw_data_1!I8=raw_data_2!I8,"","check")</f>
-        <v>check</v>
+        <v/>
       </c>
       <c r="J8" t="str">
         <f>IF(raw_data_1!J8=raw_data_2!J8,"","check")</f>
-        <v>check</v>
+        <v/>
       </c>
       <c r="K8" t="str">
         <f>IF(raw_data_1!K8=raw_data_2!K8,"","check")</f>
-        <v>check</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+        <v/>
+      </c>
+      <c r="L8" t="str">
+        <f>IF(raw_data_1!L8=raw_data_2!L8,"","check")</f>
+        <v/>
+      </c>
+      <c r="M8" t="str">
+        <f>IF(raw_data_1!M8=raw_data_2!M8,"","check")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" t="str">
         <f>IF(raw_data_1!A9=raw_data_2!A9,"","check")</f>
-        <v>check</v>
+        <v/>
       </c>
       <c r="B9" t="str">
         <f>IF(raw_data_1!B9=raw_data_2!B9,"","check")</f>
-        <v>check</v>
+        <v/>
       </c>
       <c r="C9" t="str">
         <f>IF(raw_data_1!C9=raw_data_2!C9,"","check")</f>
-        <v>check</v>
+        <v/>
       </c>
       <c r="D9" t="str">
         <f>IF(raw_data_1!D9=raw_data_2!D9,"","check")</f>
-        <v>check</v>
+        <v/>
       </c>
       <c r="E9" t="str">
         <f>IF(raw_data_1!E9=raw_data_2!E9,"","check")</f>
-        <v>check</v>
+        <v/>
       </c>
       <c r="F9" t="str">
         <f>IF(raw_data_1!F9=raw_data_2!F9,"","check")</f>
-        <v>check</v>
+        <v/>
       </c>
       <c r="G9" t="str">
         <f>IF(raw_data_1!G9=raw_data_2!G9,"","check")</f>
-        <v>check</v>
+        <v/>
       </c>
       <c r="H9" t="str">
         <f>IF(raw_data_1!H9=raw_data_2!H9,"","check")</f>
-        <v>check</v>
+        <v/>
       </c>
       <c r="I9" t="str">
         <f>IF(raw_data_1!I9=raw_data_2!I9,"","check")</f>
-        <v>check</v>
+        <v/>
       </c>
       <c r="J9" t="str">
         <f>IF(raw_data_1!J9=raw_data_2!J9,"","check")</f>
-        <v>check</v>
+        <v/>
       </c>
       <c r="K9" t="str">
         <f>IF(raw_data_1!K9=raw_data_2!K9,"","check")</f>
-        <v>check</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+        <v/>
+      </c>
+      <c r="L9" t="str">
+        <f>IF(raw_data_1!L9=raw_data_2!L9,"","check")</f>
+        <v/>
+      </c>
+      <c r="M9" t="str">
+        <f>IF(raw_data_1!M9=raw_data_2!M9,"","check")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" t="str">
         <f>IF(raw_data_1!A10=raw_data_2!A10,"","check")</f>
-        <v>check</v>
+        <v/>
       </c>
       <c r="B10" t="str">
         <f>IF(raw_data_1!B10=raw_data_2!B10,"","check")</f>
-        <v>check</v>
+        <v/>
       </c>
       <c r="C10" t="str">
         <f>IF(raw_data_1!C10=raw_data_2!C10,"","check")</f>
-        <v>check</v>
+        <v/>
       </c>
       <c r="D10" t="str">
         <f>IF(raw_data_1!D10=raw_data_2!D10,"","check")</f>
-        <v>check</v>
+        <v/>
       </c>
       <c r="E10" t="str">
         <f>IF(raw_data_1!E10=raw_data_2!E10,"","check")</f>
-        <v>check</v>
+        <v/>
       </c>
       <c r="F10" t="str">
         <f>IF(raw_data_1!F10=raw_data_2!F10,"","check")</f>
-        <v>check</v>
+        <v/>
       </c>
       <c r="G10" t="str">
         <f>IF(raw_data_1!G10=raw_data_2!G10,"","check")</f>
-        <v>check</v>
+        <v/>
       </c>
       <c r="H10" t="str">
         <f>IF(raw_data_1!H10=raw_data_2!H10,"","check")</f>
-        <v>check</v>
+        <v/>
       </c>
       <c r="I10" t="str">
         <f>IF(raw_data_1!I10=raw_data_2!I10,"","check")</f>
-        <v>check</v>
+        <v/>
       </c>
       <c r="J10" t="str">
         <f>IF(raw_data_1!J10=raw_data_2!J10,"","check")</f>
-        <v>check</v>
+        <v/>
       </c>
       <c r="K10" t="str">
         <f>IF(raw_data_1!K10=raw_data_2!K10,"","check")</f>
-        <v>check</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+        <v/>
+      </c>
+      <c r="L10" t="str">
+        <f>IF(raw_data_1!L10=raw_data_2!L10,"","check")</f>
+        <v/>
+      </c>
+      <c r="M10" t="str">
+        <f>IF(raw_data_1!M10=raw_data_2!M10,"","check")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" t="str">
         <f>IF(raw_data_1!A11=raw_data_2!A11,"","check")</f>
-        <v>check</v>
+        <v/>
       </c>
       <c r="B11" t="str">
         <f>IF(raw_data_1!B11=raw_data_2!B11,"","check")</f>
-        <v>check</v>
+        <v/>
       </c>
       <c r="C11" t="str">
         <f>IF(raw_data_1!C11=raw_data_2!C11,"","check")</f>
-        <v>check</v>
+        <v/>
       </c>
       <c r="D11" t="str">
         <f>IF(raw_data_1!D11=raw_data_2!D11,"","check")</f>
-        <v>check</v>
+        <v/>
       </c>
       <c r="E11" t="str">
         <f>IF(raw_data_1!E11=raw_data_2!E11,"","check")</f>
-        <v>check</v>
+        <v/>
       </c>
       <c r="F11" t="str">
         <f>IF(raw_data_1!F11=raw_data_2!F11,"","check")</f>
-        <v>check</v>
+        <v/>
       </c>
       <c r="G11" t="str">
         <f>IF(raw_data_1!G11=raw_data_2!G11,"","check")</f>
-        <v>check</v>
+        <v/>
       </c>
       <c r="H11" t="str">
         <f>IF(raw_data_1!H11=raw_data_2!H11,"","check")</f>
-        <v>check</v>
+        <v/>
       </c>
       <c r="I11" t="str">
         <f>IF(raw_data_1!I11=raw_data_2!I11,"","check")</f>
-        <v>check</v>
+        <v/>
       </c>
       <c r="J11" t="str">
         <f>IF(raw_data_1!J11=raw_data_2!J11,"","check")</f>
-        <v>check</v>
+        <v/>
       </c>
       <c r="K11" t="str">
         <f>IF(raw_data_1!K11=raw_data_2!K11,"","check")</f>
-        <v>check</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+        <v/>
+      </c>
+      <c r="L11" t="str">
+        <f>IF(raw_data_1!L11=raw_data_2!L11,"","check")</f>
+        <v/>
+      </c>
+      <c r="M11" t="str">
+        <f>IF(raw_data_1!M11=raw_data_2!M11,"","check")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" t="str">
         <f>IF(raw_data_1!A12=raw_data_2!A12,"","check")</f>
-        <v>check</v>
+        <v/>
       </c>
       <c r="B12" t="str">
         <f>IF(raw_data_1!B12=raw_data_2!B12,"","check")</f>
-        <v>check</v>
+        <v/>
       </c>
       <c r="C12" t="str">
         <f>IF(raw_data_1!C12=raw_data_2!C12,"","check")</f>
-        <v>check</v>
+        <v/>
       </c>
       <c r="D12" t="str">
         <f>IF(raw_data_1!D12=raw_data_2!D12,"","check")</f>
-        <v>check</v>
+        <v/>
       </c>
       <c r="E12" t="str">
         <f>IF(raw_data_1!E12=raw_data_2!E12,"","check")</f>
-        <v>check</v>
+        <v/>
       </c>
       <c r="F12" t="str">
         <f>IF(raw_data_1!F12=raw_data_2!F12,"","check")</f>
-        <v>check</v>
+        <v/>
       </c>
       <c r="G12" t="str">
         <f>IF(raw_data_1!G12=raw_data_2!G12,"","check")</f>
-        <v>check</v>
+        <v/>
       </c>
       <c r="H12" t="str">
         <f>IF(raw_data_1!H12=raw_data_2!H12,"","check")</f>
-        <v>check</v>
+        <v/>
       </c>
       <c r="I12" t="str">
         <f>IF(raw_data_1!I12=raw_data_2!I12,"","check")</f>
-        <v>check</v>
+        <v/>
       </c>
       <c r="J12" t="str">
         <f>IF(raw_data_1!J12=raw_data_2!J12,"","check")</f>
-        <v>check</v>
+        <v/>
       </c>
       <c r="K12" t="str">
         <f>IF(raw_data_1!K12=raw_data_2!K12,"","check")</f>
-        <v>check</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+        <v/>
+      </c>
+      <c r="L12" t="str">
+        <f>IF(raw_data_1!L12=raw_data_2!L12,"","check")</f>
+        <v/>
+      </c>
+      <c r="M12" t="str">
+        <f>IF(raw_data_1!M12=raw_data_2!M12,"","check")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" t="str">
         <f>IF(raw_data_1!A13=raw_data_2!A13,"","check")</f>
-        <v>check</v>
+        <v/>
       </c>
       <c r="B13" t="str">
         <f>IF(raw_data_1!B13=raw_data_2!B13,"","check")</f>
-        <v>check</v>
+        <v/>
       </c>
       <c r="C13" t="str">
         <f>IF(raw_data_1!C13=raw_data_2!C13,"","check")</f>
-        <v>check</v>
+        <v/>
       </c>
       <c r="D13" t="str">
         <f>IF(raw_data_1!D13=raw_data_2!D13,"","check")</f>
-        <v>check</v>
+        <v/>
       </c>
       <c r="E13" t="str">
         <f>IF(raw_data_1!E13=raw_data_2!E13,"","check")</f>
-        <v>check</v>
+        <v/>
       </c>
       <c r="F13" t="str">
         <f>IF(raw_data_1!F13=raw_data_2!F13,"","check")</f>
-        <v>check</v>
+        <v/>
       </c>
       <c r="G13" t="str">
         <f>IF(raw_data_1!G13=raw_data_2!G13,"","check")</f>
-        <v>check</v>
+        <v/>
       </c>
       <c r="H13" t="str">
         <f>IF(raw_data_1!H13=raw_data_2!H13,"","check")</f>
-        <v>check</v>
+        <v/>
       </c>
       <c r="I13" t="str">
         <f>IF(raw_data_1!I13=raw_data_2!I13,"","check")</f>
-        <v>check</v>
+        <v/>
       </c>
       <c r="J13" t="str">
         <f>IF(raw_data_1!J13=raw_data_2!J13,"","check")</f>
-        <v>check</v>
+        <v/>
       </c>
       <c r="K13" t="str">
         <f>IF(raw_data_1!K13=raw_data_2!K13,"","check")</f>
-        <v>check</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+        <v/>
+      </c>
+      <c r="L13" t="str">
+        <f>IF(raw_data_1!L13=raw_data_2!L13,"","check")</f>
+        <v/>
+      </c>
+      <c r="M13" t="str">
+        <f>IF(raw_data_1!M13=raw_data_2!M13,"","check")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" t="str">
         <f>IF(raw_data_1!A14=raw_data_2!A14,"","check")</f>
-        <v>check</v>
+        <v/>
       </c>
       <c r="B14" t="str">
         <f>IF(raw_data_1!B14=raw_data_2!B14,"","check")</f>
-        <v>check</v>
+        <v/>
       </c>
       <c r="C14" t="str">
         <f>IF(raw_data_1!C14=raw_data_2!C14,"","check")</f>
-        <v>check</v>
+        <v/>
       </c>
       <c r="D14" t="str">
         <f>IF(raw_data_1!D14=raw_data_2!D14,"","check")</f>
-        <v>check</v>
+        <v/>
       </c>
       <c r="E14" t="str">
         <f>IF(raw_data_1!E14=raw_data_2!E14,"","check")</f>
-        <v>check</v>
+        <v/>
       </c>
       <c r="F14" t="str">
         <f>IF(raw_data_1!F14=raw_data_2!F14,"","check")</f>
-        <v>check</v>
+        <v/>
       </c>
       <c r="G14" t="str">
         <f>IF(raw_data_1!G14=raw_data_2!G14,"","check")</f>
-        <v>check</v>
+        <v/>
       </c>
       <c r="H14" t="str">
         <f>IF(raw_data_1!H14=raw_data_2!H14,"","check")</f>
-        <v>check</v>
+        <v/>
       </c>
       <c r="I14" t="str">
         <f>IF(raw_data_1!I14=raw_data_2!I14,"","check")</f>
-        <v>check</v>
+        <v/>
       </c>
       <c r="J14" t="str">
         <f>IF(raw_data_1!J14=raw_data_2!J14,"","check")</f>
-        <v>check</v>
+        <v/>
       </c>
       <c r="K14" t="str">
         <f>IF(raw_data_1!K14=raw_data_2!K14,"","check")</f>
-        <v>check</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+        <v/>
+      </c>
+      <c r="L14" t="str">
+        <f>IF(raw_data_1!L14=raw_data_2!L14,"","check")</f>
+        <v/>
+      </c>
+      <c r="M14" t="str">
+        <f>IF(raw_data_1!M14=raw_data_2!M14,"","check")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" t="str">
         <f>IF(raw_data_1!A15=raw_data_2!A15,"","check")</f>
-        <v>check</v>
+        <v/>
       </c>
       <c r="B15" t="str">
         <f>IF(raw_data_1!B15=raw_data_2!B15,"","check")</f>
-        <v>check</v>
+        <v/>
       </c>
       <c r="C15" t="str">
         <f>IF(raw_data_1!C15=raw_data_2!C15,"","check")</f>
-        <v>check</v>
+        <v/>
       </c>
       <c r="D15" t="str">
         <f>IF(raw_data_1!D15=raw_data_2!D15,"","check")</f>
-        <v>check</v>
+        <v/>
       </c>
       <c r="E15" t="str">
         <f>IF(raw_data_1!E15=raw_data_2!E15,"","check")</f>
-        <v>check</v>
+        <v/>
       </c>
       <c r="F15" t="str">
         <f>IF(raw_data_1!F15=raw_data_2!F15,"","check")</f>
-        <v>check</v>
+        <v/>
       </c>
       <c r="G15" t="str">
         <f>IF(raw_data_1!G15=raw_data_2!G15,"","check")</f>
-        <v>check</v>
+        <v/>
       </c>
       <c r="H15" t="str">
         <f>IF(raw_data_1!H15=raw_data_2!H15,"","check")</f>
-        <v>check</v>
+        <v/>
       </c>
       <c r="I15" t="str">
         <f>IF(raw_data_1!I15=raw_data_2!I15,"","check")</f>
-        <v>check</v>
+        <v/>
       </c>
       <c r="J15" t="str">
         <f>IF(raw_data_1!J15=raw_data_2!J15,"","check")</f>
-        <v>check</v>
+        <v/>
       </c>
       <c r="K15" t="str">
         <f>IF(raw_data_1!K15=raw_data_2!K15,"","check")</f>
-        <v>check</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+        <v/>
+      </c>
+      <c r="L15" t="str">
+        <f>IF(raw_data_1!L15=raw_data_2!L15,"","check")</f>
+        <v/>
+      </c>
+      <c r="M15" t="str">
+        <f>IF(raw_data_1!M15=raw_data_2!M15,"","check")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" t="str">
         <f>IF(raw_data_1!A16=raw_data_2!A16,"","check")</f>
-        <v>check</v>
+        <v/>
       </c>
       <c r="B16" t="str">
         <f>IF(raw_data_1!B16=raw_data_2!B16,"","check")</f>
-        <v>check</v>
+        <v/>
       </c>
       <c r="C16" t="str">
         <f>IF(raw_data_1!C16=raw_data_2!C16,"","check")</f>
-        <v>check</v>
+        <v/>
       </c>
       <c r="D16" t="str">
         <f>IF(raw_data_1!D16=raw_data_2!D16,"","check")</f>
-        <v>check</v>
+        <v/>
       </c>
       <c r="E16" t="str">
         <f>IF(raw_data_1!E16=raw_data_2!E16,"","check")</f>
-        <v>check</v>
+        <v/>
       </c>
       <c r="F16" t="str">
         <f>IF(raw_data_1!F16=raw_data_2!F16,"","check")</f>
-        <v>check</v>
+        <v/>
       </c>
       <c r="G16" t="str">
         <f>IF(raw_data_1!G16=raw_data_2!G16,"","check")</f>
-        <v>check</v>
+        <v/>
       </c>
       <c r="H16" t="str">
         <f>IF(raw_data_1!H16=raw_data_2!H16,"","check")</f>
-        <v>check</v>
+        <v/>
       </c>
       <c r="I16" t="str">
         <f>IF(raw_data_1!I16=raw_data_2!I16,"","check")</f>
-        <v>check</v>
+        <v/>
       </c>
       <c r="J16" t="str">
         <f>IF(raw_data_1!J16=raw_data_2!J16,"","check")</f>
-        <v>check</v>
+        <v/>
       </c>
       <c r="K16" t="str">
         <f>IF(raw_data_1!K16=raw_data_2!K16,"","check")</f>
-        <v>check</v>
-      </c>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+        <v/>
+      </c>
+      <c r="L16" t="str">
+        <f>IF(raw_data_1!L16=raw_data_2!L16,"","check")</f>
+        <v/>
+      </c>
+      <c r="M16" t="str">
+        <f>IF(raw_data_1!M16=raw_data_2!M16,"","check")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" t="str">
         <f>IF(raw_data_1!A17=raw_data_2!A17,"","check")</f>
-        <v>check</v>
+        <v/>
       </c>
       <c r="B17" t="str">
         <f>IF(raw_data_1!B17=raw_data_2!B17,"","check")</f>
-        <v>check</v>
+        <v/>
       </c>
       <c r="C17" t="str">
         <f>IF(raw_data_1!C17=raw_data_2!C17,"","check")</f>
-        <v>check</v>
+        <v/>
       </c>
       <c r="D17" t="str">
         <f>IF(raw_data_1!D17=raw_data_2!D17,"","check")</f>
-        <v>check</v>
+        <v/>
       </c>
       <c r="E17" t="str">
         <f>IF(raw_data_1!E17=raw_data_2!E17,"","check")</f>
-        <v>check</v>
+        <v/>
       </c>
       <c r="F17" t="str">
         <f>IF(raw_data_1!F17=raw_data_2!F17,"","check")</f>
-        <v>check</v>
+        <v/>
       </c>
       <c r="G17" t="str">
         <f>IF(raw_data_1!G17=raw_data_2!G17,"","check")</f>
-        <v>check</v>
+        <v/>
       </c>
       <c r="H17" t="str">
         <f>IF(raw_data_1!H17=raw_data_2!H17,"","check")</f>
-        <v>check</v>
+        <v/>
       </c>
       <c r="I17" t="str">
         <f>IF(raw_data_1!I17=raw_data_2!I17,"","check")</f>
-        <v>check</v>
+        <v/>
       </c>
       <c r="J17" t="str">
         <f>IF(raw_data_1!J17=raw_data_2!J17,"","check")</f>
-        <v>check</v>
+        <v/>
       </c>
       <c r="K17" t="str">
         <f>IF(raw_data_1!K17=raw_data_2!K17,"","check")</f>
-        <v>check</v>
-      </c>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+        <v/>
+      </c>
+      <c r="L17" t="str">
+        <f>IF(raw_data_1!L17=raw_data_2!L17,"","check")</f>
+        <v/>
+      </c>
+      <c r="M17" t="str">
+        <f>IF(raw_data_1!M17=raw_data_2!M17,"","check")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18" t="str">
         <f>IF(raw_data_1!A18=raw_data_2!A18,"","check")</f>
         <v/>
@@ -2598,8 +3547,16 @@
         <f>IF(raw_data_1!K18=raw_data_2!K18,"","check")</f>
         <v/>
       </c>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L18" t="str">
+        <f>IF(raw_data_1!L18=raw_data_2!L18,"","check")</f>
+        <v/>
+      </c>
+      <c r="M18" t="str">
+        <f>IF(raw_data_1!M18=raw_data_2!M18,"","check")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19" t="str">
         <f>IF(raw_data_1!A19=raw_data_2!A19,"","check")</f>
         <v/>
@@ -2644,8 +3601,16 @@
         <f>IF(raw_data_1!K19=raw_data_2!K19,"","check")</f>
         <v/>
       </c>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L19" t="str">
+        <f>IF(raw_data_1!L19=raw_data_2!L19,"","check")</f>
+        <v/>
+      </c>
+      <c r="M19" t="str">
+        <f>IF(raw_data_1!M19=raw_data_2!M19,"","check")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" t="str">
         <f>IF(raw_data_1!A20=raw_data_2!A20,"","check")</f>
         <v/>
@@ -2690,8 +3655,16 @@
         <f>IF(raw_data_1!K20=raw_data_2!K20,"","check")</f>
         <v/>
       </c>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L20" t="str">
+        <f>IF(raw_data_1!L20=raw_data_2!L20,"","check")</f>
+        <v/>
+      </c>
+      <c r="M20" t="str">
+        <f>IF(raw_data_1!M20=raw_data_2!M20,"","check")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21" t="str">
         <f>IF(raw_data_1!A21=raw_data_2!A21,"","check")</f>
         <v/>
@@ -2736,8 +3709,16 @@
         <f>IF(raw_data_1!K21=raw_data_2!K21,"","check")</f>
         <v/>
       </c>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L21" t="str">
+        <f>IF(raw_data_1!L21=raw_data_2!L21,"","check")</f>
+        <v/>
+      </c>
+      <c r="M21" t="str">
+        <f>IF(raw_data_1!M21=raw_data_2!M21,"","check")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22" t="str">
         <f>IF(raw_data_1!A22=raw_data_2!A22,"","check")</f>
         <v/>
@@ -2782,8 +3763,16 @@
         <f>IF(raw_data_1!K22=raw_data_2!K22,"","check")</f>
         <v/>
       </c>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L22" t="str">
+        <f>IF(raw_data_1!L22=raw_data_2!L22,"","check")</f>
+        <v/>
+      </c>
+      <c r="M22" t="str">
+        <f>IF(raw_data_1!M22=raw_data_2!M22,"","check")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A23" t="str">
         <f>IF(raw_data_1!A23=raw_data_2!A23,"","check")</f>
         <v/>
@@ -2828,8 +3817,16 @@
         <f>IF(raw_data_1!K23=raw_data_2!K23,"","check")</f>
         <v/>
       </c>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L23" t="str">
+        <f>IF(raw_data_1!L23=raw_data_2!L23,"","check")</f>
+        <v/>
+      </c>
+      <c r="M23" t="str">
+        <f>IF(raw_data_1!M23=raw_data_2!M23,"","check")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A24" t="str">
         <f>IF(raw_data_1!A24=raw_data_2!A24,"","check")</f>
         <v/>
@@ -2874,8 +3871,16 @@
         <f>IF(raw_data_1!K24=raw_data_2!K24,"","check")</f>
         <v/>
       </c>
-    </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L24" t="str">
+        <f>IF(raw_data_1!L24=raw_data_2!L24,"","check")</f>
+        <v/>
+      </c>
+      <c r="M24" t="str">
+        <f>IF(raw_data_1!M24=raw_data_2!M24,"","check")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A25" t="str">
         <f>IF(raw_data_1!A25=raw_data_2!A25,"","check")</f>
         <v/>
@@ -2920,8 +3925,16 @@
         <f>IF(raw_data_1!K25=raw_data_2!K25,"","check")</f>
         <v/>
       </c>
-    </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L25" t="str">
+        <f>IF(raw_data_1!L25=raw_data_2!L25,"","check")</f>
+        <v/>
+      </c>
+      <c r="M25" t="str">
+        <f>IF(raw_data_1!M25=raw_data_2!M25,"","check")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A26" t="str">
         <f>IF(raw_data_1!A26=raw_data_2!A26,"","check")</f>
         <v/>
@@ -2966,8 +3979,16 @@
         <f>IF(raw_data_1!K26=raw_data_2!K26,"","check")</f>
         <v/>
       </c>
-    </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L26" t="str">
+        <f>IF(raw_data_1!L26=raw_data_2!L26,"","check")</f>
+        <v/>
+      </c>
+      <c r="M26" t="str">
+        <f>IF(raw_data_1!M26=raw_data_2!M26,"","check")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A27" t="str">
         <f>IF(raw_data_1!A27=raw_data_2!A27,"","check")</f>
         <v/>
@@ -3012,8 +4033,16 @@
         <f>IF(raw_data_1!K27=raw_data_2!K27,"","check")</f>
         <v/>
       </c>
-    </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L27" t="str">
+        <f>IF(raw_data_1!L27=raw_data_2!L27,"","check")</f>
+        <v/>
+      </c>
+      <c r="M27" t="str">
+        <f>IF(raw_data_1!M27=raw_data_2!M27,"","check")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A28" t="str">
         <f>IF(raw_data_1!A28=raw_data_2!A28,"","check")</f>
         <v/>
@@ -3058,8 +4087,16 @@
         <f>IF(raw_data_1!K28=raw_data_2!K28,"","check")</f>
         <v/>
       </c>
-    </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L28" t="str">
+        <f>IF(raw_data_1!L28=raw_data_2!L28,"","check")</f>
+        <v/>
+      </c>
+      <c r="M28" t="str">
+        <f>IF(raw_data_1!M28=raw_data_2!M28,"","check")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A29" t="str">
         <f>IF(raw_data_1!A29=raw_data_2!A29,"","check")</f>
         <v/>
@@ -3104,8 +4141,16 @@
         <f>IF(raw_data_1!K29=raw_data_2!K29,"","check")</f>
         <v/>
       </c>
-    </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L29" t="str">
+        <f>IF(raw_data_1!L29=raw_data_2!L29,"","check")</f>
+        <v/>
+      </c>
+      <c r="M29" t="str">
+        <f>IF(raw_data_1!M29=raw_data_2!M29,"","check")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A30" t="str">
         <f>IF(raw_data_1!A30=raw_data_2!A30,"","check")</f>
         <v/>
@@ -3150,8 +4195,16 @@
         <f>IF(raw_data_1!K30=raw_data_2!K30,"","check")</f>
         <v/>
       </c>
-    </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L30" t="str">
+        <f>IF(raw_data_1!L30=raw_data_2!L30,"","check")</f>
+        <v/>
+      </c>
+      <c r="M30" t="str">
+        <f>IF(raw_data_1!M30=raw_data_2!M30,"","check")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A31" t="str">
         <f>IF(raw_data_1!A31=raw_data_2!A31,"","check")</f>
         <v/>
@@ -3196,8 +4249,16 @@
         <f>IF(raw_data_1!K31=raw_data_2!K31,"","check")</f>
         <v/>
       </c>
-    </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L31" t="str">
+        <f>IF(raw_data_1!L31=raw_data_2!L31,"","check")</f>
+        <v/>
+      </c>
+      <c r="M31" t="str">
+        <f>IF(raw_data_1!M31=raw_data_2!M31,"","check")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A32" t="str">
         <f>IF(raw_data_1!A32=raw_data_2!A32,"","check")</f>
         <v/>
@@ -3242,8 +4303,16 @@
         <f>IF(raw_data_1!K32=raw_data_2!K32,"","check")</f>
         <v/>
       </c>
-    </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L32" t="str">
+        <f>IF(raw_data_1!L32=raw_data_2!L32,"","check")</f>
+        <v/>
+      </c>
+      <c r="M32" t="str">
+        <f>IF(raw_data_1!M32=raw_data_2!M32,"","check")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A33" t="str">
         <f>IF(raw_data_1!A33=raw_data_2!A33,"","check")</f>
         <v/>
@@ -3288,8 +4357,16 @@
         <f>IF(raw_data_1!K33=raw_data_2!K33,"","check")</f>
         <v/>
       </c>
-    </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L33" t="str">
+        <f>IF(raw_data_1!L33=raw_data_2!L33,"","check")</f>
+        <v/>
+      </c>
+      <c r="M33" t="str">
+        <f>IF(raw_data_1!M33=raw_data_2!M33,"","check")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A34" t="str">
         <f>IF(raw_data_1!A34=raw_data_2!A34,"","check")</f>
         <v/>
@@ -3334,8 +4411,16 @@
         <f>IF(raw_data_1!K34=raw_data_2!K34,"","check")</f>
         <v/>
       </c>
-    </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L34" t="str">
+        <f>IF(raw_data_1!L34=raw_data_2!L34,"","check")</f>
+        <v/>
+      </c>
+      <c r="M34" t="str">
+        <f>IF(raw_data_1!M34=raw_data_2!M34,"","check")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A35" t="str">
         <f>IF(raw_data_1!A35=raw_data_2!A35,"","check")</f>
         <v/>
@@ -3380,8 +4465,16 @@
         <f>IF(raw_data_1!K35=raw_data_2!K35,"","check")</f>
         <v/>
       </c>
-    </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L35" t="str">
+        <f>IF(raw_data_1!L35=raw_data_2!L35,"","check")</f>
+        <v/>
+      </c>
+      <c r="M35" t="str">
+        <f>IF(raw_data_1!M35=raw_data_2!M35,"","check")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A36" t="str">
         <f>IF(raw_data_1!A36=raw_data_2!A36,"","check")</f>
         <v/>
@@ -3426,8 +4519,16 @@
         <f>IF(raw_data_1!K36=raw_data_2!K36,"","check")</f>
         <v/>
       </c>
-    </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L36" t="str">
+        <f>IF(raw_data_1!L36=raw_data_2!L36,"","check")</f>
+        <v/>
+      </c>
+      <c r="M36" t="str">
+        <f>IF(raw_data_1!M36=raw_data_2!M36,"","check")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A37" t="str">
         <f>IF(raw_data_1!A37=raw_data_2!A37,"","check")</f>
         <v/>
@@ -3472,8 +4573,16 @@
         <f>IF(raw_data_1!K37=raw_data_2!K37,"","check")</f>
         <v/>
       </c>
-    </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L37" t="str">
+        <f>IF(raw_data_1!L37=raw_data_2!L37,"","check")</f>
+        <v/>
+      </c>
+      <c r="M37" t="str">
+        <f>IF(raw_data_1!M37=raw_data_2!M37,"","check")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A38" t="str">
         <f>IF(raw_data_1!A38=raw_data_2!A38,"","check")</f>
         <v/>
@@ -3518,8 +4627,16 @@
         <f>IF(raw_data_1!K38=raw_data_2!K38,"","check")</f>
         <v/>
       </c>
-    </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L38" t="str">
+        <f>IF(raw_data_1!L38=raw_data_2!L38,"","check")</f>
+        <v/>
+      </c>
+      <c r="M38" t="str">
+        <f>IF(raw_data_1!M38=raw_data_2!M38,"","check")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A39" t="str">
         <f>IF(raw_data_1!A39=raw_data_2!A39,"","check")</f>
         <v/>
@@ -3564,8 +4681,16 @@
         <f>IF(raw_data_1!K39=raw_data_2!K39,"","check")</f>
         <v/>
       </c>
-    </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L39" t="str">
+        <f>IF(raw_data_1!L39=raw_data_2!L39,"","check")</f>
+        <v/>
+      </c>
+      <c r="M39" t="str">
+        <f>IF(raw_data_1!M39=raw_data_2!M39,"","check")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A40" t="str">
         <f>IF(raw_data_1!A40=raw_data_2!A40,"","check")</f>
         <v/>
@@ -3610,8 +4735,16 @@
         <f>IF(raw_data_1!K40=raw_data_2!K40,"","check")</f>
         <v/>
       </c>
-    </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L40" t="str">
+        <f>IF(raw_data_1!L40=raw_data_2!L40,"","check")</f>
+        <v/>
+      </c>
+      <c r="M40" t="str">
+        <f>IF(raw_data_1!M40=raw_data_2!M40,"","check")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="41" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A41" t="str">
         <f>IF(raw_data_1!A41=raw_data_2!A41,"","check")</f>
         <v/>
@@ -3656,8 +4789,16 @@
         <f>IF(raw_data_1!K41=raw_data_2!K41,"","check")</f>
         <v/>
       </c>
-    </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L41" t="str">
+        <f>IF(raw_data_1!L41=raw_data_2!L41,"","check")</f>
+        <v/>
+      </c>
+      <c r="M41" t="str">
+        <f>IF(raw_data_1!M41=raw_data_2!M41,"","check")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="42" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A42" t="str">
         <f>IF(raw_data_1!A42=raw_data_2!A42,"","check")</f>
         <v/>
@@ -3702,8 +4843,16 @@
         <f>IF(raw_data_1!K42=raw_data_2!K42,"","check")</f>
         <v/>
       </c>
-    </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L42" t="str">
+        <f>IF(raw_data_1!L42=raw_data_2!L42,"","check")</f>
+        <v/>
+      </c>
+      <c r="M42" t="str">
+        <f>IF(raw_data_1!M42=raw_data_2!M42,"","check")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="43" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A43" t="str">
         <f>IF(raw_data_1!A43=raw_data_2!A43,"","check")</f>
         <v/>
@@ -3748,8 +4897,16 @@
         <f>IF(raw_data_1!K43=raw_data_2!K43,"","check")</f>
         <v/>
       </c>
-    </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L43" t="str">
+        <f>IF(raw_data_1!L43=raw_data_2!L43,"","check")</f>
+        <v/>
+      </c>
+      <c r="M43" t="str">
+        <f>IF(raw_data_1!M43=raw_data_2!M43,"","check")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="44" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A44" t="str">
         <f>IF(raw_data_1!A44=raw_data_2!A44,"","check")</f>
         <v/>
@@ -3794,8 +4951,16 @@
         <f>IF(raw_data_1!K44=raw_data_2!K44,"","check")</f>
         <v/>
       </c>
-    </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L44" t="str">
+        <f>IF(raw_data_1!L44=raw_data_2!L44,"","check")</f>
+        <v/>
+      </c>
+      <c r="M44" t="str">
+        <f>IF(raw_data_1!M44=raw_data_2!M44,"","check")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="45" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A45" t="str">
         <f>IF(raw_data_1!A45=raw_data_2!A45,"","check")</f>
         <v/>
@@ -3840,8 +5005,16 @@
         <f>IF(raw_data_1!K45=raw_data_2!K45,"","check")</f>
         <v/>
       </c>
-    </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L45" t="str">
+        <f>IF(raw_data_1!L45=raw_data_2!L45,"","check")</f>
+        <v/>
+      </c>
+      <c r="M45" t="str">
+        <f>IF(raw_data_1!M45=raw_data_2!M45,"","check")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="46" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A46" t="str">
         <f>IF(raw_data_1!A46=raw_data_2!A46,"","check")</f>
         <v/>
@@ -3886,8 +5059,16 @@
         <f>IF(raw_data_1!K46=raw_data_2!K46,"","check")</f>
         <v/>
       </c>
-    </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L46" t="str">
+        <f>IF(raw_data_1!L46=raw_data_2!L46,"","check")</f>
+        <v/>
+      </c>
+      <c r="M46" t="str">
+        <f>IF(raw_data_1!M46=raw_data_2!M46,"","check")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="47" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A47" t="str">
         <f>IF(raw_data_1!A47=raw_data_2!A47,"","check")</f>
         <v/>
@@ -3932,8 +5113,16 @@
         <f>IF(raw_data_1!K47=raw_data_2!K47,"","check")</f>
         <v/>
       </c>
-    </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L47" t="str">
+        <f>IF(raw_data_1!L47=raw_data_2!L47,"","check")</f>
+        <v/>
+      </c>
+      <c r="M47" t="str">
+        <f>IF(raw_data_1!M47=raw_data_2!M47,"","check")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="48" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A48" t="str">
         <f>IF(raw_data_1!A48=raw_data_2!A48,"","check")</f>
         <v/>
@@ -3978,8 +5167,16 @@
         <f>IF(raw_data_1!K48=raw_data_2!K48,"","check")</f>
         <v/>
       </c>
-    </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L48" t="str">
+        <f>IF(raw_data_1!L48=raw_data_2!L48,"","check")</f>
+        <v/>
+      </c>
+      <c r="M48" t="str">
+        <f>IF(raw_data_1!M48=raw_data_2!M48,"","check")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="49" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A49" t="str">
         <f>IF(raw_data_1!A49=raw_data_2!A49,"","check")</f>
         <v/>
@@ -4024,8 +5221,16 @@
         <f>IF(raw_data_1!K49=raw_data_2!K49,"","check")</f>
         <v/>
       </c>
-    </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L49" t="str">
+        <f>IF(raw_data_1!L49=raw_data_2!L49,"","check")</f>
+        <v/>
+      </c>
+      <c r="M49" t="str">
+        <f>IF(raw_data_1!M49=raw_data_2!M49,"","check")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="50" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A50" t="str">
         <f>IF(raw_data_1!A50=raw_data_2!A50,"","check")</f>
         <v/>
@@ -4070,8 +5275,16 @@
         <f>IF(raw_data_1!K50=raw_data_2!K50,"","check")</f>
         <v/>
       </c>
-    </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L50" t="str">
+        <f>IF(raw_data_1!L50=raw_data_2!L50,"","check")</f>
+        <v/>
+      </c>
+      <c r="M50" t="str">
+        <f>IF(raw_data_1!M50=raw_data_2!M50,"","check")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="51" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A51" t="str">
         <f>IF(raw_data_1!A51=raw_data_2!A51,"","check")</f>
         <v/>
@@ -4116,8 +5329,16 @@
         <f>IF(raw_data_1!K51=raw_data_2!K51,"","check")</f>
         <v/>
       </c>
-    </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L51" t="str">
+        <f>IF(raw_data_1!L51=raw_data_2!L51,"","check")</f>
+        <v/>
+      </c>
+      <c r="M51" t="str">
+        <f>IF(raw_data_1!M51=raw_data_2!M51,"","check")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="52" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A52" t="str">
         <f>IF(raw_data_1!A52=raw_data_2!A52,"","check")</f>
         <v/>
@@ -4162,8 +5383,16 @@
         <f>IF(raw_data_1!K52=raw_data_2!K52,"","check")</f>
         <v/>
       </c>
-    </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L52" t="str">
+        <f>IF(raw_data_1!L52=raw_data_2!L52,"","check")</f>
+        <v/>
+      </c>
+      <c r="M52" t="str">
+        <f>IF(raw_data_1!M52=raw_data_2!M52,"","check")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="53" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A53" t="str">
         <f>IF(raw_data_1!A53=raw_data_2!A53,"","check")</f>
         <v/>
@@ -4208,8 +5437,16 @@
         <f>IF(raw_data_1!K53=raw_data_2!K53,"","check")</f>
         <v/>
       </c>
-    </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L53" t="str">
+        <f>IF(raw_data_1!L53=raw_data_2!L53,"","check")</f>
+        <v/>
+      </c>
+      <c r="M53" t="str">
+        <f>IF(raw_data_1!M53=raw_data_2!M53,"","check")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="54" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A54" t="str">
         <f>IF(raw_data_1!A54=raw_data_2!A54,"","check")</f>
         <v/>
@@ -4254,8 +5491,16 @@
         <f>IF(raw_data_1!K54=raw_data_2!K54,"","check")</f>
         <v/>
       </c>
-    </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L54" t="str">
+        <f>IF(raw_data_1!L54=raw_data_2!L54,"","check")</f>
+        <v/>
+      </c>
+      <c r="M54" t="str">
+        <f>IF(raw_data_1!M54=raw_data_2!M54,"","check")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="55" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A55" t="str">
         <f>IF(raw_data_1!A55=raw_data_2!A55,"","check")</f>
         <v/>
@@ -4300,8 +5545,16 @@
         <f>IF(raw_data_1!K55=raw_data_2!K55,"","check")</f>
         <v/>
       </c>
-    </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L55" t="str">
+        <f>IF(raw_data_1!L55=raw_data_2!L55,"","check")</f>
+        <v/>
+      </c>
+      <c r="M55" t="str">
+        <f>IF(raw_data_1!M55=raw_data_2!M55,"","check")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="56" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A56" t="str">
         <f>IF(raw_data_1!A56=raw_data_2!A56,"","check")</f>
         <v/>
@@ -4346,8 +5599,16 @@
         <f>IF(raw_data_1!K56=raw_data_2!K56,"","check")</f>
         <v/>
       </c>
-    </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L56" t="str">
+        <f>IF(raw_data_1!L56=raw_data_2!L56,"","check")</f>
+        <v/>
+      </c>
+      <c r="M56" t="str">
+        <f>IF(raw_data_1!M56=raw_data_2!M56,"","check")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="57" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A57" t="str">
         <f>IF(raw_data_1!A57=raw_data_2!A57,"","check")</f>
         <v/>
@@ -4392,8 +5653,16 @@
         <f>IF(raw_data_1!K57=raw_data_2!K57,"","check")</f>
         <v/>
       </c>
-    </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L57" t="str">
+        <f>IF(raw_data_1!L57=raw_data_2!L57,"","check")</f>
+        <v/>
+      </c>
+      <c r="M57" t="str">
+        <f>IF(raw_data_1!M57=raw_data_2!M57,"","check")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="58" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A58" t="str">
         <f>IF(raw_data_1!A58=raw_data_2!A58,"","check")</f>
         <v/>
@@ -4438,8 +5707,16 @@
         <f>IF(raw_data_1!K58=raw_data_2!K58,"","check")</f>
         <v/>
       </c>
-    </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L58" t="str">
+        <f>IF(raw_data_1!L58=raw_data_2!L58,"","check")</f>
+        <v/>
+      </c>
+      <c r="M58" t="str">
+        <f>IF(raw_data_1!M58=raw_data_2!M58,"","check")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="59" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A59" t="str">
         <f>IF(raw_data_1!A59=raw_data_2!A59,"","check")</f>
         <v/>
@@ -4484,8 +5761,16 @@
         <f>IF(raw_data_1!K59=raw_data_2!K59,"","check")</f>
         <v/>
       </c>
-    </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L59" t="str">
+        <f>IF(raw_data_1!L59=raw_data_2!L59,"","check")</f>
+        <v/>
+      </c>
+      <c r="M59" t="str">
+        <f>IF(raw_data_1!M59=raw_data_2!M59,"","check")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="60" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A60" t="str">
         <f>IF(raw_data_1!A60=raw_data_2!A60,"","check")</f>
         <v/>
@@ -4530,8 +5815,16 @@
         <f>IF(raw_data_1!K60=raw_data_2!K60,"","check")</f>
         <v/>
       </c>
-    </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L60" t="str">
+        <f>IF(raw_data_1!L60=raw_data_2!L60,"","check")</f>
+        <v/>
+      </c>
+      <c r="M60" t="str">
+        <f>IF(raw_data_1!M60=raw_data_2!M60,"","check")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="61" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A61" t="str">
         <f>IF(raw_data_1!A61=raw_data_2!A61,"","check")</f>
         <v/>
@@ -4576,8 +5869,16 @@
         <f>IF(raw_data_1!K61=raw_data_2!K61,"","check")</f>
         <v/>
       </c>
-    </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L61" t="str">
+        <f>IF(raw_data_1!L61=raw_data_2!L61,"","check")</f>
+        <v/>
+      </c>
+      <c r="M61" t="str">
+        <f>IF(raw_data_1!M61=raw_data_2!M61,"","check")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="62" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A62" t="str">
         <f>IF(raw_data_1!A62=raw_data_2!A62,"","check")</f>
         <v/>
@@ -4622,8 +5923,16 @@
         <f>IF(raw_data_1!K62=raw_data_2!K62,"","check")</f>
         <v/>
       </c>
-    </row>
-    <row r="63" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L62" t="str">
+        <f>IF(raw_data_1!L62=raw_data_2!L62,"","check")</f>
+        <v/>
+      </c>
+      <c r="M62" t="str">
+        <f>IF(raw_data_1!M62=raw_data_2!M62,"","check")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="63" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A63" t="str">
         <f>IF(raw_data_1!A63=raw_data_2!A63,"","check")</f>
         <v/>
@@ -4668,8 +5977,16 @@
         <f>IF(raw_data_1!K63=raw_data_2!K63,"","check")</f>
         <v/>
       </c>
-    </row>
-    <row r="64" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L63" t="str">
+        <f>IF(raw_data_1!L63=raw_data_2!L63,"","check")</f>
+        <v/>
+      </c>
+      <c r="M63" t="str">
+        <f>IF(raw_data_1!M63=raw_data_2!M63,"","check")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="64" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A64" t="str">
         <f>IF(raw_data_1!A64=raw_data_2!A64,"","check")</f>
         <v/>
@@ -4714,8 +6031,16 @@
         <f>IF(raw_data_1!K64=raw_data_2!K64,"","check")</f>
         <v/>
       </c>
-    </row>
-    <row r="65" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L64" t="str">
+        <f>IF(raw_data_1!L64=raw_data_2!L64,"","check")</f>
+        <v/>
+      </c>
+      <c r="M64" t="str">
+        <f>IF(raw_data_1!M64=raw_data_2!M64,"","check")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="65" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A65" t="str">
         <f>IF(raw_data_1!A65=raw_data_2!A65,"","check")</f>
         <v/>
@@ -4760,8 +6085,16 @@
         <f>IF(raw_data_1!K65=raw_data_2!K65,"","check")</f>
         <v/>
       </c>
-    </row>
-    <row r="66" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L65" t="str">
+        <f>IF(raw_data_1!L65=raw_data_2!L65,"","check")</f>
+        <v/>
+      </c>
+      <c r="M65" t="str">
+        <f>IF(raw_data_1!M65=raw_data_2!M65,"","check")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="66" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A66" t="str">
         <f>IF(raw_data_1!A66=raw_data_2!A66,"","check")</f>
         <v/>
@@ -4806,8 +6139,16 @@
         <f>IF(raw_data_1!K66=raw_data_2!K66,"","check")</f>
         <v/>
       </c>
-    </row>
-    <row r="67" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L66" t="str">
+        <f>IF(raw_data_1!L66=raw_data_2!L66,"","check")</f>
+        <v/>
+      </c>
+      <c r="M66" t="str">
+        <f>IF(raw_data_1!M66=raw_data_2!M66,"","check")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="67" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A67" t="str">
         <f>IF(raw_data_1!A67=raw_data_2!A67,"","check")</f>
         <v/>
@@ -4852,8 +6193,16 @@
         <f>IF(raw_data_1!K67=raw_data_2!K67,"","check")</f>
         <v/>
       </c>
-    </row>
-    <row r="68" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L67" t="str">
+        <f>IF(raw_data_1!L67=raw_data_2!L67,"","check")</f>
+        <v/>
+      </c>
+      <c r="M67" t="str">
+        <f>IF(raw_data_1!M67=raw_data_2!M67,"","check")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="68" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A68" t="str">
         <f>IF(raw_data_1!A68=raw_data_2!A68,"","check")</f>
         <v/>
@@ -4898,8 +6247,16 @@
         <f>IF(raw_data_1!K68=raw_data_2!K68,"","check")</f>
         <v/>
       </c>
-    </row>
-    <row r="69" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L68" t="str">
+        <f>IF(raw_data_1!L68=raw_data_2!L68,"","check")</f>
+        <v/>
+      </c>
+      <c r="M68" t="str">
+        <f>IF(raw_data_1!M68=raw_data_2!M68,"","check")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="69" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A69" t="str">
         <f>IF(raw_data_1!A69=raw_data_2!A69,"","check")</f>
         <v/>
@@ -4944,8 +6301,16 @@
         <f>IF(raw_data_1!K69=raw_data_2!K69,"","check")</f>
         <v/>
       </c>
-    </row>
-    <row r="70" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L69" t="str">
+        <f>IF(raw_data_1!L69=raw_data_2!L69,"","check")</f>
+        <v/>
+      </c>
+      <c r="M69" t="str">
+        <f>IF(raw_data_1!M69=raw_data_2!M69,"","check")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="70" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A70" t="str">
         <f>IF(raw_data_1!A70=raw_data_2!A70,"","check")</f>
         <v/>
@@ -4990,8 +6355,16 @@
         <f>IF(raw_data_1!K70=raw_data_2!K70,"","check")</f>
         <v/>
       </c>
-    </row>
-    <row r="71" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L70" t="str">
+        <f>IF(raw_data_1!L70=raw_data_2!L70,"","check")</f>
+        <v/>
+      </c>
+      <c r="M70" t="str">
+        <f>IF(raw_data_1!M70=raw_data_2!M70,"","check")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="71" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A71" t="str">
         <f>IF(raw_data_1!A71=raw_data_2!A71,"","check")</f>
         <v/>
@@ -5036,8 +6409,16 @@
         <f>IF(raw_data_1!K71=raw_data_2!K71,"","check")</f>
         <v/>
       </c>
-    </row>
-    <row r="72" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L71" t="str">
+        <f>IF(raw_data_1!L71=raw_data_2!L71,"","check")</f>
+        <v/>
+      </c>
+      <c r="M71" t="str">
+        <f>IF(raw_data_1!M71=raw_data_2!M71,"","check")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="72" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A72" t="str">
         <f>IF(raw_data_1!A72=raw_data_2!A72,"","check")</f>
         <v/>
@@ -5082,8 +6463,16 @@
         <f>IF(raw_data_1!K72=raw_data_2!K72,"","check")</f>
         <v/>
       </c>
-    </row>
-    <row r="73" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L72" t="str">
+        <f>IF(raw_data_1!L72=raw_data_2!L72,"","check")</f>
+        <v/>
+      </c>
+      <c r="M72" t="str">
+        <f>IF(raw_data_1!M72=raw_data_2!M72,"","check")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="73" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A73" t="str">
         <f>IF(raw_data_1!A73=raw_data_2!A73,"","check")</f>
         <v/>
@@ -5128,8 +6517,16 @@
         <f>IF(raw_data_1!K73=raw_data_2!K73,"","check")</f>
         <v/>
       </c>
-    </row>
-    <row r="74" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L73" t="str">
+        <f>IF(raw_data_1!L73=raw_data_2!L73,"","check")</f>
+        <v/>
+      </c>
+      <c r="M73" t="str">
+        <f>IF(raw_data_1!M73=raw_data_2!M73,"","check")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="74" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A74" t="str">
         <f>IF(raw_data_1!A74=raw_data_2!A74,"","check")</f>
         <v/>
@@ -5174,8 +6571,16 @@
         <f>IF(raw_data_1!K74=raw_data_2!K74,"","check")</f>
         <v/>
       </c>
-    </row>
-    <row r="75" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L74" t="str">
+        <f>IF(raw_data_1!L74=raw_data_2!L74,"","check")</f>
+        <v/>
+      </c>
+      <c r="M74" t="str">
+        <f>IF(raw_data_1!M74=raw_data_2!M74,"","check")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="75" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A75" t="str">
         <f>IF(raw_data_1!A75=raw_data_2!A75,"","check")</f>
         <v/>
@@ -5220,8 +6625,16 @@
         <f>IF(raw_data_1!K75=raw_data_2!K75,"","check")</f>
         <v/>
       </c>
-    </row>
-    <row r="76" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L75" t="str">
+        <f>IF(raw_data_1!L75=raw_data_2!L75,"","check")</f>
+        <v/>
+      </c>
+      <c r="M75" t="str">
+        <f>IF(raw_data_1!M75=raw_data_2!M75,"","check")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="76" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A76" t="str">
         <f>IF(raw_data_1!A76=raw_data_2!A76,"","check")</f>
         <v/>
@@ -5266,8 +6679,16 @@
         <f>IF(raw_data_1!K76=raw_data_2!K76,"","check")</f>
         <v/>
       </c>
-    </row>
-    <row r="77" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L76" t="str">
+        <f>IF(raw_data_1!L76=raw_data_2!L76,"","check")</f>
+        <v/>
+      </c>
+      <c r="M76" t="str">
+        <f>IF(raw_data_1!M76=raw_data_2!M76,"","check")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="77" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A77" t="str">
         <f>IF(raw_data_1!A77=raw_data_2!A77,"","check")</f>
         <v/>
@@ -5312,8 +6733,16 @@
         <f>IF(raw_data_1!K77=raw_data_2!K77,"","check")</f>
         <v/>
       </c>
-    </row>
-    <row r="78" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L77" t="str">
+        <f>IF(raw_data_1!L77=raw_data_2!L77,"","check")</f>
+        <v/>
+      </c>
+      <c r="M77" t="str">
+        <f>IF(raw_data_1!M77=raw_data_2!M77,"","check")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="78" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A78" t="str">
         <f>IF(raw_data_1!A78=raw_data_2!A78,"","check")</f>
         <v/>
@@ -5358,8 +6787,16 @@
         <f>IF(raw_data_1!K78=raw_data_2!K78,"","check")</f>
         <v/>
       </c>
-    </row>
-    <row r="79" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L78" t="str">
+        <f>IF(raw_data_1!L78=raw_data_2!L78,"","check")</f>
+        <v/>
+      </c>
+      <c r="M78" t="str">
+        <f>IF(raw_data_1!M78=raw_data_2!M78,"","check")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="79" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A79" t="str">
         <f>IF(raw_data_1!A79=raw_data_2!A79,"","check")</f>
         <v/>
@@ -5404,8 +6841,16 @@
         <f>IF(raw_data_1!K79=raw_data_2!K79,"","check")</f>
         <v/>
       </c>
-    </row>
-    <row r="80" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L79" t="str">
+        <f>IF(raw_data_1!L79=raw_data_2!L79,"","check")</f>
+        <v/>
+      </c>
+      <c r="M79" t="str">
+        <f>IF(raw_data_1!M79=raw_data_2!M79,"","check")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="80" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A80" t="str">
         <f>IF(raw_data_1!A80=raw_data_2!A80,"","check")</f>
         <v/>
@@ -5450,8 +6895,16 @@
         <f>IF(raw_data_1!K80=raw_data_2!K80,"","check")</f>
         <v/>
       </c>
-    </row>
-    <row r="81" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L80" t="str">
+        <f>IF(raw_data_1!L80=raw_data_2!L80,"","check")</f>
+        <v/>
+      </c>
+      <c r="M80" t="str">
+        <f>IF(raw_data_1!M80=raw_data_2!M80,"","check")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="81" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A81" t="str">
         <f>IF(raw_data_1!A81=raw_data_2!A81,"","check")</f>
         <v/>
@@ -5496,8 +6949,16 @@
         <f>IF(raw_data_1!K81=raw_data_2!K81,"","check")</f>
         <v/>
       </c>
-    </row>
-    <row r="82" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L81" t="str">
+        <f>IF(raw_data_1!L81=raw_data_2!L81,"","check")</f>
+        <v/>
+      </c>
+      <c r="M81" t="str">
+        <f>IF(raw_data_1!M81=raw_data_2!M81,"","check")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="82" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A82" t="str">
         <f>IF(raw_data_1!A82=raw_data_2!A82,"","check")</f>
         <v/>
@@ -5542,8 +7003,16 @@
         <f>IF(raw_data_1!K82=raw_data_2!K82,"","check")</f>
         <v/>
       </c>
-    </row>
-    <row r="83" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L82" t="str">
+        <f>IF(raw_data_1!L82=raw_data_2!L82,"","check")</f>
+        <v/>
+      </c>
+      <c r="M82" t="str">
+        <f>IF(raw_data_1!M82=raw_data_2!M82,"","check")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="83" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A83" t="str">
         <f>IF(raw_data_1!A83=raw_data_2!A83,"","check")</f>
         <v/>
@@ -5588,8 +7057,16 @@
         <f>IF(raw_data_1!K83=raw_data_2!K83,"","check")</f>
         <v/>
       </c>
-    </row>
-    <row r="84" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L83" t="str">
+        <f>IF(raw_data_1!L83=raw_data_2!L83,"","check")</f>
+        <v/>
+      </c>
+      <c r="M83" t="str">
+        <f>IF(raw_data_1!M83=raw_data_2!M83,"","check")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="84" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A84" t="str">
         <f>IF(raw_data_1!A84=raw_data_2!A84,"","check")</f>
         <v/>
@@ -5634,8 +7111,16 @@
         <f>IF(raw_data_1!K84=raw_data_2!K84,"","check")</f>
         <v/>
       </c>
-    </row>
-    <row r="85" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L84" t="str">
+        <f>IF(raw_data_1!L84=raw_data_2!L84,"","check")</f>
+        <v/>
+      </c>
+      <c r="M84" t="str">
+        <f>IF(raw_data_1!M84=raw_data_2!M84,"","check")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="85" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A85" t="str">
         <f>IF(raw_data_1!A85=raw_data_2!A85,"","check")</f>
         <v/>
@@ -5680,8 +7165,16 @@
         <f>IF(raw_data_1!K85=raw_data_2!K85,"","check")</f>
         <v/>
       </c>
-    </row>
-    <row r="86" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L85" t="str">
+        <f>IF(raw_data_1!L85=raw_data_2!L85,"","check")</f>
+        <v/>
+      </c>
+      <c r="M85" t="str">
+        <f>IF(raw_data_1!M85=raw_data_2!M85,"","check")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="86" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A86" t="str">
         <f>IF(raw_data_1!A86=raw_data_2!A86,"","check")</f>
         <v/>
@@ -5726,8 +7219,16 @@
         <f>IF(raw_data_1!K86=raw_data_2!K86,"","check")</f>
         <v/>
       </c>
-    </row>
-    <row r="87" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L86" t="str">
+        <f>IF(raw_data_1!L86=raw_data_2!L86,"","check")</f>
+        <v/>
+      </c>
+      <c r="M86" t="str">
+        <f>IF(raw_data_1!M86=raw_data_2!M86,"","check")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="87" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A87" t="str">
         <f>IF(raw_data_1!A87=raw_data_2!A87,"","check")</f>
         <v/>
@@ -5772,8 +7273,16 @@
         <f>IF(raw_data_1!K87=raw_data_2!K87,"","check")</f>
         <v/>
       </c>
-    </row>
-    <row r="88" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L87" t="str">
+        <f>IF(raw_data_1!L87=raw_data_2!L87,"","check")</f>
+        <v/>
+      </c>
+      <c r="M87" t="str">
+        <f>IF(raw_data_1!M87=raw_data_2!M87,"","check")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="88" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A88" t="str">
         <f>IF(raw_data_1!A88=raw_data_2!A88,"","check")</f>
         <v/>
@@ -5818,8 +7327,16 @@
         <f>IF(raw_data_1!K88=raw_data_2!K88,"","check")</f>
         <v/>
       </c>
-    </row>
-    <row r="89" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L88" t="str">
+        <f>IF(raw_data_1!L88=raw_data_2!L88,"","check")</f>
+        <v/>
+      </c>
+      <c r="M88" t="str">
+        <f>IF(raw_data_1!M88=raw_data_2!M88,"","check")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="89" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A89" t="str">
         <f>IF(raw_data_1!A89=raw_data_2!A89,"","check")</f>
         <v/>
@@ -5864,8 +7381,16 @@
         <f>IF(raw_data_1!K89=raw_data_2!K89,"","check")</f>
         <v/>
       </c>
-    </row>
-    <row r="90" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L89" t="str">
+        <f>IF(raw_data_1!L89=raw_data_2!L89,"","check")</f>
+        <v/>
+      </c>
+      <c r="M89" t="str">
+        <f>IF(raw_data_1!M89=raw_data_2!M89,"","check")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="90" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A90" t="str">
         <f>IF(raw_data_1!A90=raw_data_2!A90,"","check")</f>
         <v/>
@@ -5910,8 +7435,16 @@
         <f>IF(raw_data_1!K90=raw_data_2!K90,"","check")</f>
         <v/>
       </c>
-    </row>
-    <row r="91" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L90" t="str">
+        <f>IF(raw_data_1!L90=raw_data_2!L90,"","check")</f>
+        <v/>
+      </c>
+      <c r="M90" t="str">
+        <f>IF(raw_data_1!M90=raw_data_2!M90,"","check")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="91" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A91" t="str">
         <f>IF(raw_data_1!A91=raw_data_2!A91,"","check")</f>
         <v/>
@@ -5956,8 +7489,16 @@
         <f>IF(raw_data_1!K91=raw_data_2!K91,"","check")</f>
         <v/>
       </c>
-    </row>
-    <row r="92" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L91" t="str">
+        <f>IF(raw_data_1!L91=raw_data_2!L91,"","check")</f>
+        <v/>
+      </c>
+      <c r="M91" t="str">
+        <f>IF(raw_data_1!M91=raw_data_2!M91,"","check")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="92" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A92" t="str">
         <f>IF(raw_data_1!A92=raw_data_2!A92,"","check")</f>
         <v/>
@@ -6002,8 +7543,16 @@
         <f>IF(raw_data_1!K92=raw_data_2!K92,"","check")</f>
         <v/>
       </c>
-    </row>
-    <row r="93" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L92" t="str">
+        <f>IF(raw_data_1!L92=raw_data_2!L92,"","check")</f>
+        <v/>
+      </c>
+      <c r="M92" t="str">
+        <f>IF(raw_data_1!M92=raw_data_2!M92,"","check")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="93" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A93" t="str">
         <f>IF(raw_data_1!A93=raw_data_2!A93,"","check")</f>
         <v/>
@@ -6048,8 +7597,16 @@
         <f>IF(raw_data_1!K93=raw_data_2!K93,"","check")</f>
         <v/>
       </c>
-    </row>
-    <row r="94" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L93" t="str">
+        <f>IF(raw_data_1!L93=raw_data_2!L93,"","check")</f>
+        <v/>
+      </c>
+      <c r="M93" t="str">
+        <f>IF(raw_data_1!M93=raw_data_2!M93,"","check")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="94" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A94" t="str">
         <f>IF(raw_data_1!A94=raw_data_2!A94,"","check")</f>
         <v/>
@@ -6094,8 +7651,16 @@
         <f>IF(raw_data_1!K94=raw_data_2!K94,"","check")</f>
         <v/>
       </c>
-    </row>
-    <row r="95" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L94" t="str">
+        <f>IF(raw_data_1!L94=raw_data_2!L94,"","check")</f>
+        <v/>
+      </c>
+      <c r="M94" t="str">
+        <f>IF(raw_data_1!M94=raw_data_2!M94,"","check")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="95" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A95" t="str">
         <f>IF(raw_data_1!A95=raw_data_2!A95,"","check")</f>
         <v/>
@@ -6140,8 +7705,16 @@
         <f>IF(raw_data_1!K95=raw_data_2!K95,"","check")</f>
         <v/>
       </c>
-    </row>
-    <row r="96" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L95" t="str">
+        <f>IF(raw_data_1!L95=raw_data_2!L95,"","check")</f>
+        <v/>
+      </c>
+      <c r="M95" t="str">
+        <f>IF(raw_data_1!M95=raw_data_2!M95,"","check")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="96" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A96" t="str">
         <f>IF(raw_data_1!A96=raw_data_2!A96,"","check")</f>
         <v/>
@@ -6186,8 +7759,16 @@
         <f>IF(raw_data_1!K96=raw_data_2!K96,"","check")</f>
         <v/>
       </c>
-    </row>
-    <row r="97" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L96" t="str">
+        <f>IF(raw_data_1!L96=raw_data_2!L96,"","check")</f>
+        <v/>
+      </c>
+      <c r="M96" t="str">
+        <f>IF(raw_data_1!M96=raw_data_2!M96,"","check")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="97" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A97" t="str">
         <f>IF(raw_data_1!A97=raw_data_2!A97,"","check")</f>
         <v/>
@@ -6232,8 +7813,16 @@
         <f>IF(raw_data_1!K97=raw_data_2!K97,"","check")</f>
         <v/>
       </c>
-    </row>
-    <row r="98" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L97" t="str">
+        <f>IF(raw_data_1!L97=raw_data_2!L97,"","check")</f>
+        <v/>
+      </c>
+      <c r="M97" t="str">
+        <f>IF(raw_data_1!M97=raw_data_2!M97,"","check")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="98" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A98" t="str">
         <f>IF(raw_data_1!A98=raw_data_2!A98,"","check")</f>
         <v/>
@@ -6278,8 +7867,16 @@
         <f>IF(raw_data_1!K98=raw_data_2!K98,"","check")</f>
         <v/>
       </c>
-    </row>
-    <row r="99" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L98" t="str">
+        <f>IF(raw_data_1!L98=raw_data_2!L98,"","check")</f>
+        <v/>
+      </c>
+      <c r="M98" t="str">
+        <f>IF(raw_data_1!M98=raw_data_2!M98,"","check")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="99" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A99" t="str">
         <f>IF(raw_data_1!A99=raw_data_2!A99,"","check")</f>
         <v/>
@@ -6324,8 +7921,16 @@
         <f>IF(raw_data_1!K99=raw_data_2!K99,"","check")</f>
         <v/>
       </c>
-    </row>
-    <row r="100" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L99" t="str">
+        <f>IF(raw_data_1!L99=raw_data_2!L99,"","check")</f>
+        <v/>
+      </c>
+      <c r="M99" t="str">
+        <f>IF(raw_data_1!M99=raw_data_2!M99,"","check")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="100" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A100" t="str">
         <f>IF(raw_data_1!A100=raw_data_2!A100,"","check")</f>
         <v/>
@@ -6368,6 +7973,14 @@
       </c>
       <c r="K100" t="str">
         <f>IF(raw_data_1!K100=raw_data_2!K100,"","check")</f>
+        <v/>
+      </c>
+      <c r="L100" t="str">
+        <f>IF(raw_data_1!L100=raw_data_2!L100,"","check")</f>
+        <v/>
+      </c>
+      <c r="M100" t="str">
+        <f>IF(raw_data_1!M100=raw_data_2!M100,"","check")</f>
         <v/>
       </c>
     </row>
@@ -6426,15 +8039,15 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K32"/>
+  <dimension ref="A1:M32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+      <selection activeCell="L10" sqref="L10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>16</v>
       </c>
@@ -6468,8 +8081,14 @@
       <c r="K1" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L1" t="s">
+        <v>44</v>
+      </c>
+      <c r="M1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>2019</v>
       </c>
@@ -6491,8 +8110,14 @@
       <c r="G2">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L2" t="s">
+        <v>46</v>
+      </c>
+      <c r="M2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B3">
         <v>9</v>
       </c>
@@ -6511,8 +8136,14 @@
       <c r="G3">
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L3" t="s">
+        <v>49</v>
+      </c>
+      <c r="M3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="C4">
         <v>3</v>
       </c>
@@ -6525,8 +8156,14 @@
       <c r="G4">
         <v>3</v>
       </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L4" t="s">
+        <v>50</v>
+      </c>
+      <c r="M4" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="C5">
         <v>4</v>
       </c>
@@ -6539,16 +8176,28 @@
       <c r="G5">
         <v>4</v>
       </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L5" t="s">
+        <v>51</v>
+      </c>
+      <c r="M5" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="C6">
         <v>5</v>
       </c>
       <c r="F6">
         <v>5</v>
       </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L6" t="s">
+        <v>52</v>
+      </c>
+      <c r="M6" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="C7">
         <v>6</v>
       </c>
@@ -6556,7 +8205,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="C8">
         <v>7</v>
       </c>
@@ -6564,7 +8213,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="C9">
         <v>8</v>
       </c>
@@ -6572,7 +8221,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="C10">
         <v>9</v>
       </c>
@@ -6580,7 +8229,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="C11">
         <v>10</v>
       </c>
@@ -6588,7 +8237,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="C12">
         <v>11</v>
       </c>
@@ -6596,7 +8245,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="C13">
         <v>12</v>
       </c>
@@ -6604,7 +8253,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="C14">
         <v>13</v>
       </c>
@@ -6612,7 +8261,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="C15">
         <v>14</v>
       </c>
@@ -6620,7 +8269,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="C16">
         <v>15</v>
       </c>
@@ -6730,10 +8379,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B11"/>
+  <dimension ref="A1:B13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="O17" sqref="O17"/>
+      <selection activeCell="J18" sqref="J18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6829,6 +8478,22 @@
         <v>43</v>
       </c>
     </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>44</v>
+      </c>
+      <c r="B12" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>45</v>
+      </c>
+      <c r="B13" t="s">
+        <v>48</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
update with final cultch mass locations
</commit_message>
<xml_diff>
--- a/Oyster/cultchmass/cultchmass_packet.xlsx
+++ b/Oyster/cultchmass/cultchmass_packet.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="datasheet" sheetId="1" r:id="rId1"/>
@@ -13,6 +13,7 @@
     <sheet name="raw_check" sheetId="4" r:id="rId4"/>
     <sheet name="pick" sheetId="5" r:id="rId5"/>
     <sheet name="description" sheetId="6" r:id="rId6"/>
+    <sheet name="progress" sheetId="9" r:id="rId7"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="309" uniqueCount="75">
   <si>
     <t>REEF MASS FIELD DATASHEET</t>
   </si>
@@ -184,6 +185,72 @@
   <si>
     <t>jh</t>
   </si>
+  <si>
+    <t>station</t>
+  </si>
+  <si>
+    <t>sampled</t>
+  </si>
+  <si>
+    <t>scanned</t>
+  </si>
+  <si>
+    <t>entry1</t>
+  </si>
+  <si>
+    <t>entry2</t>
+  </si>
+  <si>
+    <t>database</t>
+  </si>
+  <si>
+    <t>BTI1</t>
+  </si>
+  <si>
+    <t>BTI5</t>
+  </si>
+  <si>
+    <t>BTI6</t>
+  </si>
+  <si>
+    <t>LCI1</t>
+  </si>
+  <si>
+    <t>LCI12</t>
+  </si>
+  <si>
+    <t>LCI19</t>
+  </si>
+  <si>
+    <t>LCI2</t>
+  </si>
+  <si>
+    <t>LCI6</t>
+  </si>
+  <si>
+    <t>LCI8</t>
+  </si>
+  <si>
+    <t>LCN3</t>
+  </si>
+  <si>
+    <t>LCN7</t>
+  </si>
+  <si>
+    <t>LCN8</t>
+  </si>
+  <si>
+    <t>LTI1</t>
+  </si>
+  <si>
+    <t>LTI5</t>
+  </si>
+  <si>
+    <t>LTI6</t>
+  </si>
+  <si>
+    <t>NNI1</t>
+  </si>
 </sst>
 </file>
 
@@ -327,7 +394,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -389,6 +456,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1816,7 +1884,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="O19" sqref="O19"/>
     </sheetView>
   </sheetViews>
@@ -8497,4 +8565,1085 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G65"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="P57" sqref="P57"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="7" width="9.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D1" t="s">
+        <v>55</v>
+      </c>
+      <c r="E1" t="s">
+        <v>56</v>
+      </c>
+      <c r="F1" t="s">
+        <v>57</v>
+      </c>
+      <c r="G1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>59</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2" s="21">
+        <v>43732</v>
+      </c>
+      <c r="D2" s="21">
+        <v>43733</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>59</v>
+      </c>
+      <c r="B3">
+        <v>2</v>
+      </c>
+      <c r="C3" s="21">
+        <v>43732</v>
+      </c>
+      <c r="D3" s="21">
+        <v>43733</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>59</v>
+      </c>
+      <c r="B4">
+        <v>3</v>
+      </c>
+      <c r="C4" s="21">
+        <v>43732</v>
+      </c>
+      <c r="D4" s="21">
+        <v>43733</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>59</v>
+      </c>
+      <c r="B5">
+        <v>4</v>
+      </c>
+      <c r="C5" s="21">
+        <v>43732</v>
+      </c>
+      <c r="D5" s="21">
+        <v>43733</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>60</v>
+      </c>
+      <c r="B6">
+        <v>1</v>
+      </c>
+      <c r="C6" s="21">
+        <v>43732</v>
+      </c>
+      <c r="D6" s="21">
+        <v>43733</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>60</v>
+      </c>
+      <c r="B7">
+        <v>2</v>
+      </c>
+      <c r="C7" s="21">
+        <v>43732</v>
+      </c>
+      <c r="D7" s="21">
+        <v>43733</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>60</v>
+      </c>
+      <c r="B8">
+        <v>3</v>
+      </c>
+      <c r="C8" s="21">
+        <v>43732</v>
+      </c>
+      <c r="D8" s="21">
+        <v>43733</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>60</v>
+      </c>
+      <c r="B9">
+        <v>4</v>
+      </c>
+      <c r="C9" s="21">
+        <v>43732</v>
+      </c>
+      <c r="D9" s="21">
+        <v>43733</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>61</v>
+      </c>
+      <c r="B10">
+        <v>1</v>
+      </c>
+      <c r="C10" s="21">
+        <v>43733</v>
+      </c>
+      <c r="D10" s="21">
+        <v>43734</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>61</v>
+      </c>
+      <c r="B11">
+        <v>2</v>
+      </c>
+      <c r="C11" s="21">
+        <v>43733</v>
+      </c>
+      <c r="D11" s="21">
+        <v>43734</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>61</v>
+      </c>
+      <c r="B12">
+        <v>3</v>
+      </c>
+      <c r="C12" s="21">
+        <v>43733</v>
+      </c>
+      <c r="D12" s="21">
+        <v>43734</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>61</v>
+      </c>
+      <c r="B13">
+        <v>4</v>
+      </c>
+      <c r="C13" s="21">
+        <v>43733</v>
+      </c>
+      <c r="D13" s="21">
+        <v>43734</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>62</v>
+      </c>
+      <c r="B14">
+        <v>1</v>
+      </c>
+      <c r="C14" s="21">
+        <v>43703</v>
+      </c>
+      <c r="D14" s="21">
+        <v>43704</v>
+      </c>
+      <c r="E14" s="21">
+        <v>43720</v>
+      </c>
+      <c r="F14" s="21">
+        <v>43721</v>
+      </c>
+      <c r="G14" s="21">
+        <v>43721</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>62</v>
+      </c>
+      <c r="B15">
+        <v>2</v>
+      </c>
+      <c r="C15" s="21">
+        <v>43703</v>
+      </c>
+      <c r="D15" s="21">
+        <v>43704</v>
+      </c>
+      <c r="E15" s="21">
+        <v>43720</v>
+      </c>
+      <c r="F15" s="21">
+        <v>43721</v>
+      </c>
+      <c r="G15" s="21">
+        <v>43721</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>62</v>
+      </c>
+      <c r="B16">
+        <v>3</v>
+      </c>
+      <c r="C16" s="21">
+        <v>43703</v>
+      </c>
+      <c r="D16" s="21">
+        <v>43704</v>
+      </c>
+      <c r="E16" s="21">
+        <v>43720</v>
+      </c>
+      <c r="F16" s="21">
+        <v>43721</v>
+      </c>
+      <c r="G16" s="21">
+        <v>43721</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>62</v>
+      </c>
+      <c r="B17">
+        <v>4</v>
+      </c>
+      <c r="C17" s="21">
+        <v>43703</v>
+      </c>
+      <c r="D17" s="21">
+        <v>43704</v>
+      </c>
+      <c r="E17" s="21">
+        <v>43720</v>
+      </c>
+      <c r="F17" s="21">
+        <v>43721</v>
+      </c>
+      <c r="G17" s="21">
+        <v>43721</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>63</v>
+      </c>
+      <c r="B18">
+        <v>1</v>
+      </c>
+      <c r="C18" s="21">
+        <v>43703</v>
+      </c>
+      <c r="D18" s="21">
+        <v>43704</v>
+      </c>
+      <c r="E18" s="21">
+        <v>43720</v>
+      </c>
+      <c r="F18" s="21">
+        <v>43721</v>
+      </c>
+      <c r="G18" s="21">
+        <v>43721</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>63</v>
+      </c>
+      <c r="B19">
+        <v>2</v>
+      </c>
+      <c r="C19" s="21">
+        <v>43703</v>
+      </c>
+      <c r="D19" s="21">
+        <v>43704</v>
+      </c>
+      <c r="E19" s="21">
+        <v>43720</v>
+      </c>
+      <c r="F19" s="21">
+        <v>43721</v>
+      </c>
+      <c r="G19" s="21">
+        <v>43721</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>63</v>
+      </c>
+      <c r="B20">
+        <v>3</v>
+      </c>
+      <c r="C20" s="21">
+        <v>43703</v>
+      </c>
+      <c r="D20" s="21">
+        <v>43704</v>
+      </c>
+      <c r="E20" s="21">
+        <v>43720</v>
+      </c>
+      <c r="F20" s="21">
+        <v>43721</v>
+      </c>
+      <c r="G20" s="21">
+        <v>43721</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>63</v>
+      </c>
+      <c r="B21">
+        <v>4</v>
+      </c>
+      <c r="C21" s="21">
+        <v>43703</v>
+      </c>
+      <c r="D21" s="21">
+        <v>43704</v>
+      </c>
+      <c r="E21" s="21">
+        <v>43720</v>
+      </c>
+      <c r="F21" s="21">
+        <v>43721</v>
+      </c>
+      <c r="G21" s="21">
+        <v>43721</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>64</v>
+      </c>
+      <c r="B22">
+        <v>1</v>
+      </c>
+      <c r="C22" s="21">
+        <v>43703</v>
+      </c>
+      <c r="D22" s="21">
+        <v>43704</v>
+      </c>
+      <c r="E22" s="21">
+        <v>43720</v>
+      </c>
+      <c r="F22" s="21">
+        <v>43721</v>
+      </c>
+      <c r="G22" s="21">
+        <v>43721</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>64</v>
+      </c>
+      <c r="B23">
+        <v>2</v>
+      </c>
+      <c r="C23" s="21">
+        <v>43703</v>
+      </c>
+      <c r="D23" s="21">
+        <v>43704</v>
+      </c>
+      <c r="E23" s="21">
+        <v>43720</v>
+      </c>
+      <c r="F23" s="21">
+        <v>43721</v>
+      </c>
+      <c r="G23" s="21">
+        <v>43721</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>64</v>
+      </c>
+      <c r="B24">
+        <v>3</v>
+      </c>
+      <c r="C24" s="21">
+        <v>43703</v>
+      </c>
+      <c r="D24" s="21">
+        <v>43704</v>
+      </c>
+      <c r="E24" s="21">
+        <v>43720</v>
+      </c>
+      <c r="F24" s="21">
+        <v>43721</v>
+      </c>
+      <c r="G24" s="21">
+        <v>43721</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>64</v>
+      </c>
+      <c r="B25">
+        <v>4</v>
+      </c>
+      <c r="C25" s="21">
+        <v>43703</v>
+      </c>
+      <c r="D25" s="21">
+        <v>43704</v>
+      </c>
+      <c r="E25" s="21">
+        <v>43720</v>
+      </c>
+      <c r="F25" s="21">
+        <v>43721</v>
+      </c>
+      <c r="G25" s="21">
+        <v>43721</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>65</v>
+      </c>
+      <c r="B26">
+        <v>1</v>
+      </c>
+      <c r="C26" s="21">
+        <v>43703</v>
+      </c>
+      <c r="D26" s="21">
+        <v>43704</v>
+      </c>
+      <c r="E26" s="21">
+        <v>43720</v>
+      </c>
+      <c r="F26" s="21">
+        <v>43721</v>
+      </c>
+      <c r="G26" s="21">
+        <v>43721</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>65</v>
+      </c>
+      <c r="B27">
+        <v>2</v>
+      </c>
+      <c r="C27" s="21">
+        <v>43703</v>
+      </c>
+      <c r="D27" s="21">
+        <v>43704</v>
+      </c>
+      <c r="E27" s="21">
+        <v>43720</v>
+      </c>
+      <c r="F27" s="21">
+        <v>43721</v>
+      </c>
+      <c r="G27" s="21">
+        <v>43721</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>65</v>
+      </c>
+      <c r="B28">
+        <v>3</v>
+      </c>
+      <c r="C28" s="21">
+        <v>43703</v>
+      </c>
+      <c r="D28" s="21">
+        <v>43704</v>
+      </c>
+      <c r="E28" s="21">
+        <v>43720</v>
+      </c>
+      <c r="F28" s="21">
+        <v>43721</v>
+      </c>
+      <c r="G28" s="21">
+        <v>43721</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>65</v>
+      </c>
+      <c r="B29">
+        <v>4</v>
+      </c>
+      <c r="C29" s="21">
+        <v>43703</v>
+      </c>
+      <c r="D29" s="21">
+        <v>43704</v>
+      </c>
+      <c r="E29" s="21">
+        <v>43720</v>
+      </c>
+      <c r="F29" s="21">
+        <v>43721</v>
+      </c>
+      <c r="G29" s="21">
+        <v>43721</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>66</v>
+      </c>
+      <c r="B30">
+        <v>1</v>
+      </c>
+      <c r="C30" s="21">
+        <v>43731</v>
+      </c>
+      <c r="D30" s="21">
+        <v>43732</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>66</v>
+      </c>
+      <c r="B31">
+        <v>2</v>
+      </c>
+      <c r="C31" s="21">
+        <v>43731</v>
+      </c>
+      <c r="D31" s="21">
+        <v>43732</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>66</v>
+      </c>
+      <c r="B32">
+        <v>3</v>
+      </c>
+      <c r="C32" s="21">
+        <v>43731</v>
+      </c>
+      <c r="D32" s="21">
+        <v>43732</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>66</v>
+      </c>
+      <c r="B33">
+        <v>4</v>
+      </c>
+      <c r="C33" s="21">
+        <v>43731</v>
+      </c>
+      <c r="D33" s="21">
+        <v>43732</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>67</v>
+      </c>
+      <c r="B34">
+        <v>1</v>
+      </c>
+      <c r="C34" s="21">
+        <v>43731</v>
+      </c>
+      <c r="D34" s="21">
+        <v>43732</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>67</v>
+      </c>
+      <c r="B35">
+        <v>2</v>
+      </c>
+      <c r="C35" s="21">
+        <v>43731</v>
+      </c>
+      <c r="D35" s="21">
+        <v>43732</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>67</v>
+      </c>
+      <c r="B36">
+        <v>3</v>
+      </c>
+      <c r="C36" s="21">
+        <v>43731</v>
+      </c>
+      <c r="D36" s="21">
+        <v>43732</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>67</v>
+      </c>
+      <c r="B37">
+        <v>4</v>
+      </c>
+      <c r="C37" s="21">
+        <v>43731</v>
+      </c>
+      <c r="D37" s="21">
+        <v>43732</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>68</v>
+      </c>
+      <c r="B38">
+        <v>1</v>
+      </c>
+      <c r="C38" s="21">
+        <v>43732</v>
+      </c>
+      <c r="D38" s="21">
+        <v>43733</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>68</v>
+      </c>
+      <c r="B39">
+        <v>2</v>
+      </c>
+      <c r="C39" s="21">
+        <v>43732</v>
+      </c>
+      <c r="D39" s="21">
+        <v>43733</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>68</v>
+      </c>
+      <c r="B40">
+        <v>3</v>
+      </c>
+      <c r="C40" s="21">
+        <v>43732</v>
+      </c>
+      <c r="D40" s="21">
+        <v>43733</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>68</v>
+      </c>
+      <c r="B41">
+        <v>4</v>
+      </c>
+      <c r="C41" s="21">
+        <v>43732</v>
+      </c>
+      <c r="D41" s="21">
+        <v>43733</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>69</v>
+      </c>
+      <c r="B42">
+        <v>1</v>
+      </c>
+      <c r="C42" s="21">
+        <v>43731</v>
+      </c>
+      <c r="D42" s="21">
+        <v>43732</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>69</v>
+      </c>
+      <c r="B43">
+        <v>2</v>
+      </c>
+      <c r="C43" s="21">
+        <v>43731</v>
+      </c>
+      <c r="D43" s="21">
+        <v>43732</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>69</v>
+      </c>
+      <c r="B44">
+        <v>3</v>
+      </c>
+      <c r="C44" s="21">
+        <v>43731</v>
+      </c>
+      <c r="D44" s="21">
+        <v>43732</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>69</v>
+      </c>
+      <c r="B45">
+        <v>4</v>
+      </c>
+      <c r="C45" s="21">
+        <v>43731</v>
+      </c>
+      <c r="D45" s="21">
+        <v>43732</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>70</v>
+      </c>
+      <c r="B46">
+        <v>1</v>
+      </c>
+      <c r="C46" s="21">
+        <v>43731</v>
+      </c>
+      <c r="D46" s="21">
+        <v>43732</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>70</v>
+      </c>
+      <c r="B47">
+        <v>2</v>
+      </c>
+      <c r="C47" s="21">
+        <v>43731</v>
+      </c>
+      <c r="D47" s="21">
+        <v>43732</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>70</v>
+      </c>
+      <c r="B48">
+        <v>3</v>
+      </c>
+      <c r="C48" s="21">
+        <v>43731</v>
+      </c>
+      <c r="D48" s="21">
+        <v>43732</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>70</v>
+      </c>
+      <c r="B49">
+        <v>4</v>
+      </c>
+      <c r="C49" s="21">
+        <v>43731</v>
+      </c>
+      <c r="D49" s="21">
+        <v>43732</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>71</v>
+      </c>
+      <c r="B50">
+        <v>1</v>
+      </c>
+      <c r="C50" s="21">
+        <v>43733</v>
+      </c>
+      <c r="D50" s="21">
+        <v>43734</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>71</v>
+      </c>
+      <c r="B51">
+        <v>2</v>
+      </c>
+      <c r="C51" s="21">
+        <v>43733</v>
+      </c>
+      <c r="D51" s="21">
+        <v>43734</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>71</v>
+      </c>
+      <c r="B52">
+        <v>3</v>
+      </c>
+      <c r="C52" s="21">
+        <v>43733</v>
+      </c>
+      <c r="D52" s="21">
+        <v>43734</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>71</v>
+      </c>
+      <c r="B53">
+        <v>4</v>
+      </c>
+      <c r="C53" s="21">
+        <v>43733</v>
+      </c>
+      <c r="D53" s="21">
+        <v>43734</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>72</v>
+      </c>
+      <c r="B54">
+        <v>1</v>
+      </c>
+      <c r="C54" s="21">
+        <v>43731</v>
+      </c>
+      <c r="D54" s="21">
+        <v>43732</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>72</v>
+      </c>
+      <c r="B55">
+        <v>2</v>
+      </c>
+      <c r="C55" s="21">
+        <v>43731</v>
+      </c>
+      <c r="D55" s="21">
+        <v>43732</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>72</v>
+      </c>
+      <c r="B56">
+        <v>3</v>
+      </c>
+      <c r="C56" s="21">
+        <v>43731</v>
+      </c>
+      <c r="D56" s="21">
+        <v>43732</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>72</v>
+      </c>
+      <c r="B57">
+        <v>4</v>
+      </c>
+      <c r="C57" s="21">
+        <v>43731</v>
+      </c>
+      <c r="D57" s="21">
+        <v>43732</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>73</v>
+      </c>
+      <c r="B58">
+        <v>1</v>
+      </c>
+      <c r="C58" s="21">
+        <v>43733</v>
+      </c>
+      <c r="D58" s="21">
+        <v>43734</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>73</v>
+      </c>
+      <c r="B59">
+        <v>2</v>
+      </c>
+      <c r="C59" s="21">
+        <v>43733</v>
+      </c>
+      <c r="D59" s="21">
+        <v>43734</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>73</v>
+      </c>
+      <c r="B60">
+        <v>3</v>
+      </c>
+      <c r="C60" s="21">
+        <v>43733</v>
+      </c>
+      <c r="D60" s="21">
+        <v>43734</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>73</v>
+      </c>
+      <c r="B61">
+        <v>4</v>
+      </c>
+      <c r="C61" s="21">
+        <v>43733</v>
+      </c>
+      <c r="D61" s="21">
+        <v>43734</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>74</v>
+      </c>
+      <c r="B62">
+        <v>1</v>
+      </c>
+      <c r="C62" s="21">
+        <v>43732</v>
+      </c>
+      <c r="D62" s="21">
+        <v>43733</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>74</v>
+      </c>
+      <c r="B63">
+        <v>2</v>
+      </c>
+      <c r="C63" s="21">
+        <v>43732</v>
+      </c>
+      <c r="D63" s="21">
+        <v>43733</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>74</v>
+      </c>
+      <c r="B64">
+        <v>3</v>
+      </c>
+      <c r="C64" s="21">
+        <v>43732</v>
+      </c>
+      <c r="D64" s="21">
+        <v>43733</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>74</v>
+      </c>
+      <c r="B65">
+        <v>4</v>
+      </c>
+      <c r="C65" s="21">
+        <v>43732</v>
+      </c>
+      <c r="D65" s="21">
+        <v>43733</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
correct small and medium mesh size differences between aug 2019 and jan 2020
</commit_message>
<xml_diff>
--- a/Oyster/cultchmass/cultchmass_packet.xlsx
+++ b/Oyster/cultchmass/cultchmass_packet.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="960" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="962" uniqueCount="84">
   <si>
     <t>DATE (YYYYMMDD):</t>
   </si>
@@ -274,6 +274,9 @@
   </si>
   <si>
     <t>md_rf_kg</t>
+  </si>
+  <si>
+    <t>mass of the weighing bucket plus all reef material retained in the 2.5 x 2.5cm seive in kg.  This excludes the material retained in the 5cm and 10cm seives.</t>
   </si>
 </sst>
 </file>
@@ -1136,8 +1139,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N98"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A81" workbookViewId="0">
-      <selection activeCell="P100" sqref="P100"/>
+    <sheetView tabSelected="1" topLeftCell="A85" workbookViewId="0">
+      <selection activeCell="A99" sqref="A99"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1221,10 +1224,10 @@
         <v>4.53</v>
       </c>
       <c r="K2">
-        <v>-999</v>
+        <v>2.15</v>
       </c>
       <c r="L2">
-        <v>2.15</v>
+        <v>-999</v>
       </c>
       <c r="M2" t="s">
         <v>47</v>
@@ -1265,10 +1268,10 @@
         <v>4.99</v>
       </c>
       <c r="K3">
-        <v>-999</v>
+        <v>2.4900000000000002</v>
       </c>
       <c r="L3">
-        <v>2.4900000000000002</v>
+        <v>-999</v>
       </c>
       <c r="M3" t="s">
         <v>47</v>
@@ -1309,10 +1312,10 @@
         <v>2.38</v>
       </c>
       <c r="K4">
-        <v>-999</v>
+        <v>7.03</v>
       </c>
       <c r="L4">
-        <v>7.03</v>
+        <v>-999</v>
       </c>
       <c r="M4" t="s">
         <v>47</v>
@@ -1353,10 +1356,10 @@
         <v>0.86</v>
       </c>
       <c r="K5">
-        <v>-999</v>
+        <v>1.25</v>
       </c>
       <c r="L5">
-        <v>1.25</v>
+        <v>-999</v>
       </c>
       <c r="M5" t="s">
         <v>47</v>
@@ -1397,10 +1400,10 @@
         <v>1.84</v>
       </c>
       <c r="K6">
-        <v>-999</v>
+        <v>1.22</v>
       </c>
       <c r="L6">
-        <v>1.22</v>
+        <v>-999</v>
       </c>
       <c r="M6" t="s">
         <v>47</v>
@@ -1441,10 +1444,10 @@
         <v>2.86</v>
       </c>
       <c r="K7">
-        <v>-999</v>
+        <v>1.6</v>
       </c>
       <c r="L7">
-        <v>1.6</v>
+        <v>-999</v>
       </c>
       <c r="M7" t="s">
         <v>47</v>
@@ -1485,10 +1488,10 @@
         <v>2.2599999999999998</v>
       </c>
       <c r="K8">
-        <v>-999</v>
+        <v>0.96</v>
       </c>
       <c r="L8">
-        <v>0.96</v>
+        <v>-999</v>
       </c>
       <c r="M8" t="s">
         <v>47</v>
@@ -1529,10 +1532,10 @@
         <v>1.36</v>
       </c>
       <c r="K9">
-        <v>-999</v>
+        <v>0.86</v>
       </c>
       <c r="L9">
-        <v>0.86</v>
+        <v>-999</v>
       </c>
       <c r="M9" t="s">
         <v>47</v>
@@ -1573,10 +1576,10 @@
         <v>2.4900000000000002</v>
       </c>
       <c r="K10">
-        <v>-999</v>
+        <v>2.15</v>
       </c>
       <c r="L10">
-        <v>2.15</v>
+        <v>-999</v>
       </c>
       <c r="M10" t="s">
         <v>47</v>
@@ -1617,10 +1620,10 @@
         <v>1.59</v>
       </c>
       <c r="K11">
-        <v>-999</v>
+        <v>0.86</v>
       </c>
       <c r="L11">
-        <v>0.86</v>
+        <v>-999</v>
       </c>
       <c r="M11" t="s">
         <v>47</v>
@@ -1661,10 +1664,10 @@
         <v>0.86</v>
       </c>
       <c r="K12">
-        <v>-999</v>
+        <v>0.86</v>
       </c>
       <c r="L12">
-        <v>0.86</v>
+        <v>-999</v>
       </c>
       <c r="M12" t="s">
         <v>47</v>
@@ -1705,10 +1708,10 @@
         <v>4.08</v>
       </c>
       <c r="K13">
-        <v>-999</v>
+        <v>0.86</v>
       </c>
       <c r="L13">
-        <v>0.86</v>
+        <v>-999</v>
       </c>
       <c r="M13" t="s">
         <v>47</v>
@@ -1749,10 +1752,10 @@
         <v>0.86</v>
       </c>
       <c r="K14">
-        <v>-999</v>
+        <v>1.06</v>
       </c>
       <c r="L14">
-        <v>1.06</v>
+        <v>-999</v>
       </c>
       <c r="M14" t="s">
         <v>47</v>
@@ -1793,10 +1796,10 @@
         <v>0.86</v>
       </c>
       <c r="K15">
-        <v>-999</v>
+        <v>1.08</v>
       </c>
       <c r="L15">
-        <v>1.08</v>
+        <v>-999</v>
       </c>
       <c r="M15" t="s">
         <v>47</v>
@@ -1837,10 +1840,10 @@
         <v>0.86</v>
       </c>
       <c r="K16">
-        <v>-999</v>
+        <v>1.06</v>
       </c>
       <c r="L16">
-        <v>1.06</v>
+        <v>-999</v>
       </c>
       <c r="M16" t="s">
         <v>47</v>
@@ -1881,10 +1884,10 @@
         <v>0.86</v>
       </c>
       <c r="K17">
-        <v>-999</v>
+        <v>1.86</v>
       </c>
       <c r="L17">
-        <v>1.86</v>
+        <v>-999</v>
       </c>
       <c r="M17" t="s">
         <v>47</v>
@@ -1925,10 +1928,10 @@
         <v>2.9</v>
       </c>
       <c r="K18">
-        <v>-999</v>
+        <v>2.8</v>
       </c>
       <c r="L18">
-        <v>2.8</v>
+        <v>-999</v>
       </c>
       <c r="M18" t="s">
         <v>72</v>
@@ -1969,10 +1972,10 @@
         <v>2.7</v>
       </c>
       <c r="K19">
-        <v>-999</v>
+        <v>3</v>
       </c>
       <c r="L19">
-        <v>3</v>
+        <v>-999</v>
       </c>
       <c r="M19" t="s">
         <v>72</v>
@@ -2013,10 +2016,10 @@
         <v>0.8</v>
       </c>
       <c r="K20">
-        <v>-999</v>
+        <v>0.9</v>
       </c>
       <c r="L20">
-        <v>0.9</v>
+        <v>-999</v>
       </c>
       <c r="M20" t="s">
         <v>72</v>
@@ -2057,10 +2060,10 @@
         <v>0.8</v>
       </c>
       <c r="K21">
-        <v>-999</v>
+        <v>1.4</v>
       </c>
       <c r="L21">
-        <v>1.4</v>
+        <v>-999</v>
       </c>
       <c r="M21" t="s">
         <v>72</v>
@@ -2101,10 +2104,10 @@
         <v>2.8</v>
       </c>
       <c r="K22">
-        <v>-999</v>
+        <v>5.2</v>
       </c>
       <c r="L22">
-        <v>5.2</v>
+        <v>-999</v>
       </c>
       <c r="M22" t="s">
         <v>72</v>
@@ -2145,10 +2148,10 @@
         <v>1.2</v>
       </c>
       <c r="K23">
-        <v>-999</v>
+        <v>5.6</v>
       </c>
       <c r="L23">
-        <v>5.6</v>
+        <v>-999</v>
       </c>
       <c r="M23" t="s">
         <v>72</v>
@@ -2189,10 +2192,10 @@
         <v>2.5</v>
       </c>
       <c r="K24">
-        <v>-999</v>
+        <v>4.8</v>
       </c>
       <c r="L24">
-        <v>4.8</v>
+        <v>-999</v>
       </c>
       <c r="M24" t="s">
         <v>72</v>
@@ -2233,10 +2236,10 @@
         <v>2.4</v>
       </c>
       <c r="K25">
-        <v>-999</v>
+        <v>4.5</v>
       </c>
       <c r="L25">
-        <v>4.5</v>
+        <v>-999</v>
       </c>
       <c r="M25" t="s">
         <v>72</v>
@@ -2277,10 +2280,10 @@
         <v>0.8</v>
       </c>
       <c r="K26">
-        <v>-999</v>
+        <v>1</v>
       </c>
       <c r="L26">
-        <v>1</v>
+        <v>-999</v>
       </c>
       <c r="M26" t="s">
         <v>72</v>
@@ -2321,10 +2324,10 @@
         <v>0.8</v>
       </c>
       <c r="K27">
-        <v>-999</v>
+        <v>1.7</v>
       </c>
       <c r="L27">
-        <v>1.7</v>
+        <v>-999</v>
       </c>
       <c r="M27" t="s">
         <v>72</v>
@@ -2365,10 +2368,10 @@
         <v>0.8</v>
       </c>
       <c r="K28">
-        <v>-999</v>
+        <v>0.8</v>
       </c>
       <c r="L28">
-        <v>0.8</v>
+        <v>-999</v>
       </c>
       <c r="M28" t="s">
         <v>72</v>
@@ -2409,10 +2412,10 @@
         <v>0.8</v>
       </c>
       <c r="K29">
-        <v>-999</v>
+        <v>1.7</v>
       </c>
       <c r="L29">
-        <v>1.7</v>
+        <v>-999</v>
       </c>
       <c r="M29" t="s">
         <v>72</v>
@@ -2453,10 +2456,10 @@
         <v>0.8</v>
       </c>
       <c r="K30">
-        <v>-999</v>
+        <v>2.4</v>
       </c>
       <c r="L30">
-        <v>2.4</v>
+        <v>-999</v>
       </c>
       <c r="M30" t="s">
         <v>72</v>
@@ -2497,10 +2500,10 @@
         <v>0.8</v>
       </c>
       <c r="K31">
-        <v>-999</v>
+        <v>1</v>
       </c>
       <c r="L31">
-        <v>1</v>
+        <v>-999</v>
       </c>
       <c r="M31" t="s">
         <v>72</v>
@@ -2541,10 +2544,10 @@
         <v>0.8</v>
       </c>
       <c r="K32">
-        <v>-999</v>
+        <v>0.9</v>
       </c>
       <c r="L32">
-        <v>0.9</v>
+        <v>-999</v>
       </c>
       <c r="M32" t="s">
         <v>72</v>
@@ -2585,10 +2588,10 @@
         <v>0.8</v>
       </c>
       <c r="K33">
-        <v>-999</v>
+        <v>0.9</v>
       </c>
       <c r="L33">
-        <v>0.9</v>
+        <v>-999</v>
       </c>
       <c r="M33" t="s">
         <v>72</v>
@@ -2629,10 +2632,10 @@
         <v>1.7</v>
       </c>
       <c r="K34">
-        <v>-999</v>
+        <v>1.4</v>
       </c>
       <c r="L34">
-        <v>1.4</v>
+        <v>-999</v>
       </c>
       <c r="M34" t="s">
         <v>72</v>
@@ -2673,10 +2676,10 @@
         <v>9.4</v>
       </c>
       <c r="K35">
-        <v>-999</v>
+        <v>2.4</v>
       </c>
       <c r="L35">
-        <v>2.4</v>
+        <v>-999</v>
       </c>
       <c r="M35" t="s">
         <v>72</v>
@@ -2717,10 +2720,10 @@
         <v>9</v>
       </c>
       <c r="K36">
-        <v>-999</v>
+        <v>2.2999999999999998</v>
       </c>
       <c r="L36">
-        <v>2.2999999999999998</v>
+        <v>-999</v>
       </c>
       <c r="M36" t="s">
         <v>72</v>
@@ -2761,10 +2764,10 @@
         <v>4.9000000000000004</v>
       </c>
       <c r="K37">
-        <v>-999</v>
+        <v>1.4</v>
       </c>
       <c r="L37">
-        <v>1.4</v>
+        <v>-999</v>
       </c>
       <c r="M37" t="s">
         <v>72</v>
@@ -2805,10 +2808,10 @@
         <v>1.3</v>
       </c>
       <c r="K38">
-        <v>-999</v>
+        <v>4.4000000000000004</v>
       </c>
       <c r="L38">
-        <v>4.4000000000000004</v>
+        <v>-999</v>
       </c>
       <c r="M38" t="s">
         <v>73</v>
@@ -2849,10 +2852,10 @@
         <v>0.8</v>
       </c>
       <c r="K39">
-        <v>-999</v>
+        <v>1.9</v>
       </c>
       <c r="L39">
-        <v>1.9</v>
+        <v>-999</v>
       </c>
       <c r="M39" t="s">
         <v>73</v>
@@ -2893,10 +2896,10 @@
         <v>2.7</v>
       </c>
       <c r="K40">
-        <v>-999</v>
+        <v>3.4</v>
       </c>
       <c r="L40">
-        <v>3.4</v>
+        <v>-999</v>
       </c>
       <c r="M40" t="s">
         <v>73</v>
@@ -2937,10 +2940,10 @@
         <v>2.4</v>
       </c>
       <c r="K41">
-        <v>-999</v>
+        <v>5.2</v>
       </c>
       <c r="L41">
-        <v>5.2</v>
+        <v>-999</v>
       </c>
       <c r="M41" t="s">
         <v>73</v>
@@ -2981,10 +2984,10 @@
         <v>6.1</v>
       </c>
       <c r="K42">
-        <v>-999</v>
+        <v>3.5</v>
       </c>
       <c r="L42">
-        <v>3.5</v>
+        <v>-999</v>
       </c>
       <c r="M42" t="s">
         <v>73</v>
@@ -3025,10 +3028,10 @@
         <v>0.8</v>
       </c>
       <c r="K43">
-        <v>-999</v>
+        <v>0.9</v>
       </c>
       <c r="L43">
-        <v>0.9</v>
+        <v>-999</v>
       </c>
       <c r="M43" t="s">
         <v>73</v>
@@ -3069,10 +3072,10 @@
         <v>1.3</v>
       </c>
       <c r="K44">
-        <v>-999</v>
+        <v>0.9</v>
       </c>
       <c r="L44">
-        <v>0.9</v>
+        <v>-999</v>
       </c>
       <c r="M44" t="s">
         <v>73</v>
@@ -3113,10 +3116,10 @@
         <v>1.9</v>
       </c>
       <c r="K45">
-        <v>-999</v>
+        <v>2</v>
       </c>
       <c r="L45">
-        <v>2</v>
+        <v>-999</v>
       </c>
       <c r="M45" t="s">
         <v>73</v>
@@ -3157,10 +3160,10 @@
         <v>0.8</v>
       </c>
       <c r="K46">
-        <v>-999</v>
+        <v>0.8</v>
       </c>
       <c r="L46">
-        <v>0.8</v>
+        <v>-999</v>
       </c>
       <c r="M46" t="s">
         <v>73</v>
@@ -3201,10 +3204,10 @@
         <v>0.8</v>
       </c>
       <c r="K47">
-        <v>-999</v>
+        <v>0.9</v>
       </c>
       <c r="L47">
-        <v>0.9</v>
+        <v>-999</v>
       </c>
       <c r="M47" t="s">
         <v>73</v>
@@ -3245,10 +3248,10 @@
         <v>0.8</v>
       </c>
       <c r="K48">
-        <v>-999</v>
+        <v>0.9</v>
       </c>
       <c r="L48">
-        <v>0.9</v>
+        <v>-999</v>
       </c>
       <c r="M48" t="s">
         <v>73</v>
@@ -3289,10 +3292,10 @@
         <v>0.8</v>
       </c>
       <c r="K49">
-        <v>-999</v>
+        <v>0.8</v>
       </c>
       <c r="L49">
-        <v>0.8</v>
+        <v>-999</v>
       </c>
       <c r="M49" t="s">
         <v>73</v>
@@ -3333,10 +3336,10 @@
         <v>5.3</v>
       </c>
       <c r="K50">
-        <v>-999</v>
+        <v>3.3</v>
       </c>
       <c r="L50">
-        <v>3.3</v>
+        <v>-999</v>
       </c>
       <c r="M50" t="s">
         <v>73</v>
@@ -3377,10 +3380,10 @@
         <v>1.9</v>
       </c>
       <c r="K51">
-        <v>-999</v>
+        <v>3</v>
       </c>
       <c r="L51">
-        <v>3</v>
+        <v>-999</v>
       </c>
       <c r="M51" t="s">
         <v>73</v>
@@ -3421,10 +3424,10 @@
         <v>0.8</v>
       </c>
       <c r="K52">
-        <v>-999</v>
+        <v>1</v>
       </c>
       <c r="L52">
-        <v>1</v>
+        <v>-999</v>
       </c>
       <c r="M52" t="s">
         <v>73</v>
@@ -3465,10 +3468,10 @@
         <v>0.8</v>
       </c>
       <c r="K53">
-        <v>-999</v>
+        <v>3.3</v>
       </c>
       <c r="L53">
-        <v>3.3</v>
+        <v>-999</v>
       </c>
       <c r="M53" t="s">
         <v>73</v>
@@ -3509,10 +3512,10 @@
         <v>2</v>
       </c>
       <c r="K54">
-        <v>-999</v>
+        <v>1</v>
       </c>
       <c r="L54">
-        <v>1</v>
+        <v>-999</v>
       </c>
       <c r="M54" t="s">
         <v>74</v>
@@ -3553,10 +3556,10 @@
         <v>2.9</v>
       </c>
       <c r="K55">
-        <v>-999</v>
+        <v>3.5</v>
       </c>
       <c r="L55">
-        <v>3.5</v>
+        <v>-999</v>
       </c>
       <c r="M55" t="s">
         <v>74</v>
@@ -3597,10 +3600,10 @@
         <v>4.5</v>
       </c>
       <c r="K56">
-        <v>-999</v>
+        <v>4.4000000000000004</v>
       </c>
       <c r="L56">
-        <v>4.4000000000000004</v>
+        <v>-999</v>
       </c>
       <c r="M56" t="s">
         <v>74</v>
@@ -3641,10 +3644,10 @@
         <v>5.5</v>
       </c>
       <c r="K57">
-        <v>-999</v>
+        <v>3.4</v>
       </c>
       <c r="L57">
-        <v>3.4</v>
+        <v>-999</v>
       </c>
       <c r="M57" t="s">
         <v>74</v>
@@ -3685,10 +3688,10 @@
         <v>0.8</v>
       </c>
       <c r="K58">
-        <v>-999</v>
+        <v>1.6</v>
       </c>
       <c r="L58">
-        <v>1.6</v>
+        <v>-999</v>
       </c>
       <c r="M58" t="s">
         <v>74</v>
@@ -3729,10 +3732,10 @@
         <v>0.8</v>
       </c>
       <c r="K59">
-        <v>-999</v>
+        <v>1.4</v>
       </c>
       <c r="L59">
-        <v>1.4</v>
+        <v>-999</v>
       </c>
       <c r="M59" t="s">
         <v>74</v>
@@ -3773,10 +3776,10 @@
         <v>0.8</v>
       </c>
       <c r="K60">
-        <v>-999</v>
+        <v>1.4</v>
       </c>
       <c r="L60">
-        <v>1.4</v>
+        <v>-999</v>
       </c>
       <c r="M60" t="s">
         <v>74</v>
@@ -3817,10 +3820,10 @@
         <v>1.6</v>
       </c>
       <c r="K61">
-        <v>-999</v>
+        <v>1</v>
       </c>
       <c r="L61">
-        <v>1</v>
+        <v>-999</v>
       </c>
       <c r="M61" t="s">
         <v>74</v>
@@ -3861,10 +3864,10 @@
         <v>2.1</v>
       </c>
       <c r="K62">
-        <v>-999</v>
+        <v>0.8</v>
       </c>
       <c r="L62">
-        <v>0.8</v>
+        <v>-999</v>
       </c>
       <c r="M62" t="s">
         <v>74</v>
@@ -3905,10 +3908,10 @@
         <v>0.8</v>
       </c>
       <c r="K63">
-        <v>-999</v>
+        <v>1.4</v>
       </c>
       <c r="L63">
-        <v>1.4</v>
+        <v>-999</v>
       </c>
       <c r="M63" t="s">
         <v>74</v>
@@ -3949,10 +3952,10 @@
         <v>0.8</v>
       </c>
       <c r="K64">
-        <v>-999</v>
+        <v>1.4</v>
       </c>
       <c r="L64">
-        <v>1.4</v>
+        <v>-999</v>
       </c>
       <c r="M64" t="s">
         <v>74</v>
@@ -3993,10 +3996,10 @@
         <v>5</v>
       </c>
       <c r="K65">
-        <v>-999</v>
+        <v>2.9</v>
       </c>
       <c r="L65">
-        <v>2.9</v>
+        <v>-999</v>
       </c>
       <c r="M65" t="s">
         <v>74</v>
@@ -5516,19 +5519,19 @@
           <x14:formula1>
             <xm:f>pick!$L$2:$L$12</xm:f>
           </x14:formula1>
-          <xm:sqref>M1:M17 M66:M1048576</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
-          <x14:formula1>
-            <xm:f>pick!$M$2:$M$16</xm:f>
-          </x14:formula1>
-          <xm:sqref>N1:N1048576</xm:sqref>
+          <xm:sqref>M66:M1048576 M2:M17 M1</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>pick!$L$2:$L$16</xm:f>
           </x14:formula1>
           <xm:sqref>M18:M65</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>pick!$M$2:$M$16</xm:f>
+          </x14:formula1>
+          <xm:sqref>N66:N1048576 N1 N2:N65</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -10027,7 +10030,7 @@
         <v/>
       </c>
       <c r="K2" t="str">
-        <f>IF(raw_data_1!L2=raw_data_2!L2,"","check")</f>
+        <f>IF(raw_data_1!K2=raw_data_2!L2,"","check")</f>
         <v/>
       </c>
       <c r="L2" t="str">
@@ -10081,7 +10084,7 @@
         <v/>
       </c>
       <c r="K3" t="str">
-        <f>IF(raw_data_1!L3=raw_data_2!L3,"","check")</f>
+        <f>IF(raw_data_1!K3=raw_data_2!L3,"","check")</f>
         <v/>
       </c>
       <c r="L3" t="str">
@@ -10135,7 +10138,7 @@
         <v/>
       </c>
       <c r="K4" t="str">
-        <f>IF(raw_data_1!L4=raw_data_2!L4,"","check")</f>
+        <f>IF(raw_data_1!K4=raw_data_2!L4,"","check")</f>
         <v/>
       </c>
       <c r="L4" t="str">
@@ -10189,7 +10192,7 @@
         <v/>
       </c>
       <c r="K5" t="str">
-        <f>IF(raw_data_1!L5=raw_data_2!L5,"","check")</f>
+        <f>IF(raw_data_1!K5=raw_data_2!L5,"","check")</f>
         <v/>
       </c>
       <c r="L5" t="str">
@@ -10243,7 +10246,7 @@
         <v/>
       </c>
       <c r="K6" t="str">
-        <f>IF(raw_data_1!L6=raw_data_2!L6,"","check")</f>
+        <f>IF(raw_data_1!K6=raw_data_2!L6,"","check")</f>
         <v/>
       </c>
       <c r="L6" t="str">
@@ -10297,7 +10300,7 @@
         <v/>
       </c>
       <c r="K7" t="str">
-        <f>IF(raw_data_1!L7=raw_data_2!L7,"","check")</f>
+        <f>IF(raw_data_1!K7=raw_data_2!L7,"","check")</f>
         <v/>
       </c>
       <c r="L7" t="str">
@@ -10351,7 +10354,7 @@
         <v/>
       </c>
       <c r="K8" t="str">
-        <f>IF(raw_data_1!L8=raw_data_2!L8,"","check")</f>
+        <f>IF(raw_data_1!K8=raw_data_2!L8,"","check")</f>
         <v/>
       </c>
       <c r="L8" t="str">
@@ -10405,7 +10408,7 @@
         <v/>
       </c>
       <c r="K9" t="str">
-        <f>IF(raw_data_1!L9=raw_data_2!L9,"","check")</f>
+        <f>IF(raw_data_1!K9=raw_data_2!L9,"","check")</f>
         <v/>
       </c>
       <c r="L9" t="str">
@@ -10459,7 +10462,7 @@
         <v/>
       </c>
       <c r="K10" t="str">
-        <f>IF(raw_data_1!L10=raw_data_2!L10,"","check")</f>
+        <f>IF(raw_data_1!K10=raw_data_2!L10,"","check")</f>
         <v/>
       </c>
       <c r="L10" t="str">
@@ -10513,7 +10516,7 @@
         <v/>
       </c>
       <c r="K11" t="str">
-        <f>IF(raw_data_1!L11=raw_data_2!L11,"","check")</f>
+        <f>IF(raw_data_1!K11=raw_data_2!L11,"","check")</f>
         <v/>
       </c>
       <c r="L11" t="str">
@@ -10567,7 +10570,7 @@
         <v/>
       </c>
       <c r="K12" t="str">
-        <f>IF(raw_data_1!L12=raw_data_2!L12,"","check")</f>
+        <f>IF(raw_data_1!K12=raw_data_2!L12,"","check")</f>
         <v/>
       </c>
       <c r="L12" t="str">
@@ -10621,7 +10624,7 @@
         <v/>
       </c>
       <c r="K13" t="str">
-        <f>IF(raw_data_1!L13=raw_data_2!L13,"","check")</f>
+        <f>IF(raw_data_1!K13=raw_data_2!L13,"","check")</f>
         <v/>
       </c>
       <c r="L13" t="str">
@@ -10675,7 +10678,7 @@
         <v/>
       </c>
       <c r="K14" t="str">
-        <f>IF(raw_data_1!L14=raw_data_2!L14,"","check")</f>
+        <f>IF(raw_data_1!K14=raw_data_2!L14,"","check")</f>
         <v/>
       </c>
       <c r="L14" t="str">
@@ -10729,7 +10732,7 @@
         <v/>
       </c>
       <c r="K15" t="str">
-        <f>IF(raw_data_1!L15=raw_data_2!L15,"","check")</f>
+        <f>IF(raw_data_1!K15=raw_data_2!L15,"","check")</f>
         <v/>
       </c>
       <c r="L15" t="str">
@@ -10783,7 +10786,7 @@
         <v/>
       </c>
       <c r="K16" t="str">
-        <f>IF(raw_data_1!L16=raw_data_2!L16,"","check")</f>
+        <f>IF(raw_data_1!K16=raw_data_2!L16,"","check")</f>
         <v/>
       </c>
       <c r="L16" t="str">
@@ -10837,7 +10840,7 @@
         <v/>
       </c>
       <c r="K17" t="str">
-        <f>IF(raw_data_1!L17=raw_data_2!L17,"","check")</f>
+        <f>IF(raw_data_1!K17=raw_data_2!L17,"","check")</f>
         <v/>
       </c>
       <c r="L17" t="str">
@@ -10891,7 +10894,7 @@
         <v/>
       </c>
       <c r="K18" t="str">
-        <f>IF(raw_data_1!L18=raw_data_2!L18,"","check")</f>
+        <f>IF(raw_data_1!K18=raw_data_2!L18,"","check")</f>
         <v/>
       </c>
       <c r="L18" t="str">
@@ -10945,7 +10948,7 @@
         <v/>
       </c>
       <c r="K19" t="str">
-        <f>IF(raw_data_1!L19=raw_data_2!L19,"","check")</f>
+        <f>IF(raw_data_1!K19=raw_data_2!L19,"","check")</f>
         <v/>
       </c>
       <c r="L19" t="str">
@@ -10999,7 +11002,7 @@
         <v/>
       </c>
       <c r="K20" t="str">
-        <f>IF(raw_data_1!L20=raw_data_2!L20,"","check")</f>
+        <f>IF(raw_data_1!K20=raw_data_2!L20,"","check")</f>
         <v/>
       </c>
       <c r="L20" t="str">
@@ -11053,7 +11056,7 @@
         <v/>
       </c>
       <c r="K21" t="str">
-        <f>IF(raw_data_1!L21=raw_data_2!L21,"","check")</f>
+        <f>IF(raw_data_1!K21=raw_data_2!L21,"","check")</f>
         <v/>
       </c>
       <c r="L21" t="str">
@@ -11107,7 +11110,7 @@
         <v/>
       </c>
       <c r="K22" t="str">
-        <f>IF(raw_data_1!L22=raw_data_2!L22,"","check")</f>
+        <f>IF(raw_data_1!K22=raw_data_2!L22,"","check")</f>
         <v/>
       </c>
       <c r="L22" t="str">
@@ -11161,7 +11164,7 @@
         <v/>
       </c>
       <c r="K23" t="str">
-        <f>IF(raw_data_1!L23=raw_data_2!L23,"","check")</f>
+        <f>IF(raw_data_1!K23=raw_data_2!L23,"","check")</f>
         <v/>
       </c>
       <c r="L23" t="str">
@@ -11215,7 +11218,7 @@
         <v/>
       </c>
       <c r="K24" t="str">
-        <f>IF(raw_data_1!L24=raw_data_2!L24,"","check")</f>
+        <f>IF(raw_data_1!K24=raw_data_2!L24,"","check")</f>
         <v/>
       </c>
       <c r="L24" t="str">
@@ -11269,7 +11272,7 @@
         <v/>
       </c>
       <c r="K25" t="str">
-        <f>IF(raw_data_1!L25=raw_data_2!L25,"","check")</f>
+        <f>IF(raw_data_1!K25=raw_data_2!L25,"","check")</f>
         <v/>
       </c>
       <c r="L25" t="str">
@@ -11323,7 +11326,7 @@
         <v/>
       </c>
       <c r="K26" t="str">
-        <f>IF(raw_data_1!L26=raw_data_2!L26,"","check")</f>
+        <f>IF(raw_data_1!K26=raw_data_2!L26,"","check")</f>
         <v/>
       </c>
       <c r="L26" t="str">
@@ -11377,7 +11380,7 @@
         <v/>
       </c>
       <c r="K27" t="str">
-        <f>IF(raw_data_1!L27=raw_data_2!L27,"","check")</f>
+        <f>IF(raw_data_1!K27=raw_data_2!L27,"","check")</f>
         <v/>
       </c>
       <c r="L27" t="str">
@@ -11431,7 +11434,7 @@
         <v/>
       </c>
       <c r="K28" t="str">
-        <f>IF(raw_data_1!L28=raw_data_2!L28,"","check")</f>
+        <f>IF(raw_data_1!K28=raw_data_2!L28,"","check")</f>
         <v/>
       </c>
       <c r="L28" t="str">
@@ -11485,7 +11488,7 @@
         <v/>
       </c>
       <c r="K29" t="str">
-        <f>IF(raw_data_1!L29=raw_data_2!L29,"","check")</f>
+        <f>IF(raw_data_1!K29=raw_data_2!L29,"","check")</f>
         <v/>
       </c>
       <c r="L29" t="str">
@@ -11539,7 +11542,7 @@
         <v/>
       </c>
       <c r="K30" t="str">
-        <f>IF(raw_data_1!L30=raw_data_2!L30,"","check")</f>
+        <f>IF(raw_data_1!K30=raw_data_2!L30,"","check")</f>
         <v/>
       </c>
       <c r="L30" t="str">
@@ -11593,7 +11596,7 @@
         <v/>
       </c>
       <c r="K31" t="str">
-        <f>IF(raw_data_1!L31=raw_data_2!L31,"","check")</f>
+        <f>IF(raw_data_1!K31=raw_data_2!L31,"","check")</f>
         <v/>
       </c>
       <c r="L31" t="str">
@@ -11647,7 +11650,7 @@
         <v/>
       </c>
       <c r="K32" t="str">
-        <f>IF(raw_data_1!L32=raw_data_2!L32,"","check")</f>
+        <f>IF(raw_data_1!K32=raw_data_2!L32,"","check")</f>
         <v/>
       </c>
       <c r="L32" t="str">
@@ -11701,7 +11704,7 @@
         <v/>
       </c>
       <c r="K33" t="str">
-        <f>IF(raw_data_1!L33=raw_data_2!L33,"","check")</f>
+        <f>IF(raw_data_1!K33=raw_data_2!L33,"","check")</f>
         <v/>
       </c>
       <c r="L33" t="str">
@@ -11755,7 +11758,7 @@
         <v/>
       </c>
       <c r="K34" t="str">
-        <f>IF(raw_data_1!L34=raw_data_2!L34,"","check")</f>
+        <f>IF(raw_data_1!K34=raw_data_2!L34,"","check")</f>
         <v/>
       </c>
       <c r="L34" t="str">
@@ -11809,7 +11812,7 @@
         <v/>
       </c>
       <c r="K35" t="str">
-        <f>IF(raw_data_1!L35=raw_data_2!L35,"","check")</f>
+        <f>IF(raw_data_1!K35=raw_data_2!L35,"","check")</f>
         <v/>
       </c>
       <c r="L35" t="str">
@@ -11863,7 +11866,7 @@
         <v/>
       </c>
       <c r="K36" t="str">
-        <f>IF(raw_data_1!L36=raw_data_2!L36,"","check")</f>
+        <f>IF(raw_data_1!K36=raw_data_2!L36,"","check")</f>
         <v/>
       </c>
       <c r="L36" t="str">
@@ -11917,7 +11920,7 @@
         <v/>
       </c>
       <c r="K37" t="str">
-        <f>IF(raw_data_1!L37=raw_data_2!L37,"","check")</f>
+        <f>IF(raw_data_1!K37=raw_data_2!L37,"","check")</f>
         <v/>
       </c>
       <c r="L37" t="str">
@@ -11971,7 +11974,7 @@
         <v/>
       </c>
       <c r="K38" t="str">
-        <f>IF(raw_data_1!L38=raw_data_2!L38,"","check")</f>
+        <f>IF(raw_data_1!K38=raw_data_2!L38,"","check")</f>
         <v/>
       </c>
       <c r="L38" t="str">
@@ -12025,7 +12028,7 @@
         <v/>
       </c>
       <c r="K39" t="str">
-        <f>IF(raw_data_1!L39=raw_data_2!L39,"","check")</f>
+        <f>IF(raw_data_1!K39=raw_data_2!L39,"","check")</f>
         <v/>
       </c>
       <c r="L39" t="str">
@@ -12079,7 +12082,7 @@
         <v/>
       </c>
       <c r="K40" t="str">
-        <f>IF(raw_data_1!L40=raw_data_2!L40,"","check")</f>
+        <f>IF(raw_data_1!K40=raw_data_2!L40,"","check")</f>
         <v/>
       </c>
       <c r="L40" t="str">
@@ -12133,7 +12136,7 @@
         <v/>
       </c>
       <c r="K41" t="str">
-        <f>IF(raw_data_1!L41=raw_data_2!L41,"","check")</f>
+        <f>IF(raw_data_1!K41=raw_data_2!L41,"","check")</f>
         <v/>
       </c>
       <c r="L41" t="str">
@@ -12187,7 +12190,7 @@
         <v/>
       </c>
       <c r="K42" t="str">
-        <f>IF(raw_data_1!L42=raw_data_2!L42,"","check")</f>
+        <f>IF(raw_data_1!K42=raw_data_2!L42,"","check")</f>
         <v/>
       </c>
       <c r="L42" t="str">
@@ -12241,7 +12244,7 @@
         <v/>
       </c>
       <c r="K43" t="str">
-        <f>IF(raw_data_1!L43=raw_data_2!L43,"","check")</f>
+        <f>IF(raw_data_1!K43=raw_data_2!L43,"","check")</f>
         <v/>
       </c>
       <c r="L43" t="str">
@@ -12295,7 +12298,7 @@
         <v/>
       </c>
       <c r="K44" t="str">
-        <f>IF(raw_data_1!L44=raw_data_2!L44,"","check")</f>
+        <f>IF(raw_data_1!K44=raw_data_2!L44,"","check")</f>
         <v/>
       </c>
       <c r="L44" t="str">
@@ -12349,7 +12352,7 @@
         <v/>
       </c>
       <c r="K45" t="str">
-        <f>IF(raw_data_1!L45=raw_data_2!L45,"","check")</f>
+        <f>IF(raw_data_1!K45=raw_data_2!L45,"","check")</f>
         <v/>
       </c>
       <c r="L45" t="str">
@@ -12403,7 +12406,7 @@
         <v/>
       </c>
       <c r="K46" t="str">
-        <f>IF(raw_data_1!L46=raw_data_2!L46,"","check")</f>
+        <f>IF(raw_data_1!K46=raw_data_2!L46,"","check")</f>
         <v/>
       </c>
       <c r="L46" t="str">
@@ -12457,7 +12460,7 @@
         <v/>
       </c>
       <c r="K47" t="str">
-        <f>IF(raw_data_1!L47=raw_data_2!L47,"","check")</f>
+        <f>IF(raw_data_1!K47=raw_data_2!L47,"","check")</f>
         <v/>
       </c>
       <c r="L47" t="str">
@@ -12511,7 +12514,7 @@
         <v/>
       </c>
       <c r="K48" t="str">
-        <f>IF(raw_data_1!L48=raw_data_2!L48,"","check")</f>
+        <f>IF(raw_data_1!K48=raw_data_2!L48,"","check")</f>
         <v/>
       </c>
       <c r="L48" t="str">
@@ -12565,7 +12568,7 @@
         <v/>
       </c>
       <c r="K49" t="str">
-        <f>IF(raw_data_1!L49=raw_data_2!L49,"","check")</f>
+        <f>IF(raw_data_1!K49=raw_data_2!L49,"","check")</f>
         <v/>
       </c>
       <c r="L49" t="str">
@@ -12619,7 +12622,7 @@
         <v/>
       </c>
       <c r="K50" t="str">
-        <f>IF(raw_data_1!L50=raw_data_2!L50,"","check")</f>
+        <f>IF(raw_data_1!K50=raw_data_2!L50,"","check")</f>
         <v/>
       </c>
       <c r="L50" t="str">
@@ -12673,7 +12676,7 @@
         <v/>
       </c>
       <c r="K51" t="str">
-        <f>IF(raw_data_1!L51=raw_data_2!L51,"","check")</f>
+        <f>IF(raw_data_1!K51=raw_data_2!L51,"","check")</f>
         <v/>
       </c>
       <c r="L51" t="str">
@@ -12727,7 +12730,7 @@
         <v/>
       </c>
       <c r="K52" t="str">
-        <f>IF(raw_data_1!L52=raw_data_2!L52,"","check")</f>
+        <f>IF(raw_data_1!K52=raw_data_2!L52,"","check")</f>
         <v/>
       </c>
       <c r="L52" t="str">
@@ -12781,7 +12784,7 @@
         <v/>
       </c>
       <c r="K53" t="str">
-        <f>IF(raw_data_1!L53=raw_data_2!L53,"","check")</f>
+        <f>IF(raw_data_1!K53=raw_data_2!L53,"","check")</f>
         <v/>
       </c>
       <c r="L53" t="str">
@@ -12835,7 +12838,7 @@
         <v/>
       </c>
       <c r="K54" t="str">
-        <f>IF(raw_data_1!L54=raw_data_2!L54,"","check")</f>
+        <f>IF(raw_data_1!K54=raw_data_2!L54,"","check")</f>
         <v/>
       </c>
       <c r="L54" t="str">
@@ -12889,7 +12892,7 @@
         <v/>
       </c>
       <c r="K55" t="str">
-        <f>IF(raw_data_1!L55=raw_data_2!L55,"","check")</f>
+        <f>IF(raw_data_1!K55=raw_data_2!L55,"","check")</f>
         <v/>
       </c>
       <c r="L55" t="str">
@@ -12943,7 +12946,7 @@
         <v/>
       </c>
       <c r="K56" t="str">
-        <f>IF(raw_data_1!L56=raw_data_2!L56,"","check")</f>
+        <f>IF(raw_data_1!K56=raw_data_2!L56,"","check")</f>
         <v/>
       </c>
       <c r="L56" t="str">
@@ -12997,7 +13000,7 @@
         <v/>
       </c>
       <c r="K57" t="str">
-        <f>IF(raw_data_1!L57=raw_data_2!L57,"","check")</f>
+        <f>IF(raw_data_1!K57=raw_data_2!L57,"","check")</f>
         <v/>
       </c>
       <c r="L57" t="str">
@@ -13051,7 +13054,7 @@
         <v/>
       </c>
       <c r="K58" t="str">
-        <f>IF(raw_data_1!L58=raw_data_2!L58,"","check")</f>
+        <f>IF(raw_data_1!K58=raw_data_2!L58,"","check")</f>
         <v/>
       </c>
       <c r="L58" t="str">
@@ -13105,7 +13108,7 @@
         <v/>
       </c>
       <c r="K59" t="str">
-        <f>IF(raw_data_1!L59=raw_data_2!L59,"","check")</f>
+        <f>IF(raw_data_1!K59=raw_data_2!L59,"","check")</f>
         <v/>
       </c>
       <c r="L59" t="str">
@@ -13159,7 +13162,7 @@
         <v/>
       </c>
       <c r="K60" t="str">
-        <f>IF(raw_data_1!L60=raw_data_2!L60,"","check")</f>
+        <f>IF(raw_data_1!K60=raw_data_2!L60,"","check")</f>
         <v/>
       </c>
       <c r="L60" t="str">
@@ -13213,7 +13216,7 @@
         <v/>
       </c>
       <c r="K61" t="str">
-        <f>IF(raw_data_1!L61=raw_data_2!L61,"","check")</f>
+        <f>IF(raw_data_1!K61=raw_data_2!L61,"","check")</f>
         <v/>
       </c>
       <c r="L61" t="str">
@@ -13267,7 +13270,7 @@
         <v/>
       </c>
       <c r="K62" t="str">
-        <f>IF(raw_data_1!L62=raw_data_2!L62,"","check")</f>
+        <f>IF(raw_data_1!K62=raw_data_2!L62,"","check")</f>
         <v/>
       </c>
       <c r="L62" t="str">
@@ -13321,7 +13324,7 @@
         <v/>
       </c>
       <c r="K63" t="str">
-        <f>IF(raw_data_1!L63=raw_data_2!L63,"","check")</f>
+        <f>IF(raw_data_1!K63=raw_data_2!L63,"","check")</f>
         <v/>
       </c>
       <c r="L63" t="str">
@@ -13375,7 +13378,7 @@
         <v/>
       </c>
       <c r="K64" t="str">
-        <f>IF(raw_data_1!L64=raw_data_2!L64,"","check")</f>
+        <f>IF(raw_data_1!K64=raw_data_2!L64,"","check")</f>
         <v/>
       </c>
       <c r="L64" t="str">
@@ -13429,7 +13432,7 @@
         <v/>
       </c>
       <c r="K65" t="str">
-        <f>IF(raw_data_1!L65=raw_data_2!L65,"","check")</f>
+        <f>IF(raw_data_1!K65=raw_data_2!L65,"","check")</f>
         <v/>
       </c>
       <c r="L65" t="str">
@@ -15862,10 +15865,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B13"/>
+  <dimension ref="A1:B14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J18" sqref="J18"/>
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -15955,7 +15958,7 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>34</v>
+        <v>82</v>
       </c>
       <c r="B11" t="s">
         <v>40</v>
@@ -15963,17 +15966,25 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>41</v>
+        <v>82</v>
       </c>
       <c r="B12" t="s">
-        <v>44</v>
+        <v>83</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
+        <v>41</v>
+      </c>
+      <c r="B13" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
         <v>42</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B14" t="s">
         <v>45</v>
       </c>
     </row>

</xml_diff>